<commit_message>
Water Heater Update 1
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/UEF Check Sheet.xlsx
+++ b/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/UEF Check Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FF7E6C-9BEC-46A6-A9E7-6DD35C459AB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE4F481-65A0-4140-87F7-5A6E54A0D78A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{4525C065-1982-4190-BA1C-76B51CDE7E26}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4525C065-1982-4190-BA1C-76B51CDE7E26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -367,8 +367,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -464,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -490,6 +491,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E368A452-0E99-44F6-9903-45AB1358FD53}">
   <dimension ref="A2:AI53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AJ12" sqref="AJ12"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AD60" sqref="AD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,13 +1069,13 @@
         <f>AD3-AE3</f>
         <v>0</v>
       </c>
-      <c r="AG3" s="1">
+      <c r="AG3" s="15">
         <v>0.63692918484900474</v>
       </c>
-      <c r="AH3" s="11">
+      <c r="AH3" s="16">
         <v>0.63882300000000003</v>
       </c>
-      <c r="AI3" s="14">
+      <c r="AI3" s="17">
         <f>AG3-AH3</f>
         <v>-1.8938151509952927E-3</v>
       </c>
@@ -1179,13 +1183,13 @@
         <f t="shared" ref="AF4:AF46" si="7">AD4-AE4</f>
         <v>0</v>
       </c>
-      <c r="AG4" s="1">
+      <c r="AG4" s="15">
         <v>0.64192391753402256</v>
       </c>
-      <c r="AH4" s="11">
+      <c r="AH4" s="16">
         <v>0.64266000000000001</v>
       </c>
-      <c r="AI4" s="14">
+      <c r="AI4" s="17">
         <f t="shared" ref="AI4:AI53" si="8">AG4-AH4</f>
         <v>-7.3608246597745008E-4</v>
       </c>
@@ -1289,13 +1293,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG5" s="1">
+      <c r="AG5" s="15">
         <v>0.91486436538534088</v>
       </c>
-      <c r="AH5" s="11">
+      <c r="AH5" s="16">
         <v>0.91491400000000001</v>
       </c>
-      <c r="AI5" s="14">
+      <c r="AI5" s="17">
         <f t="shared" si="8"/>
         <v>-4.9634614659122001E-5</v>
       </c>
@@ -1399,13 +1403,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG6" s="1">
+      <c r="AG6" s="15">
         <v>0.9167086694055423</v>
       </c>
-      <c r="AH6" s="11">
+      <c r="AH6" s="16">
         <v>0.91672200000000004</v>
       </c>
-      <c r="AI6" s="14">
+      <c r="AI6" s="17">
         <f t="shared" si="8"/>
         <v>-1.3330594457738876E-5</v>
       </c>
@@ -1509,13 +1513,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG7" s="1">
+      <c r="AG7" s="15">
         <v>0.92429892689988069</v>
       </c>
-      <c r="AH7" s="11">
+      <c r="AH7" s="16">
         <v>0.92431399999999997</v>
       </c>
-      <c r="AI7" s="14">
+      <c r="AI7" s="17">
         <f t="shared" si="8"/>
         <v>-1.5073100119278315E-5</v>
       </c>
@@ -1619,13 +1623,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG8" s="1">
+      <c r="AG8" s="15">
         <v>0.92263872730338636</v>
       </c>
-      <c r="AH8" s="11">
+      <c r="AH8" s="16">
         <v>0.92368099999999997</v>
       </c>
-      <c r="AI8" s="14">
+      <c r="AI8" s="17">
         <f t="shared" si="8"/>
         <v>-1.0422726966136109E-3</v>
       </c>
@@ -1729,13 +1733,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG9" s="1">
+      <c r="AG9" s="15">
         <v>0.91811639759826613</v>
       </c>
-      <c r="AH9" s="11">
+      <c r="AH9" s="16">
         <v>0.91810899999999995</v>
       </c>
-      <c r="AI9" s="14">
+      <c r="AI9" s="17">
         <f t="shared" si="8"/>
         <v>7.3975982661789175E-6</v>
       </c>
@@ -1839,13 +1843,13 @@
         <f t="shared" si="7"/>
         <v>-3</v>
       </c>
-      <c r="AG10" s="1">
+      <c r="AG10" s="15">
         <v>0.91780516938713574</v>
       </c>
-      <c r="AH10" s="11">
+      <c r="AH10" s="16">
         <v>0.91780499999999998</v>
       </c>
-      <c r="AI10" s="14">
+      <c r="AI10" s="17">
         <f t="shared" si="8"/>
         <v>1.693871357622001E-7</v>
       </c>
@@ -1949,13 +1953,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG11" s="1">
+      <c r="AG11" s="15">
         <v>0.91925132915549479</v>
       </c>
-      <c r="AH11" s="11">
+      <c r="AH11" s="16">
         <v>0.91928900000000002</v>
       </c>
-      <c r="AI11" s="14">
+      <c r="AI11" s="17">
         <f t="shared" si="8"/>
         <v>-3.767084450523317E-5</v>
       </c>
@@ -2059,13 +2063,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG12" s="1">
+      <c r="AG12" s="15">
         <v>0.88967514351634858</v>
       </c>
-      <c r="AH12" s="11">
+      <c r="AH12" s="16">
         <v>0.88994200000000001</v>
       </c>
-      <c r="AI12" s="14">
+      <c r="AI12" s="17">
         <f t="shared" si="8"/>
         <v>-2.6685648365143422E-4</v>
       </c>
@@ -2169,13 +2173,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG13" s="1">
+      <c r="AG13" s="15">
         <v>0.92035093322632699</v>
       </c>
-      <c r="AH13" s="11">
+      <c r="AH13" s="16">
         <v>0.92105099999999995</v>
       </c>
-      <c r="AI13" s="14">
+      <c r="AI13" s="17">
         <f t="shared" si="8"/>
         <v>-7.0006677367295822E-4</v>
       </c>
@@ -2279,13 +2283,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG14" s="1">
+      <c r="AG14" s="15">
         <v>0.92238581240683915</v>
       </c>
-      <c r="AH14" s="11">
+      <c r="AH14" s="16">
         <v>0.92272200000000004</v>
       </c>
-      <c r="AI14" s="14">
+      <c r="AI14" s="17">
         <f t="shared" si="8"/>
         <v>-3.3618759316089708E-4</v>
       </c>
@@ -2389,13 +2393,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG15" s="1">
+      <c r="AG15" s="15">
         <v>0.91517757628246044</v>
       </c>
-      <c r="AH15" s="11">
+      <c r="AH15" s="16">
         <v>0.91556099999999996</v>
       </c>
-      <c r="AI15" s="14">
+      <c r="AI15" s="17">
         <f t="shared" si="8"/>
         <v>-3.8342371753952165E-4</v>
       </c>
@@ -2499,13 +2503,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG16" s="1">
+      <c r="AG16" s="15">
         <v>0.91693398324447473</v>
       </c>
-      <c r="AH16" s="11">
+      <c r="AH16" s="16">
         <v>0.91695599999999999</v>
       </c>
-      <c r="AI16" s="14">
+      <c r="AI16" s="17">
         <f t="shared" si="8"/>
         <v>-2.2016755525267051E-5</v>
       </c>
@@ -2609,13 +2613,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG17" s="1">
+      <c r="AG17" s="15">
         <v>0.91499736714872371</v>
       </c>
-      <c r="AH17" s="11">
+      <c r="AH17" s="16">
         <v>0.91480700000000004</v>
       </c>
-      <c r="AI17" s="14">
+      <c r="AI17" s="17">
         <f t="shared" si="8"/>
         <v>1.9036714872366911E-4</v>
       </c>
@@ -2719,13 +2723,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG18" s="1">
+      <c r="AG18" s="15">
         <v>0.91584282945008366</v>
       </c>
-      <c r="AH18" s="11">
+      <c r="AH18" s="16">
         <v>0.91579900000000003</v>
       </c>
-      <c r="AI18" s="14">
+      <c r="AI18" s="17">
         <f t="shared" si="8"/>
         <v>4.382945008363226E-5</v>
       </c>
@@ -2829,13 +2833,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG19" s="1">
+      <c r="AG19" s="15">
         <v>0.90950537153338806</v>
       </c>
-      <c r="AH19" s="11">
+      <c r="AH19" s="16">
         <v>0.90962900000000002</v>
       </c>
-      <c r="AI19" s="14">
+      <c r="AI19" s="17">
         <f t="shared" si="8"/>
         <v>-1.2362846661195803E-4</v>
       </c>
@@ -2939,13 +2943,13 @@
         <f t="shared" si="7"/>
         <v>-2.9900000000052387</v>
       </c>
-      <c r="AG20" s="1">
+      <c r="AG20" s="15">
         <v>0.9181107354306689</v>
       </c>
-      <c r="AH20" s="11">
+      <c r="AH20" s="16">
         <v>0.918543</v>
       </c>
-      <c r="AI20" s="14">
+      <c r="AI20" s="17">
         <f t="shared" si="8"/>
         <v>-4.322645693310978E-4</v>
       </c>
@@ -3049,13 +3053,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG21" s="1">
+      <c r="AG21" s="15">
         <v>0.90923498497209809</v>
       </c>
-      <c r="AH21" s="11">
+      <c r="AH21" s="16">
         <v>0.90926899999999999</v>
       </c>
-      <c r="AI21" s="14">
+      <c r="AI21" s="17">
         <f t="shared" si="8"/>
         <v>-3.4015027901901362E-5</v>
       </c>
@@ -3159,13 +3163,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG22" s="1">
+      <c r="AG22" s="15">
         <v>0.91170649315209085</v>
       </c>
-      <c r="AH22" s="11">
+      <c r="AH22" s="16">
         <v>0.91155699999999995</v>
       </c>
-      <c r="AI22" s="14">
+      <c r="AI22" s="17">
         <f t="shared" si="8"/>
         <v>1.4949315209089598E-4</v>
       </c>
@@ -3269,13 +3273,13 @@
         <f t="shared" si="7"/>
         <v>-3</v>
       </c>
-      <c r="AG23" s="1">
+      <c r="AG23" s="15">
         <v>0.9235547669353702</v>
       </c>
-      <c r="AH23" s="11">
+      <c r="AH23" s="16">
         <v>0.923516</v>
       </c>
-      <c r="AI23" s="14">
+      <c r="AI23" s="17">
         <f t="shared" si="8"/>
         <v>3.87669353701936E-5</v>
       </c>
@@ -3379,13 +3383,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG24" s="1">
+      <c r="AG24" s="15">
         <v>0.92471339100958849</v>
       </c>
-      <c r="AH24" s="11">
+      <c r="AH24" s="16">
         <v>0.92467500000000002</v>
       </c>
-      <c r="AI24" s="14">
+      <c r="AI24" s="17">
         <f t="shared" si="8"/>
         <v>3.8391009588467639E-5</v>
       </c>
@@ -3489,13 +3493,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG25" s="1">
+      <c r="AG25" s="15">
         <v>0.91440189369811065</v>
       </c>
-      <c r="AH25" s="11">
+      <c r="AH25" s="16">
         <v>0.91542599999999996</v>
       </c>
-      <c r="AI25" s="14">
+      <c r="AI25" s="17">
         <f t="shared" si="8"/>
         <v>-1.024106301889316E-3</v>
       </c>
@@ -3599,13 +3603,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG26" s="1">
+      <c r="AG26" s="15">
         <v>0.91119750217455808</v>
       </c>
-      <c r="AH26" s="11">
+      <c r="AH26" s="16">
         <v>0.91116299999999995</v>
       </c>
-      <c r="AI26" s="14">
+      <c r="AI26" s="17">
         <f t="shared" si="8"/>
         <v>3.4502174558137533E-5</v>
       </c>
@@ -3709,13 +3713,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG27" s="1">
+      <c r="AG27" s="15">
         <v>0.91740136721349375</v>
       </c>
-      <c r="AH27" s="11">
+      <c r="AH27" s="16">
         <v>0.91737299999999999</v>
       </c>
-      <c r="AI27" s="14">
+      <c r="AI27" s="17">
         <f t="shared" si="8"/>
         <v>2.8367213493751819E-5</v>
       </c>
@@ -3819,13 +3823,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG28" s="1">
+      <c r="AG28" s="15">
         <v>0.90184813249726981</v>
       </c>
-      <c r="AH28" s="11">
+      <c r="AH28" s="16">
         <v>0.90227999999999997</v>
       </c>
-      <c r="AI28" s="14">
+      <c r="AI28" s="17">
         <f t="shared" si="8"/>
         <v>-4.318675027301655E-4</v>
       </c>
@@ -3929,13 +3933,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG29" s="1">
+      <c r="AG29" s="15">
         <v>0.91584433411827804</v>
       </c>
-      <c r="AH29" s="11">
+      <c r="AH29" s="16">
         <v>0.91574800000000001</v>
       </c>
-      <c r="AI29" s="14">
+      <c r="AI29" s="17">
         <f t="shared" si="8"/>
         <v>9.6334118278029734E-5</v>
       </c>
@@ -4039,13 +4043,13 @@
         <f t="shared" si="7"/>
         <v>-2.9899999999906868</v>
       </c>
-      <c r="AG30" s="1">
+      <c r="AG30" s="15">
         <v>0.91582419377934587</v>
       </c>
-      <c r="AH30" s="11">
+      <c r="AH30" s="16">
         <v>0.91591900000000004</v>
       </c>
-      <c r="AI30" s="14">
+      <c r="AI30" s="17">
         <f t="shared" si="8"/>
         <v>-9.4806220654164441E-5</v>
       </c>
@@ -4149,13 +4153,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG31" s="1">
+      <c r="AG31" s="15">
         <v>0.91000303824766082</v>
       </c>
-      <c r="AH31" s="11">
+      <c r="AH31" s="16">
         <v>0.91001900000000002</v>
       </c>
-      <c r="AI31" s="14">
+      <c r="AI31" s="17">
         <f t="shared" si="8"/>
         <v>-1.596175233919972E-5</v>
       </c>
@@ -4259,13 +4263,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG32" s="1">
+      <c r="AG32" s="15">
         <v>0.91609225355188495</v>
       </c>
-      <c r="AH32" s="11">
+      <c r="AH32" s="16">
         <v>0.91575799999999996</v>
       </c>
-      <c r="AI32" s="14">
+      <c r="AI32" s="17">
         <f t="shared" si="8"/>
         <v>3.3425355188498873E-4</v>
       </c>
@@ -4369,13 +4373,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG33" s="1">
+      <c r="AG33" s="15">
         <v>0.93137405678912</v>
       </c>
-      <c r="AH33" s="11">
+      <c r="AH33" s="16">
         <v>0.93142899999999995</v>
       </c>
-      <c r="AI33" s="14">
+      <c r="AI33" s="17">
         <f t="shared" si="8"/>
         <v>-5.494321087995413E-5</v>
       </c>
@@ -4479,13 +4483,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG34" s="1">
+      <c r="AG34" s="15">
         <v>0.93408475016627335</v>
       </c>
-      <c r="AH34" s="11">
+      <c r="AH34" s="16">
         <v>0.93481700000000001</v>
       </c>
-      <c r="AI34" s="14">
+      <c r="AI34" s="17">
         <f t="shared" si="8"/>
         <v>-7.3224983372666141E-4</v>
       </c>
@@ -4589,13 +4593,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG35" s="1">
+      <c r="AG35" s="15">
         <v>0.9313425672130492</v>
       </c>
-      <c r="AH35" s="11">
+      <c r="AH35" s="16">
         <v>0.93180399999999997</v>
       </c>
-      <c r="AI35" s="14">
+      <c r="AI35" s="17">
         <f t="shared" si="8"/>
         <v>-4.6143278695076617E-4</v>
       </c>
@@ -4699,18 +4703,18 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG36" s="1">
+      <c r="AG36" s="15">
         <v>0.92871686126712338</v>
       </c>
-      <c r="AH36" s="11">
+      <c r="AH36" s="16">
         <v>0.92897099999999999</v>
       </c>
-      <c r="AI36" s="14">
+      <c r="AI36" s="17">
         <f t="shared" si="8"/>
         <v>-2.541387328766076E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>53</v>
       </c>
@@ -4789,13 +4793,13 @@
         <f t="shared" si="7"/>
         <v>95043.94</v>
       </c>
-      <c r="AG37" s="1">
+      <c r="AG37" s="15">
         <v>0.92668440912607419</v>
       </c>
-      <c r="AH37" s="11">
+      <c r="AH37" s="16">
         <v>1.546189</v>
       </c>
-      <c r="AI37" s="14">
+      <c r="AI37" s="17">
         <f t="shared" si="8"/>
         <v>-0.61950459087392584</v>
       </c>
@@ -4899,13 +4903,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG38" s="1">
+      <c r="AG38" s="15">
         <v>0.93102933417843436</v>
       </c>
-      <c r="AH38" s="11">
+      <c r="AH38" s="16">
         <v>0.93119300000000005</v>
       </c>
-      <c r="AI38" s="14">
+      <c r="AI38" s="17">
         <f t="shared" si="8"/>
         <v>-1.6366582156568388E-4</v>
       </c>
@@ -5009,13 +5013,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG39" s="1">
+      <c r="AG39" s="15">
         <v>0.92971749366237477</v>
       </c>
-      <c r="AH39" s="11">
+      <c r="AH39" s="16">
         <v>0.93007600000000001</v>
       </c>
-      <c r="AI39" s="14">
+      <c r="AI39" s="17">
         <f t="shared" si="8"/>
         <v>-3.5850633762524176E-4</v>
       </c>
@@ -5119,13 +5123,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG40" s="1">
+      <c r="AG40" s="15">
         <v>0.88089077504082924</v>
       </c>
-      <c r="AH40" s="11">
+      <c r="AH40" s="16">
         <v>0.88096399999999997</v>
       </c>
-      <c r="AI40" s="14">
+      <c r="AI40" s="17">
         <f t="shared" si="8"/>
         <v>-7.322495917072569E-5</v>
       </c>
@@ -5229,13 +5233,13 @@
         <f t="shared" si="7"/>
         <v>-2.9899999999906868</v>
       </c>
-      <c r="AG41" s="1">
+      <c r="AG41" s="15">
         <v>0.9331024980123428</v>
       </c>
-      <c r="AH41" s="11">
+      <c r="AH41" s="16">
         <v>0.93317499999999998</v>
       </c>
-      <c r="AI41" s="14">
+      <c r="AI41" s="17">
         <f t="shared" si="8"/>
         <v>-7.2501987657180855E-5</v>
       </c>
@@ -5339,13 +5343,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG42" s="1">
+      <c r="AG42" s="15">
         <v>0.92968255944153733</v>
       </c>
-      <c r="AH42" s="11">
+      <c r="AH42" s="16">
         <v>0.92973899999999998</v>
       </c>
-      <c r="AI42" s="14">
+      <c r="AI42" s="17">
         <f t="shared" si="8"/>
         <v>-5.6440558462655943E-5</v>
       </c>
@@ -5449,13 +5453,13 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG43" s="1">
+      <c r="AG43" s="15">
         <v>0.92867786805463182</v>
       </c>
-      <c r="AH43" s="11">
+      <c r="AH43" s="16">
         <v>0.92833600000000005</v>
       </c>
-      <c r="AI43" s="14">
+      <c r="AI43" s="17">
         <f t="shared" si="8"/>
         <v>3.418680546317665E-4</v>
       </c>
@@ -5559,18 +5563,18 @@
         <f t="shared" si="7"/>
         <v>-3</v>
       </c>
-      <c r="AG44" s="1">
+      <c r="AG44" s="15">
         <v>0.92883400573334829</v>
       </c>
-      <c r="AH44" s="11">
+      <c r="AH44" s="16">
         <v>0.92969999999999997</v>
       </c>
-      <c r="AI44" s="14">
+      <c r="AI44" s="17">
         <f t="shared" si="8"/>
         <v>-8.6599426665168178E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>63</v>
       </c>
@@ -5640,7 +5644,7 @@
         <v>-0.63917199999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>64</v>
       </c>
@@ -5750,7 +5754,7 @@
         <v>0.2628809578956095</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="AH47">
         <v>0.63624999999999998</v>
       </c>
@@ -5759,7 +5763,7 @@
         <v>-0.63624999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="AH48">
         <v>0.631243</v>
       </c>
@@ -5768,7 +5772,7 @@
         <v>-0.631243</v>
       </c>
     </row>
-    <row r="49" spans="34:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="34:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="AH49">
         <v>0.63383199999999995</v>
       </c>
@@ -5777,7 +5781,7 @@
         <v>-0.63383199999999995</v>
       </c>
     </row>
-    <row r="50" spans="34:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="34:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="AH50">
         <v>0.65466800000000003</v>
       </c>
@@ -5786,7 +5790,7 @@
         <v>-0.65466800000000003</v>
       </c>
     </row>
-    <row r="51" spans="34:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="34:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="AH51">
         <v>0.63808200000000004</v>
       </c>
@@ -5795,7 +5799,7 @@
         <v>-0.63808200000000004</v>
       </c>
     </row>
-    <row r="52" spans="34:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="34:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="AH52">
         <v>3.1419169999999998</v>
       </c>
@@ -5804,7 +5808,7 @@
         <v>-3.1419169999999998</v>
       </c>
     </row>
-    <row r="53" spans="34:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="34:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="AH53">
         <v>0.81592699999999996</v>
       </c>

</xml_diff>

<commit_message>
Updated UEF calculation from 23 hours to 24 hours. updated gea3 to allow for inverter turning off. Updated ritter to have a reset
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/UEF Check Sheet.xlsx
+++ b/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/UEF Check Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5AB116-CAEF-4C1F-A5C1-54660E5298A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19D62BC-75B1-4E46-BDD4-6D1139C5294A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4525C065-1982-4190-BA1C-76B51CDE7E26}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4525C065-1982-4190-BA1C-76B51CDE7E26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -916,7 +916,7 @@
     <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -927,7 +927,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -943,17 +942,15 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1013,9 +1010,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1053,7 +1050,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1159,7 +1156,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1301,7 +1298,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1311,56 +1308,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E368A452-0E99-44F6-9903-45AB1358FD53}">
   <dimension ref="A2:AI54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" style="6" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="7.88671875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="14" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="9" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="9" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="26" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="22" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="29" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27.88671875" customWidth="1"/>
-    <col min="40" max="40" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="27.85546875" customWidth="1"/>
+    <col min="40" max="40" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1376,7 +1373,7 @@
       <c r="E2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>85</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1391,7 +1388,7 @@
       <c r="J2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>88</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1400,7 +1397,7 @@
       <c r="M2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>87</v>
       </c>
       <c r="O2" s="2" t="s">
@@ -1409,7 +1406,7 @@
       <c r="P2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="7" t="s">
         <v>84</v>
       </c>
       <c r="R2" s="2" t="s">
@@ -1418,7 +1415,7 @@
       <c r="S2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="7" t="s">
         <v>86</v>
       </c>
       <c r="U2" s="2" t="s">
@@ -1427,7 +1424,7 @@
       <c r="V2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="W2" s="7" t="s">
         <v>89</v>
       </c>
       <c r="X2" s="2" t="s">
@@ -1436,7 +1433,7 @@
       <c r="Y2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Z2" s="7" t="s">
         <v>82</v>
       </c>
       <c r="AA2" s="2" t="s">
@@ -1445,7 +1442,7 @@
       <c r="AB2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AC2" s="8" t="s">
+      <c r="AC2" s="7" t="s">
         <v>83</v>
       </c>
       <c r="AD2" s="2" t="s">
@@ -1454,97 +1451,97 @@
       <c r="AE2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AF2" s="7" t="s">
         <v>81</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AH2" s="11" t="s">
+      <c r="AH2" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="AI2" s="12" t="s">
+      <c r="AI2" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="15">
         <v>30</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="17">
+      <c r="D3" s="15"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="15">
         <v>4904.07</v>
       </c>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="9">
+      <c r="P3" s="15"/>
+      <c r="Q3" s="8">
         <f>O3-P3</f>
         <v>4904.07</v>
       </c>
-      <c r="R3" s="17">
+      <c r="R3" s="15">
         <v>4963.07</v>
       </c>
-      <c r="S3" s="17"/>
-      <c r="T3" s="9">
+      <c r="S3" s="15"/>
+      <c r="T3" s="8">
         <f>R3-S3</f>
         <v>4963.07</v>
       </c>
-      <c r="U3" s="17">
+      <c r="U3" s="15">
         <v>6744.1</v>
       </c>
-      <c r="V3" s="17"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="17">
+      <c r="V3" s="15"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="15">
         <v>13847.21</v>
       </c>
       <c r="Y3" s="5"/>
-      <c r="Z3" s="9">
+      <c r="Z3" s="8">
         <f>X3-Y3</f>
         <v>13847.21</v>
       </c>
-      <c r="AA3" s="17">
+      <c r="AA3" s="15">
         <v>42702.74</v>
       </c>
-      <c r="AB3" s="17"/>
-      <c r="AC3" s="9">
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="8">
         <f>AA3-AB3</f>
         <v>42702.74</v>
       </c>
-      <c r="AD3" s="17">
+      <c r="AD3" s="15">
         <v>91372.67</v>
       </c>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="9">
+      <c r="AE3" s="15"/>
+      <c r="AF3" s="8">
         <f>AD3-AE3</f>
         <v>91372.67</v>
       </c>
-      <c r="AG3" s="19">
+      <c r="AG3" s="17">
         <v>0.61577700000000002</v>
       </c>
-      <c r="AH3" s="20">
-        <v>0.60873100000000002</v>
-      </c>
-      <c r="AI3" s="15">
+      <c r="AH3">
+        <v>0.61577700000000002</v>
+      </c>
+      <c r="AI3" s="14">
         <f>AG3-AH3</f>
-        <v>7.0459999999999967E-3</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1560,7 +1557,7 @@
       <c r="E4" s="5">
         <v>121.15</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <f>D4-E4</f>
         <v>0</v>
       </c>
@@ -1576,7 +1573,7 @@
       <c r="J4" s="5">
         <v>130.25</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <f>I4-J4</f>
         <v>0</v>
       </c>
@@ -1586,7 +1583,7 @@
       <c r="M4" s="5">
         <v>127.983</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="6">
         <f>L4-M4</f>
         <v>0</v>
       </c>
@@ -1596,7 +1593,7 @@
       <c r="P4" s="5">
         <v>18787.61</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="8">
         <f>O4-P4</f>
         <v>0</v>
       </c>
@@ -1606,7 +1603,7 @@
       <c r="S4" s="5">
         <v>18847.27</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T4" s="8">
         <f>R4-S4</f>
         <v>0</v>
       </c>
@@ -1616,14 +1613,14 @@
       <c r="V4" s="5">
         <v>20599.63</v>
       </c>
-      <c r="W4" s="10"/>
+      <c r="W4" s="9"/>
       <c r="X4" s="1">
         <v>27206.45</v>
       </c>
       <c r="Y4" s="5">
         <v>27206.45</v>
       </c>
-      <c r="Z4" s="9">
+      <c r="Z4" s="8">
         <f>X4-Y4</f>
         <v>0</v>
       </c>
@@ -1633,7 +1630,7 @@
       <c r="AB4" s="5">
         <v>56586.12</v>
       </c>
-      <c r="AC4" s="9">
+      <c r="AC4" s="8">
         <f>AA4-AB4</f>
         <v>0</v>
       </c>
@@ -1643,22 +1640,22 @@
       <c r="AE4" s="5">
         <v>105247.53</v>
       </c>
-      <c r="AF4" s="9">
+      <c r="AF4" s="8">
         <f>AD4-AE4</f>
         <v>0</v>
       </c>
-      <c r="AG4" s="14">
+      <c r="AG4" s="13">
         <v>0.63692918484900474</v>
       </c>
-      <c r="AH4" s="20">
+      <c r="AH4">
         <v>0.63919899999999996</v>
       </c>
-      <c r="AI4" s="15">
+      <c r="AI4" s="14">
         <f>AG4-AH4</f>
         <v>-2.2698151509952247E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1674,7 +1671,7 @@
       <c r="E5" s="5">
         <v>119.833</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <f t="shared" ref="F5:F47" si="0">D5-E5</f>
         <v>0</v>
       </c>
@@ -1690,7 +1687,7 @@
       <c r="J5" s="5">
         <v>130</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <f t="shared" ref="K5:K47" si="1">I5-J5</f>
         <v>0</v>
       </c>
@@ -1700,7 +1697,7 @@
       <c r="M5" s="5">
         <v>128.30000000000001</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="6">
         <f t="shared" ref="N5:N47" si="2">L5-M5</f>
         <v>0</v>
       </c>
@@ -1710,7 +1707,7 @@
       <c r="P5" s="5">
         <v>5815.91</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="Q5" s="8">
         <f t="shared" ref="Q5:Q47" si="3">O5-P5</f>
         <v>-0.98999999999978172</v>
       </c>
@@ -1720,7 +1717,7 @@
       <c r="S5" s="5">
         <v>5875.22</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="8">
         <f t="shared" ref="T5:T47" si="4">R5-S5</f>
         <v>0</v>
       </c>
@@ -1730,14 +1727,14 @@
       <c r="V5" s="5">
         <v>7711.59</v>
       </c>
-      <c r="W5" s="10"/>
+      <c r="W5" s="9"/>
       <c r="X5" s="1">
         <v>14447.78</v>
       </c>
       <c r="Y5" s="5">
         <v>14447.78</v>
       </c>
-      <c r="Z5" s="9">
+      <c r="Z5" s="8">
         <f t="shared" ref="Z5:Z47" si="5">X5-Y5</f>
         <v>0</v>
       </c>
@@ -1747,7 +1744,7 @@
       <c r="AB5" s="5">
         <v>43614.46</v>
       </c>
-      <c r="AC5" s="9">
+      <c r="AC5" s="8">
         <f t="shared" ref="AC5:AC47" si="6">AA5-AB5</f>
         <v>0</v>
       </c>
@@ -1757,22 +1754,22 @@
       <c r="AE5" s="5">
         <v>92276.92</v>
       </c>
-      <c r="AF5" s="9">
+      <c r="AF5" s="8">
         <f t="shared" ref="AF5:AF47" si="7">AD5-AE5</f>
         <v>0</v>
       </c>
-      <c r="AG5" s="14">
+      <c r="AG5" s="13">
         <v>0.64192391753402256</v>
       </c>
-      <c r="AH5" s="20">
+      <c r="AH5">
         <v>0.64308200000000004</v>
       </c>
-      <c r="AI5" s="15">
+      <c r="AI5" s="14">
         <f t="shared" ref="AI5:AI54" si="8">AG5-AH5</f>
         <v>-1.1580824659774835E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -1788,7 +1785,7 @@
       <c r="E6" s="5">
         <v>121.717</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1802,7 +1799,7 @@
       <c r="J6" s="5">
         <v>122.883</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <f t="shared" si="1"/>
         <v>-4.9999999999997158E-2</v>
       </c>
@@ -1812,7 +1809,7 @@
       <c r="M6" s="5">
         <v>117.95</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="6">
         <f t="shared" si="2"/>
         <v>-1.6999999999995907E-2</v>
       </c>
@@ -1822,7 +1819,7 @@
       <c r="P6" s="5">
         <v>6503.73</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="Q6" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1832,7 +1829,7 @@
       <c r="S6" s="5">
         <v>6563.38</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1840,14 +1837,14 @@
       <c r="V6" s="5">
         <v>0</v>
       </c>
-      <c r="W6" s="10"/>
+      <c r="W6" s="9"/>
       <c r="X6" s="1">
         <v>14192.69</v>
       </c>
       <c r="Y6" s="5">
         <v>14198.58</v>
       </c>
-      <c r="Z6" s="9">
+      <c r="Z6" s="8">
         <f t="shared" si="5"/>
         <v>-5.8899999999994179</v>
       </c>
@@ -1857,7 +1854,7 @@
       <c r="AB6" s="5">
         <v>44303.17</v>
       </c>
-      <c r="AC6" s="9">
+      <c r="AC6" s="8">
         <f t="shared" si="6"/>
         <v>1.0200000000040745</v>
       </c>
@@ -1867,22 +1864,22 @@
       <c r="AE6" s="5">
         <v>92963.53</v>
       </c>
-      <c r="AF6" s="9">
+      <c r="AF6" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG6" s="14">
+      <c r="AG6" s="13">
         <v>0.91486436538534088</v>
       </c>
-      <c r="AH6" s="20">
+      <c r="AH6">
         <v>0.91566599999999998</v>
       </c>
-      <c r="AI6" s="15">
+      <c r="AI6" s="14">
         <f t="shared" si="8"/>
         <v>-8.0163461465909691E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1898,7 +1895,7 @@
       <c r="E7" s="5">
         <v>119.68300000000001</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1912,7 +1909,7 @@
       <c r="J7" s="5">
         <v>119.25</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1922,7 +1919,7 @@
       <c r="M7" s="5">
         <v>122.65</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1932,7 +1929,7 @@
       <c r="P7" s="5">
         <v>6629.48</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1942,7 +1939,7 @@
       <c r="S7" s="5">
         <v>6689.04</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1950,14 +1947,14 @@
       <c r="V7" s="5">
         <v>0</v>
       </c>
-      <c r="W7" s="10"/>
+      <c r="W7" s="9"/>
       <c r="X7" s="1">
         <v>17663.689999999999</v>
       </c>
       <c r="Y7" s="5">
         <v>17663.689999999999</v>
       </c>
-      <c r="Z7" s="9">
+      <c r="Z7" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1967,7 +1964,7 @@
       <c r="AB7" s="5">
         <v>44428.44</v>
       </c>
-      <c r="AC7" s="9">
+      <c r="AC7" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -1977,22 +1974,22 @@
       <c r="AE7" s="5">
         <v>93090.13</v>
       </c>
-      <c r="AF7" s="9">
+      <c r="AF7" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG7" s="14">
+      <c r="AG7" s="13">
         <v>0.9167086694055423</v>
       </c>
-      <c r="AH7" s="20">
+      <c r="AH7">
         <v>0.91733299999999995</v>
       </c>
-      <c r="AI7" s="15">
+      <c r="AI7" s="14">
         <f t="shared" si="8"/>
         <v>-6.2433059445765604E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -2008,7 +2005,7 @@
       <c r="E8" s="5">
         <v>120.167</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <f t="shared" si="0"/>
         <v>1.6000000000005343E-2</v>
       </c>
@@ -2022,7 +2019,7 @@
       <c r="J8" s="5">
         <v>119.55</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2032,7 +2029,7 @@
       <c r="M8" s="5">
         <v>122.717</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2042,7 +2039,7 @@
       <c r="P8" s="5">
         <v>6523.35</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="Q8" s="8">
         <f t="shared" si="3"/>
         <v>-2.75</v>
       </c>
@@ -2052,7 +2049,7 @@
       <c r="S8" s="5">
         <v>6582.77</v>
       </c>
-      <c r="T8" s="9">
+      <c r="T8" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2060,14 +2057,14 @@
       <c r="V8" s="5">
         <v>0</v>
       </c>
-      <c r="W8" s="10"/>
+      <c r="W8" s="9"/>
       <c r="X8" s="1">
         <v>17258.75</v>
       </c>
       <c r="Y8" s="5">
         <v>17258.75</v>
       </c>
-      <c r="Z8" s="9">
+      <c r="Z8" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2077,7 +2074,7 @@
       <c r="AB8" s="5">
         <v>44320.99</v>
       </c>
-      <c r="AC8" s="9">
+      <c r="AC8" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2087,22 +2084,22 @@
       <c r="AE8" s="5">
         <v>92983.6</v>
       </c>
-      <c r="AF8" s="9">
+      <c r="AF8" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG8" s="14">
+      <c r="AG8" s="13">
         <v>0.92429892689988069</v>
       </c>
-      <c r="AH8" s="20">
+      <c r="AH8">
         <v>0.92431399999999997</v>
       </c>
-      <c r="AI8" s="15">
+      <c r="AI8" s="14">
         <f t="shared" si="8"/>
         <v>-1.5073100119278315E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -2118,7 +2115,7 @@
       <c r="E9" s="5">
         <v>120.35</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2132,7 +2129,7 @@
       <c r="J9" s="5">
         <v>119.75</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2142,7 +2139,7 @@
       <c r="M9" s="5">
         <v>122.43300000000001</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2152,7 +2149,7 @@
       <c r="P9" s="5">
         <v>6650.74</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="Q9" s="8">
         <f t="shared" si="3"/>
         <v>-2.2100000000000364</v>
       </c>
@@ -2162,7 +2159,7 @@
       <c r="S9" s="5">
         <v>6709.62</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2170,14 +2167,14 @@
       <c r="V9" s="5">
         <v>0</v>
       </c>
-      <c r="W9" s="10"/>
+      <c r="W9" s="9"/>
       <c r="X9" s="1">
         <v>17467.46</v>
       </c>
       <c r="Y9" s="5">
         <v>17467.46</v>
       </c>
-      <c r="Z9" s="9">
+      <c r="Z9" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2187,7 +2184,7 @@
       <c r="AB9" s="5">
         <v>44448.15</v>
       </c>
-      <c r="AC9" s="9">
+      <c r="AC9" s="8">
         <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
@@ -2197,22 +2194,22 @@
       <c r="AE9" s="5">
         <v>93110.21</v>
       </c>
-      <c r="AF9" s="9">
+      <c r="AF9" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG9" s="14">
+      <c r="AG9" s="13">
         <v>0.92263872730338636</v>
       </c>
-      <c r="AH9" s="20">
+      <c r="AH9">
         <v>0.92395300000000002</v>
       </c>
-      <c r="AI9" s="15">
+      <c r="AI9" s="14">
         <f t="shared" si="8"/>
         <v>-1.3142726966136609E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -2228,7 +2225,7 @@
       <c r="E10" s="5">
         <v>120.917</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2242,7 +2239,7 @@
       <c r="J10" s="5">
         <v>120.167</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2252,7 +2249,7 @@
       <c r="M10" s="5">
         <v>122.75</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="6">
         <f t="shared" si="2"/>
         <v>6.6999999999993065E-2</v>
       </c>
@@ -2262,7 +2259,7 @@
       <c r="P10" s="5">
         <v>6638.47</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="Q10" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2272,7 +2269,7 @@
       <c r="S10" s="5">
         <v>6697.99</v>
       </c>
-      <c r="T10" s="9">
+      <c r="T10" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2280,14 +2277,14 @@
       <c r="V10" s="5">
         <v>0</v>
       </c>
-      <c r="W10" s="10"/>
+      <c r="W10" s="9"/>
       <c r="X10" s="1">
         <v>17973.599999999999</v>
       </c>
       <c r="Y10" s="5">
         <v>17973.599999999999</v>
       </c>
-      <c r="Z10" s="9">
+      <c r="Z10" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2297,7 +2294,7 @@
       <c r="AB10" s="5">
         <v>44436.56</v>
       </c>
-      <c r="AC10" s="9">
+      <c r="AC10" s="8">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -2307,22 +2304,22 @@
       <c r="AE10" s="5">
         <v>93098.3</v>
       </c>
-      <c r="AF10" s="9">
+      <c r="AF10" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG10" s="14">
+      <c r="AG10" s="13">
         <v>0.91811639759826613</v>
       </c>
-      <c r="AH10" s="20">
+      <c r="AH10">
         <v>0.91961700000000002</v>
       </c>
-      <c r="AI10" s="15">
+      <c r="AI10" s="14">
         <f t="shared" si="8"/>
         <v>-1.5006024017338859E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -2338,7 +2335,7 @@
       <c r="E11" s="5">
         <v>120.533</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <f t="shared" si="0"/>
         <v>-4.9999999999997158E-2</v>
       </c>
@@ -2352,7 +2349,7 @@
       <c r="J11" s="5">
         <v>120.283</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2362,7 +2359,7 @@
       <c r="M11" s="5">
         <v>123.18300000000001</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2372,7 +2369,7 @@
       <c r="P11" s="5">
         <v>6634.3</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="Q11" s="8">
         <f t="shared" si="3"/>
         <v>-1.0200000000004366</v>
       </c>
@@ -2382,7 +2379,7 @@
       <c r="S11" s="5">
         <v>6693.28</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2390,14 +2387,14 @@
       <c r="V11" s="5">
         <v>0</v>
       </c>
-      <c r="W11" s="10"/>
+      <c r="W11" s="9"/>
       <c r="X11" s="1">
         <v>17328.54</v>
       </c>
       <c r="Y11" s="5">
         <v>17328.54</v>
       </c>
-      <c r="Z11" s="9">
+      <c r="Z11" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2407,7 +2404,7 @@
       <c r="AB11" s="5">
         <v>44432.89</v>
       </c>
-      <c r="AC11" s="9">
+      <c r="AC11" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2417,22 +2414,22 @@
       <c r="AE11" s="5">
         <v>93096.16</v>
       </c>
-      <c r="AF11" s="9">
+      <c r="AF11" s="8">
         <f t="shared" si="7"/>
         <v>-3</v>
       </c>
-      <c r="AG11" s="14">
+      <c r="AG11" s="13">
         <v>0.91780516938713574</v>
       </c>
-      <c r="AH11" s="20">
+      <c r="AH11">
         <v>0.91934800000000005</v>
       </c>
-      <c r="AI11" s="15">
+      <c r="AI11" s="14">
         <f t="shared" si="8"/>
         <v>-1.5428306128643099E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -2448,7 +2445,7 @@
       <c r="E12" s="5">
         <v>121.617</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2462,7 +2459,7 @@
       <c r="J12" s="5">
         <v>121.15</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2472,7 +2469,7 @@
       <c r="M12" s="5">
         <v>117.767</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2482,7 +2479,7 @@
       <c r="P12" s="5">
         <v>6689.07</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q12" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2492,7 +2489,7 @@
       <c r="S12" s="5">
         <v>6748.59</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2500,14 +2497,14 @@
       <c r="V12" s="5">
         <v>0</v>
       </c>
-      <c r="W12" s="10"/>
+      <c r="W12" s="9"/>
       <c r="X12" s="1">
         <v>16288.1</v>
       </c>
       <c r="Y12" s="5">
         <v>16288.1</v>
       </c>
-      <c r="Z12" s="9">
+      <c r="Z12" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2517,7 +2514,7 @@
       <c r="AB12" s="5">
         <v>44487.17</v>
       </c>
-      <c r="AC12" s="9">
+      <c r="AC12" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2527,22 +2524,22 @@
       <c r="AE12" s="5">
         <v>93148.17</v>
       </c>
-      <c r="AF12" s="9">
+      <c r="AF12" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG12" s="14">
+      <c r="AG12" s="13">
         <v>0.91925132915549479</v>
       </c>
-      <c r="AH12" s="20">
+      <c r="AH12">
         <v>0.91936099999999998</v>
       </c>
-      <c r="AI12" s="15">
+      <c r="AI12" s="14">
         <f t="shared" si="8"/>
         <v>-1.0967084450519415E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -2558,7 +2555,7 @@
       <c r="E13" s="5">
         <v>152.75</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <f t="shared" si="0"/>
         <v>1.6999999999995907E-2</v>
       </c>
@@ -2572,7 +2569,7 @@
       <c r="J13" s="5">
         <v>151.583</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2582,7 +2579,7 @@
       <c r="M13" s="5">
         <v>156.18299999999999</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2592,7 +2589,7 @@
       <c r="P13" s="5">
         <v>14485.99</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="Q13" s="8">
         <f t="shared" si="3"/>
         <v>-1.0200000000004366</v>
       </c>
@@ -2602,7 +2599,7 @@
       <c r="S13" s="5">
         <v>14545.48</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2610,14 +2607,14 @@
       <c r="V13" s="5">
         <v>0</v>
       </c>
-      <c r="W13" s="10"/>
+      <c r="W13" s="9"/>
       <c r="X13" s="1">
         <v>26362.78</v>
       </c>
       <c r="Y13" s="5">
         <v>26362.78</v>
       </c>
-      <c r="Z13" s="9">
+      <c r="Z13" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2627,7 +2624,7 @@
       <c r="AB13" s="5">
         <v>52285.51</v>
       </c>
-      <c r="AC13" s="9">
+      <c r="AC13" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2637,22 +2634,22 @@
       <c r="AE13" s="5">
         <v>100946.82</v>
       </c>
-      <c r="AF13" s="9">
+      <c r="AF13" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG13" s="14">
+      <c r="AG13" s="13">
         <v>0.88967514351634858</v>
       </c>
-      <c r="AH13" s="20">
+      <c r="AH13">
         <v>0.89018200000000003</v>
       </c>
-      <c r="AI13" s="15">
+      <c r="AI13" s="14">
         <f t="shared" si="8"/>
         <v>-5.0685648365145219E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -2668,7 +2665,7 @@
       <c r="E14" s="5">
         <v>120.35</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2682,7 +2679,7 @@
       <c r="J14" s="5">
         <v>119.717</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2692,7 +2689,7 @@
       <c r="M14" s="5">
         <v>121.917</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2702,7 +2699,7 @@
       <c r="P14" s="5">
         <v>6449.32</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="Q14" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2712,7 +2709,7 @@
       <c r="S14" s="5">
         <v>6508.89</v>
       </c>
-      <c r="T14" s="9">
+      <c r="T14" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2720,14 +2717,14 @@
       <c r="V14" s="5">
         <v>0</v>
       </c>
-      <c r="W14" s="10"/>
+      <c r="W14" s="9"/>
       <c r="X14" s="1">
         <v>18236.78</v>
       </c>
       <c r="Y14" s="5">
         <v>18236.78</v>
       </c>
-      <c r="Z14" s="9">
+      <c r="Z14" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2737,7 +2734,7 @@
       <c r="AB14" s="5">
         <v>44247.6</v>
       </c>
-      <c r="AC14" s="9">
+      <c r="AC14" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2747,22 +2744,22 @@
       <c r="AE14" s="5">
         <v>92908.88</v>
       </c>
-      <c r="AF14" s="9">
+      <c r="AF14" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG14" s="14">
+      <c r="AG14" s="13">
         <v>0.92035093322632699</v>
       </c>
-      <c r="AH14" s="20">
+      <c r="AH14">
         <v>0.92149899999999996</v>
       </c>
-      <c r="AI14" s="15">
+      <c r="AI14" s="14">
         <f t="shared" si="8"/>
         <v>-1.1480667736729622E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -2778,7 +2775,7 @@
       <c r="E15" s="5">
         <v>121.1</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2792,7 +2789,7 @@
       <c r="J15" s="5">
         <v>120.06699999999999</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <f t="shared" si="1"/>
         <v>-0.76699999999999591</v>
       </c>
@@ -2802,7 +2799,7 @@
       <c r="M15" s="5">
         <v>122.083</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2812,7 +2809,7 @@
       <c r="P15" s="5">
         <v>6549.46</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="Q15" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2822,7 +2819,7 @@
       <c r="S15" s="5">
         <v>6608.97</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2830,14 +2827,14 @@
       <c r="V15" s="5">
         <v>0</v>
       </c>
-      <c r="W15" s="10"/>
+      <c r="W15" s="9"/>
       <c r="X15" s="1">
         <v>14773.59</v>
       </c>
       <c r="Y15" s="5">
         <v>17986.59</v>
       </c>
-      <c r="Z15" s="9">
+      <c r="Z15" s="8">
         <f t="shared" si="5"/>
         <v>-3213</v>
       </c>
@@ -2847,7 +2844,7 @@
       <c r="AB15" s="5">
         <v>44347.59</v>
       </c>
-      <c r="AC15" s="9">
+      <c r="AC15" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2857,22 +2854,22 @@
       <c r="AE15" s="5">
         <v>93009.26</v>
       </c>
-      <c r="AF15" s="9">
+      <c r="AF15" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG15" s="14">
+      <c r="AG15" s="13">
         <v>0.92238581240683915</v>
       </c>
-      <c r="AH15" s="20">
+      <c r="AH15">
         <v>0.92390399999999995</v>
       </c>
-      <c r="AI15" s="15">
+      <c r="AI15" s="14">
         <f t="shared" si="8"/>
         <v>-1.5181875931608024E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -2888,7 +2885,7 @@
       <c r="E16" s="5">
         <v>120.55</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <f t="shared" si="0"/>
         <v>3.3000000000001251E-2</v>
       </c>
@@ -2902,7 +2899,7 @@
       <c r="J16" s="5">
         <v>119.68300000000001</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2912,7 +2909,7 @@
       <c r="M16" s="5">
         <v>121.31699999999999</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2922,7 +2919,7 @@
       <c r="P16" s="5">
         <v>6654.01</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="Q16" s="8">
         <f t="shared" si="3"/>
         <v>-1.0300000000006548</v>
       </c>
@@ -2932,7 +2929,7 @@
       <c r="S16" s="5">
         <v>6713.22</v>
       </c>
-      <c r="T16" s="9">
+      <c r="T16" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2940,14 +2937,14 @@
       <c r="V16" s="5">
         <v>0</v>
       </c>
-      <c r="W16" s="10"/>
+      <c r="W16" s="9"/>
       <c r="X16" s="1">
         <v>18650.75</v>
       </c>
       <c r="Y16" s="5">
         <v>18650.75</v>
       </c>
-      <c r="Z16" s="9">
+      <c r="Z16" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2957,7 +2954,7 @@
       <c r="AB16" s="5">
         <v>44452.85</v>
       </c>
-      <c r="AC16" s="9">
+      <c r="AC16" s="8">
         <f t="shared" si="6"/>
         <v>0.98999999999796273</v>
       </c>
@@ -2967,22 +2964,22 @@
       <c r="AE16" s="5">
         <v>93113.279999999999</v>
       </c>
-      <c r="AF16" s="9">
+      <c r="AF16" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG16" s="14">
+      <c r="AG16" s="13">
         <v>0.91517757628246044</v>
       </c>
-      <c r="AH16" s="20">
+      <c r="AH16">
         <v>0.91652</v>
       </c>
-      <c r="AI16" s="15">
+      <c r="AI16" s="14">
         <f t="shared" si="8"/>
         <v>-1.3424237175395648E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -2998,7 +2995,7 @@
       <c r="E17" s="5">
         <v>121.883</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3012,7 +3009,7 @@
       <c r="J17" s="5">
         <v>121.2</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3022,7 +3019,7 @@
       <c r="M17" s="5">
         <v>117.833</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N17" s="6">
         <f t="shared" si="2"/>
         <v>3.4000000000006025E-2</v>
       </c>
@@ -3032,7 +3029,7 @@
       <c r="P17" s="5">
         <v>6295.09</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="Q17" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3042,7 +3039,7 @@
       <c r="S17" s="5">
         <v>6354.77</v>
       </c>
-      <c r="T17" s="9">
+      <c r="T17" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3050,14 +3047,14 @@
       <c r="V17" s="5">
         <v>0</v>
       </c>
-      <c r="W17" s="10"/>
+      <c r="W17" s="9"/>
       <c r="X17" s="1">
         <v>16570.43</v>
       </c>
       <c r="Y17" s="5">
         <v>16570.43</v>
       </c>
-      <c r="Z17" s="9">
+      <c r="Z17" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3067,7 +3064,7 @@
       <c r="AB17" s="5">
         <v>44093.89</v>
       </c>
-      <c r="AC17" s="9">
+      <c r="AC17" s="8">
         <f t="shared" si="6"/>
         <v>0.98999999999796273</v>
       </c>
@@ -3077,22 +3074,22 @@
       <c r="AE17" s="5">
         <v>92754.94</v>
       </c>
-      <c r="AF17" s="9">
+      <c r="AF17" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG17" s="14">
+      <c r="AG17" s="13">
         <v>0.91693398324447473</v>
       </c>
-      <c r="AH17" s="20">
+      <c r="AH17">
         <v>0.918161</v>
       </c>
-      <c r="AI17" s="15">
+      <c r="AI17" s="14">
         <f t="shared" si="8"/>
         <v>-1.2270167555252787E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
@@ -3108,7 +3105,7 @@
       <c r="E18" s="5">
         <v>123.7</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <f t="shared" si="0"/>
         <v>-1.6999999999995907E-2</v>
       </c>
@@ -3122,7 +3119,7 @@
       <c r="J18" s="5">
         <v>106.633</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="6">
         <f t="shared" si="1"/>
         <v>-0.8160000000000025</v>
       </c>
@@ -3132,7 +3129,7 @@
       <c r="M18" s="5">
         <v>104.93300000000001</v>
       </c>
-      <c r="N18" s="7">
+      <c r="N18" s="6">
         <f t="shared" si="2"/>
         <v>-5.0000000000011369E-2</v>
       </c>
@@ -3142,7 +3139,7 @@
       <c r="P18" s="5">
         <v>7248.99</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="Q18" s="8">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
@@ -3152,7 +3149,7 @@
       <c r="S18" s="5">
         <v>7308.18</v>
       </c>
-      <c r="T18" s="9">
+      <c r="T18" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3160,14 +3157,14 @@
       <c r="V18" s="5">
         <v>0</v>
       </c>
-      <c r="W18" s="10"/>
+      <c r="W18" s="9"/>
       <c r="X18" s="1">
         <v>13935.88</v>
       </c>
       <c r="Y18" s="5">
         <v>19554.939999999999</v>
       </c>
-      <c r="Z18" s="9">
+      <c r="Z18" s="8">
         <f t="shared" si="5"/>
         <v>-5619.0599999999995</v>
       </c>
@@ -3177,7 +3174,7 @@
       <c r="AB18" s="5">
         <v>45047.199999999997</v>
       </c>
-      <c r="AC18" s="9">
+      <c r="AC18" s="8">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -3187,22 +3184,22 @@
       <c r="AE18" s="5">
         <v>93708.5</v>
       </c>
-      <c r="AF18" s="9">
+      <c r="AF18" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG18" s="14">
+      <c r="AG18" s="13">
         <v>0.91499736714872371</v>
       </c>
-      <c r="AH18" s="20">
+      <c r="AH18">
         <v>0.91571599999999997</v>
       </c>
-      <c r="AI18" s="15">
+      <c r="AI18" s="14">
         <f t="shared" si="8"/>
         <v>-7.1863285127626852E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
@@ -3218,7 +3215,7 @@
       <c r="E19" s="5">
         <v>122.633</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3232,7 +3229,7 @@
       <c r="J19" s="5">
         <v>105.783</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="6">
         <f t="shared" si="1"/>
         <v>-0.63299999999999557</v>
       </c>
@@ -3242,7 +3239,7 @@
       <c r="M19" s="5">
         <v>104.083</v>
       </c>
-      <c r="N19" s="7">
+      <c r="N19" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3252,7 +3249,7 @@
       <c r="P19" s="5">
         <v>7661.06</v>
       </c>
-      <c r="Q19" s="9">
+      <c r="Q19" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3262,7 +3259,7 @@
       <c r="S19" s="5">
         <v>7720.7</v>
       </c>
-      <c r="T19" s="9">
+      <c r="T19" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3270,14 +3267,14 @@
       <c r="V19" s="5">
         <v>0</v>
       </c>
-      <c r="W19" s="10"/>
+      <c r="W19" s="9"/>
       <c r="X19" s="1">
         <v>14345.82</v>
       </c>
       <c r="Y19" s="5">
         <v>17699.810000000001</v>
       </c>
-      <c r="Z19" s="9">
+      <c r="Z19" s="8">
         <f t="shared" si="5"/>
         <v>-3353.9900000000016</v>
       </c>
@@ -3287,7 +3284,7 @@
       <c r="AB19" s="5">
         <v>45460.160000000003</v>
       </c>
-      <c r="AC19" s="9">
+      <c r="AC19" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3297,22 +3294,22 @@
       <c r="AE19" s="5">
         <v>94120.46</v>
       </c>
-      <c r="AF19" s="9">
+      <c r="AF19" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG19" s="14">
+      <c r="AG19" s="13">
         <v>0.91584282945008366</v>
       </c>
-      <c r="AH19" s="20">
+      <c r="AH19">
         <v>0.91695899999999997</v>
       </c>
-      <c r="AI19" s="15">
+      <c r="AI19" s="14">
         <f t="shared" si="8"/>
         <v>-1.1161705499163066E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
@@ -3328,7 +3325,7 @@
       <c r="E20" s="5">
         <v>123.45</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3342,7 +3339,7 @@
       <c r="J20" s="5">
         <v>106.267</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="6">
         <f t="shared" si="1"/>
         <v>-0.84999999999999432</v>
       </c>
@@ -3352,7 +3349,7 @@
       <c r="M20" s="5">
         <v>104.46705</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="6">
         <f t="shared" si="2"/>
         <v>-5.0000000001659828E-5</v>
       </c>
@@ -3362,7 +3359,7 @@
       <c r="P20" s="5">
         <v>7395.48</v>
       </c>
-      <c r="Q20" s="9">
+      <c r="Q20" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3372,7 +3369,7 @@
       <c r="S20" s="5">
         <v>7455.15</v>
       </c>
-      <c r="T20" s="9">
+      <c r="T20" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3380,14 +3377,14 @@
       <c r="V20" s="5">
         <v>0</v>
       </c>
-      <c r="W20" s="10"/>
+      <c r="W20" s="9"/>
       <c r="X20" s="1">
         <v>14082.26</v>
       </c>
       <c r="Y20" s="5">
         <v>19035.259999999998</v>
       </c>
-      <c r="Z20" s="9">
+      <c r="Z20" s="8">
         <f t="shared" si="5"/>
         <v>-4952.9999999999982</v>
       </c>
@@ -3397,7 +3394,7 @@
       <c r="AB20" s="5">
         <v>45194.239999999998</v>
       </c>
-      <c r="AC20" s="9">
+      <c r="AC20" s="8">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -3407,22 +3404,22 @@
       <c r="AE20" s="5">
         <v>93854.95</v>
       </c>
-      <c r="AF20" s="9">
+      <c r="AF20" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG20" s="14">
+      <c r="AG20" s="13">
         <v>0.90950537153338806</v>
       </c>
-      <c r="AH20" s="20">
+      <c r="AH20">
         <v>0.91079399999999999</v>
       </c>
-      <c r="AI20" s="15">
+      <c r="AI20" s="14">
         <f t="shared" si="8"/>
         <v>-1.2886284666119296E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
@@ -3438,7 +3435,7 @@
       <c r="E21" s="5">
         <v>122.583</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <f t="shared" si="0"/>
         <v>4.9999999999997158E-2</v>
       </c>
@@ -3452,7 +3449,7 @@
       <c r="J21" s="5">
         <v>105.733</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <f t="shared" si="1"/>
         <v>-0.71600000000000819</v>
       </c>
@@ -3462,7 +3459,7 @@
       <c r="M21" s="5">
         <v>104.133</v>
       </c>
-      <c r="N21" s="7">
+      <c r="N21" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3472,7 +3469,7 @@
       <c r="P21" s="5">
         <v>7369.86</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="Q21" s="8">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
@@ -3482,7 +3479,7 @@
       <c r="S21" s="5">
         <v>7429.02</v>
       </c>
-      <c r="T21" s="9">
+      <c r="T21" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3490,14 +3487,14 @@
       <c r="V21" s="5">
         <v>0</v>
       </c>
-      <c r="W21" s="10"/>
+      <c r="W21" s="9"/>
       <c r="X21" s="1">
         <v>14054.07</v>
       </c>
       <c r="Y21" s="5">
         <v>17894.150000000001</v>
       </c>
-      <c r="Z21" s="9">
+      <c r="Z21" s="8">
         <f t="shared" si="5"/>
         <v>-3840.0800000000017</v>
       </c>
@@ -3507,7 +3504,7 @@
       <c r="AB21" s="5">
         <v>45167.76</v>
       </c>
-      <c r="AC21" s="9">
+      <c r="AC21" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3517,22 +3514,22 @@
       <c r="AE21" s="5">
         <v>93830.720000000001</v>
       </c>
-      <c r="AF21" s="9">
+      <c r="AF21" s="8">
         <f t="shared" si="7"/>
         <v>-2.9900000000052387</v>
       </c>
-      <c r="AG21" s="14">
+      <c r="AG21" s="13">
         <v>0.9181107354306689</v>
       </c>
-      <c r="AH21" s="20">
+      <c r="AH21">
         <v>0.91930999999999996</v>
       </c>
-      <c r="AI21" s="15">
+      <c r="AI21" s="14">
         <f t="shared" si="8"/>
         <v>-1.19926456933106E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
@@ -3548,7 +3545,7 @@
       <c r="E22" s="5">
         <v>122.85</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3562,7 +3559,7 @@
       <c r="J22" s="5">
         <v>108.217</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="6">
         <f t="shared" si="1"/>
         <v>-0.59999999999999432</v>
       </c>
@@ -3572,7 +3569,7 @@
       <c r="M22" s="5">
         <v>106.483</v>
       </c>
-      <c r="N22" s="7">
+      <c r="N22" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3582,7 +3579,7 @@
       <c r="P22" s="5">
         <v>6123.84</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="Q22" s="8">
         <f t="shared" si="3"/>
         <v>-1.7300000000004729</v>
       </c>
@@ -3592,7 +3589,7 @@
       <c r="S22" s="5">
         <v>6182.47</v>
       </c>
-      <c r="T22" s="9">
+      <c r="T22" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3600,14 +3597,14 @@
       <c r="V22" s="5">
         <v>0</v>
       </c>
-      <c r="W22" s="10"/>
+      <c r="W22" s="9"/>
       <c r="X22" s="1">
         <v>12806.1</v>
       </c>
       <c r="Y22" s="5">
         <v>16693.419999999998</v>
       </c>
-      <c r="Z22" s="9">
+      <c r="Z22" s="8">
         <f t="shared" si="5"/>
         <v>-3887.3199999999979</v>
       </c>
@@ -3617,7 +3614,7 @@
       <c r="AB22" s="5">
         <v>43921.919999999998</v>
       </c>
-      <c r="AC22" s="9">
+      <c r="AC22" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3627,22 +3624,22 @@
       <c r="AE22" s="5">
         <v>92582.88</v>
       </c>
-      <c r="AF22" s="9">
+      <c r="AF22" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG22" s="14">
+      <c r="AG22" s="13">
         <v>0.90923498497209809</v>
       </c>
-      <c r="AH22" s="20">
+      <c r="AH22">
         <v>0.91016799999999998</v>
       </c>
-      <c r="AI22" s="15">
+      <c r="AI22" s="14">
         <f t="shared" si="8"/>
         <v>-9.3301502790188451E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -3658,7 +3655,7 @@
       <c r="E23" s="5">
         <v>123</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <f t="shared" si="0"/>
         <v>-3.3000000000001251E-2</v>
       </c>
@@ -3672,7 +3669,7 @@
       <c r="J23" s="5">
         <v>108.55</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K23" s="6">
         <f t="shared" si="1"/>
         <v>-6.6999999999993065E-2</v>
       </c>
@@ -3682,7 +3679,7 @@
       <c r="M23" s="5">
         <v>106.583</v>
       </c>
-      <c r="N23" s="7">
+      <c r="N23" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3692,7 +3689,7 @@
       <c r="P23" s="5">
         <v>7335.16</v>
       </c>
-      <c r="Q23" s="9">
+      <c r="Q23" s="8">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
@@ -3702,7 +3699,7 @@
       <c r="S23" s="5">
         <v>7394.28</v>
       </c>
-      <c r="T23" s="9">
+      <c r="T23" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3710,14 +3707,14 @@
       <c r="V23" s="5">
         <v>0</v>
       </c>
-      <c r="W23" s="10"/>
+      <c r="W23" s="9"/>
       <c r="X23" s="1">
         <v>14023.95</v>
       </c>
       <c r="Y23" s="5">
         <v>15875</v>
       </c>
-      <c r="Z23" s="9">
+      <c r="Z23" s="8">
         <f t="shared" si="5"/>
         <v>-1851.0499999999993</v>
       </c>
@@ -3727,7 +3724,7 @@
       <c r="AB23" s="5">
         <v>45133.98</v>
       </c>
-      <c r="AC23" s="9">
+      <c r="AC23" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3737,22 +3734,22 @@
       <c r="AE23" s="5">
         <v>93794.47</v>
       </c>
-      <c r="AF23" s="9">
+      <c r="AF23" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG23" s="14">
+      <c r="AG23" s="13">
         <v>0.91170649315209085</v>
       </c>
-      <c r="AH23" s="20">
+      <c r="AH23">
         <v>0.91240900000000003</v>
       </c>
-      <c r="AI23" s="15">
+      <c r="AI23" s="14">
         <f t="shared" si="8"/>
         <v>-7.0250684790917894E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>37</v>
       </c>
@@ -3768,7 +3765,7 @@
       <c r="E24" s="5">
         <v>119.917</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <f t="shared" si="0"/>
         <v>1.6000000000005343E-2</v>
       </c>
@@ -3782,7 +3779,7 @@
       <c r="J24" s="5">
         <v>103.8</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="6">
         <f t="shared" si="1"/>
         <v>-0.61699999999999022</v>
       </c>
@@ -3792,7 +3789,7 @@
       <c r="M24" s="5">
         <v>102.283</v>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3802,7 +3799,7 @@
       <c r="P24" s="5">
         <v>6044.37</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="Q24" s="8">
         <f t="shared" si="3"/>
         <v>-1.0199999999995271</v>
       </c>
@@ -3812,7 +3809,7 @@
       <c r="S24" s="5">
         <v>6103.86</v>
       </c>
-      <c r="T24" s="9">
+      <c r="T24" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3820,14 +3817,14 @@
       <c r="V24" s="5">
         <v>0</v>
       </c>
-      <c r="W24" s="10"/>
+      <c r="W24" s="9"/>
       <c r="X24" s="1">
         <v>12729.55</v>
       </c>
       <c r="Y24" s="5">
         <v>16893.62</v>
       </c>
-      <c r="Z24" s="9">
+      <c r="Z24" s="8">
         <f t="shared" si="5"/>
         <v>-4164.07</v>
       </c>
@@ -3837,7 +3834,7 @@
       <c r="AB24" s="5">
         <v>43842.91</v>
       </c>
-      <c r="AC24" s="9">
+      <c r="AC24" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3847,22 +3844,22 @@
       <c r="AE24" s="5">
         <v>92505.66</v>
       </c>
-      <c r="AF24" s="9">
+      <c r="AF24" s="8">
         <f t="shared" si="7"/>
         <v>-3</v>
       </c>
-      <c r="AG24" s="14">
+      <c r="AG24" s="13">
         <v>0.9235547669353702</v>
       </c>
-      <c r="AH24" s="20">
+      <c r="AH24">
         <v>0.92468399999999995</v>
       </c>
-      <c r="AI24" s="15">
+      <c r="AI24" s="14">
         <f t="shared" si="8"/>
         <v>-1.1292330646297533E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>38</v>
       </c>
@@ -3878,7 +3875,7 @@
       <c r="E25" s="5">
         <v>121.133</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3892,7 +3889,7 @@
       <c r="J25" s="5">
         <v>103.8</v>
       </c>
-      <c r="K25" s="7">
+      <c r="K25" s="6">
         <f t="shared" si="1"/>
         <v>-0.70000000000000284</v>
       </c>
@@ -3902,7 +3899,7 @@
       <c r="M25" s="5">
         <v>102.367</v>
       </c>
-      <c r="N25" s="7">
+      <c r="N25" s="6">
         <f t="shared" si="2"/>
         <v>3.3000000000001251E-2</v>
       </c>
@@ -3912,7 +3909,7 @@
       <c r="P25" s="5">
         <v>6475.78</v>
       </c>
-      <c r="Q25" s="9">
+      <c r="Q25" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3922,7 +3919,7 @@
       <c r="S25" s="5">
         <v>6535.76</v>
       </c>
-      <c r="T25" s="9">
+      <c r="T25" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3930,14 +3927,14 @@
       <c r="V25" s="5">
         <v>0</v>
       </c>
-      <c r="W25" s="10"/>
+      <c r="W25" s="9"/>
       <c r="X25" s="1">
         <v>13162.47</v>
       </c>
       <c r="Y25" s="5">
         <v>17785.52</v>
       </c>
-      <c r="Z25" s="9">
+      <c r="Z25" s="8">
         <f t="shared" si="5"/>
         <v>-4623.0500000000011</v>
       </c>
@@ -3947,7 +3944,7 @@
       <c r="AB25" s="5">
         <v>44274.36</v>
       </c>
-      <c r="AC25" s="9">
+      <c r="AC25" s="8">
         <f t="shared" si="6"/>
         <v>1.5299999999988358</v>
       </c>
@@ -3957,22 +3954,22 @@
       <c r="AE25" s="5">
         <v>92936.66</v>
       </c>
-      <c r="AF25" s="9">
+      <c r="AF25" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG25" s="14">
+      <c r="AG25" s="13">
         <v>0.92471339100958849</v>
       </c>
-      <c r="AH25" s="20">
+      <c r="AH25">
         <v>0.92580200000000001</v>
       </c>
-      <c r="AI25" s="15">
+      <c r="AI25" s="14">
         <f t="shared" si="8"/>
         <v>-1.0886089904115215E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
@@ -3988,7 +3985,7 @@
       <c r="E26" s="5">
         <v>120.967</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <f t="shared" si="0"/>
         <v>3.3000000000001251E-2</v>
       </c>
@@ -4002,7 +3999,7 @@
       <c r="J26" s="5">
         <v>104.18300000000001</v>
       </c>
-      <c r="K26" s="7">
+      <c r="K26" s="6">
         <f t="shared" si="1"/>
         <v>-1.1330000000000098</v>
       </c>
@@ -4012,7 +4009,7 @@
       <c r="M26" s="5">
         <v>102.717</v>
       </c>
-      <c r="N26" s="7">
+      <c r="N26" s="6">
         <f t="shared" si="2"/>
         <v>-1.6999999999995907E-2</v>
       </c>
@@ -4022,7 +4019,7 @@
       <c r="P26" s="5">
         <v>7134.8</v>
       </c>
-      <c r="Q26" s="9">
+      <c r="Q26" s="8">
         <f t="shared" si="3"/>
         <v>-1.4899999999997817</v>
       </c>
@@ -4032,7 +4029,7 @@
       <c r="S26" s="5">
         <v>7193.4</v>
       </c>
-      <c r="T26" s="9">
+      <c r="T26" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4040,14 +4037,14 @@
       <c r="V26" s="5">
         <v>0</v>
       </c>
-      <c r="W26" s="10"/>
+      <c r="W26" s="9"/>
       <c r="X26" s="1">
         <v>13821.33</v>
       </c>
       <c r="Y26" s="5">
         <v>21813</v>
       </c>
-      <c r="Z26" s="9">
+      <c r="Z26" s="8">
         <f t="shared" si="5"/>
         <v>-7991.67</v>
       </c>
@@ -4057,7 +4054,7 @@
       <c r="AB26" s="5">
         <v>44932.38</v>
       </c>
-      <c r="AC26" s="9">
+      <c r="AC26" s="8">
         <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
@@ -4067,22 +4064,22 @@
       <c r="AE26" s="5">
         <v>93593.5</v>
       </c>
-      <c r="AF26" s="9">
+      <c r="AF26" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG26" s="14">
+      <c r="AG26" s="13">
         <v>0.91440189369811065</v>
       </c>
-      <c r="AH26" s="20">
+      <c r="AH26">
         <v>0.91599799999999998</v>
       </c>
-      <c r="AI26" s="15">
+      <c r="AI26" s="14">
         <f t="shared" si="8"/>
         <v>-1.5961063018893329E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>41</v>
       </c>
@@ -4098,7 +4095,7 @@
       <c r="E27" s="5">
         <v>121.55</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4112,7 +4109,7 @@
       <c r="J27" s="5">
         <v>104.517</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="6">
         <f t="shared" si="1"/>
         <v>-1.1499999999999915</v>
       </c>
@@ -4122,7 +4119,7 @@
       <c r="M27" s="5">
         <v>103.1</v>
       </c>
-      <c r="N27" s="7">
+      <c r="N27" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4132,7 +4129,7 @@
       <c r="P27" s="5">
         <v>7224.57</v>
       </c>
-      <c r="Q27" s="9">
+      <c r="Q27" s="8">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
@@ -4142,7 +4139,7 @@
       <c r="S27" s="5">
         <v>7283.87</v>
       </c>
-      <c r="T27" s="9">
+      <c r="T27" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4150,14 +4147,14 @@
       <c r="V27" s="5">
         <v>0</v>
       </c>
-      <c r="W27" s="10"/>
+      <c r="W27" s="9"/>
       <c r="X27" s="1">
         <v>13909.37</v>
       </c>
       <c r="Y27" s="5">
         <v>21214.42</v>
       </c>
-      <c r="Z27" s="9">
+      <c r="Z27" s="8">
         <f t="shared" si="5"/>
         <v>-7305.0499999999975</v>
       </c>
@@ -4167,7 +4164,7 @@
       <c r="AB27" s="5">
         <v>45022.87</v>
       </c>
-      <c r="AC27" s="9">
+      <c r="AC27" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4177,22 +4174,22 @@
       <c r="AE27" s="5">
         <v>93684.92</v>
       </c>
-      <c r="AF27" s="9">
+      <c r="AF27" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG27" s="14">
+      <c r="AG27" s="13">
         <v>0.91119750217455808</v>
       </c>
-      <c r="AH27" s="20">
+      <c r="AH27">
         <v>0.912215</v>
       </c>
-      <c r="AI27" s="15">
+      <c r="AI27" s="14">
         <f t="shared" si="8"/>
         <v>-1.0174978254419154E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>42</v>
       </c>
@@ -4208,7 +4205,7 @@
       <c r="E28" s="5">
         <v>124.117</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4222,7 +4219,7 @@
       <c r="J28" s="5">
         <v>105.25</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K28" s="6">
         <f t="shared" si="1"/>
         <v>-1.1500000000000057</v>
       </c>
@@ -4232,7 +4229,7 @@
       <c r="M28" s="5">
         <v>103.6</v>
       </c>
-      <c r="N28" s="7">
+      <c r="N28" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4242,7 +4239,7 @@
       <c r="P28" s="5">
         <v>6778.4</v>
       </c>
-      <c r="Q28" s="9">
+      <c r="Q28" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4252,7 +4249,7 @@
       <c r="S28" s="5">
         <v>6838.02</v>
       </c>
-      <c r="T28" s="9">
+      <c r="T28" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4260,14 +4257,14 @@
       <c r="V28" s="5">
         <v>0</v>
       </c>
-      <c r="W28" s="10"/>
+      <c r="W28" s="9"/>
       <c r="X28" s="1">
         <v>6627.95</v>
       </c>
       <c r="Y28" s="5">
         <v>19462.71</v>
       </c>
-      <c r="Z28" s="9">
+      <c r="Z28" s="8">
         <f t="shared" si="5"/>
         <v>-12834.759999999998</v>
       </c>
@@ -4277,7 +4274,7 @@
       <c r="AB28" s="5">
         <v>44577.15</v>
       </c>
-      <c r="AC28" s="9">
+      <c r="AC28" s="8">
         <f t="shared" si="6"/>
         <v>-6836.7000000000044</v>
       </c>
@@ -4287,22 +4284,22 @@
       <c r="AE28" s="5">
         <v>93238.29</v>
       </c>
-      <c r="AF28" s="9">
+      <c r="AF28" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG28" s="14">
+      <c r="AG28" s="13">
         <v>0.91740136721349375</v>
       </c>
-      <c r="AH28" s="20">
+      <c r="AH28">
         <v>0.91833699999999996</v>
       </c>
-      <c r="AI28" s="15">
+      <c r="AI28" s="14">
         <f t="shared" si="8"/>
         <v>-9.3563278650621307E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>43</v>
       </c>
@@ -4318,7 +4315,7 @@
       <c r="E29" s="5">
         <v>120.95</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <f t="shared" si="0"/>
         <v>1.6999999999995907E-2</v>
       </c>
@@ -4332,7 +4329,7 @@
       <c r="J29" s="5">
         <v>104.8</v>
       </c>
-      <c r="K29" s="7">
+      <c r="K29" s="6">
         <f t="shared" si="1"/>
         <v>-1.4500000000000028</v>
       </c>
@@ -4342,7 +4339,7 @@
       <c r="M29" s="5">
         <v>103.283</v>
       </c>
-      <c r="N29" s="7">
+      <c r="N29" s="6">
         <f t="shared" si="2"/>
         <v>1.6999999999995907E-2</v>
       </c>
@@ -4352,7 +4349,7 @@
       <c r="P29" s="5">
         <v>7385.12</v>
       </c>
-      <c r="Q29" s="9">
+      <c r="Q29" s="8">
         <f t="shared" si="3"/>
         <v>-1.5</v>
       </c>
@@ -4362,7 +4359,7 @@
       <c r="S29" s="5">
         <v>7444.44</v>
       </c>
-      <c r="T29" s="9">
+      <c r="T29" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4370,14 +4367,14 @@
       <c r="V29" s="5">
         <v>0</v>
       </c>
-      <c r="W29" s="10"/>
+      <c r="W29" s="9"/>
       <c r="X29" s="1">
         <v>14067.49</v>
       </c>
       <c r="Y29" s="5">
         <v>20353.93</v>
       </c>
-      <c r="Z29" s="9">
+      <c r="Z29" s="8">
         <f t="shared" si="5"/>
         <v>-6286.4400000000005</v>
       </c>
@@ -4387,7 +4384,7 @@
       <c r="AB29" s="5">
         <v>45182.39</v>
       </c>
-      <c r="AC29" s="9">
+      <c r="AC29" s="8">
         <f t="shared" si="6"/>
         <v>1.8600000000005821</v>
       </c>
@@ -4397,22 +4394,22 @@
       <c r="AE29" s="5">
         <v>93844.44</v>
       </c>
-      <c r="AF29" s="9">
+      <c r="AF29" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG29" s="14">
+      <c r="AG29" s="13">
         <v>0.90184813249726981</v>
       </c>
-      <c r="AH29" s="20">
+      <c r="AH29">
         <v>0.90239000000000003</v>
       </c>
-      <c r="AI29" s="15">
+      <c r="AI29" s="14">
         <f t="shared" si="8"/>
         <v>-5.4186750273022E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>44</v>
       </c>
@@ -4428,7 +4425,7 @@
       <c r="E30" s="5">
         <v>120.533</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4442,7 +4439,7 @@
       <c r="J30" s="5">
         <v>103.18300000000001</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="6">
         <f t="shared" si="1"/>
         <v>-0.75</v>
       </c>
@@ -4452,7 +4449,7 @@
       <c r="M30" s="5">
         <v>101.8</v>
       </c>
-      <c r="N30" s="7">
+      <c r="N30" s="6">
         <f t="shared" si="2"/>
         <v>-1.6999999999995907E-2</v>
       </c>
@@ -4462,7 +4459,7 @@
       <c r="P30" s="5">
         <v>7244.53</v>
       </c>
-      <c r="Q30" s="9">
+      <c r="Q30" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4472,7 +4469,7 @@
       <c r="S30" s="5">
         <v>7304.16</v>
       </c>
-      <c r="T30" s="9">
+      <c r="T30" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4480,14 +4477,14 @@
       <c r="V30" s="5">
         <v>0</v>
       </c>
-      <c r="W30" s="10"/>
+      <c r="W30" s="9"/>
       <c r="X30" s="1">
         <v>13928.38</v>
       </c>
       <c r="Y30" s="5">
         <v>19430.419999999998</v>
       </c>
-      <c r="Z30" s="9">
+      <c r="Z30" s="8">
         <f t="shared" si="5"/>
         <v>-5502.0399999999991</v>
       </c>
@@ -4497,7 +4494,7 @@
       <c r="AB30" s="5">
         <v>45042.99</v>
       </c>
-      <c r="AC30" s="9">
+      <c r="AC30" s="8">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -4507,22 +4504,22 @@
       <c r="AE30" s="5">
         <v>93704.21</v>
       </c>
-      <c r="AF30" s="9">
+      <c r="AF30" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG30" s="14">
+      <c r="AG30" s="13">
         <v>0.91584433411827804</v>
       </c>
-      <c r="AH30" s="20">
+      <c r="AH30">
         <v>0.91680700000000004</v>
       </c>
-      <c r="AI30" s="15">
+      <c r="AI30" s="14">
         <f t="shared" si="8"/>
         <v>-9.626658817220024E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>45</v>
       </c>
@@ -4538,7 +4535,7 @@
       <c r="E31" s="5">
         <v>121.6</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4552,7 +4549,7 @@
       <c r="J31" s="5">
         <v>104.68300000000001</v>
       </c>
-      <c r="K31" s="7">
+      <c r="K31" s="6">
         <f t="shared" si="1"/>
         <v>-1.25</v>
       </c>
@@ -4562,7 +4559,7 @@
       <c r="M31" s="5">
         <v>103.267</v>
       </c>
-      <c r="N31" s="7">
+      <c r="N31" s="6">
         <f t="shared" si="2"/>
         <v>-1.6999999999995907E-2</v>
       </c>
@@ -4572,7 +4569,7 @@
       <c r="P31" s="5">
         <v>7108.57</v>
       </c>
-      <c r="Q31" s="9">
+      <c r="Q31" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4582,7 +4579,7 @@
       <c r="S31" s="5">
         <v>7168.21</v>
       </c>
-      <c r="T31" s="9">
+      <c r="T31" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4590,14 +4587,14 @@
       <c r="V31" s="5">
         <v>0</v>
       </c>
-      <c r="W31" s="10"/>
+      <c r="W31" s="9"/>
       <c r="X31" s="1">
         <v>13794.41</v>
       </c>
       <c r="Y31" s="5">
         <v>21381.53</v>
       </c>
-      <c r="Z31" s="9">
+      <c r="Z31" s="8">
         <f t="shared" si="5"/>
         <v>-7587.119999999999</v>
       </c>
@@ -4607,7 +4604,7 @@
       <c r="AB31" s="5">
         <v>44907.66</v>
       </c>
-      <c r="AC31" s="9">
+      <c r="AC31" s="8">
         <f t="shared" si="6"/>
         <v>-0.55000000000291038</v>
       </c>
@@ -4617,22 +4614,22 @@
       <c r="AE31" s="5">
         <v>93570.54</v>
       </c>
-      <c r="AF31" s="9">
+      <c r="AF31" s="8">
         <f t="shared" si="7"/>
         <v>-2.9899999999906868</v>
       </c>
-      <c r="AG31" s="14">
+      <c r="AG31" s="13">
         <v>0.91582419377934587</v>
       </c>
-      <c r="AH31" s="20">
+      <c r="AH31">
         <v>0.91665300000000005</v>
       </c>
-      <c r="AI31" s="15">
+      <c r="AI31" s="14">
         <f t="shared" si="8"/>
         <v>-8.2880622065417686E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>46</v>
       </c>
@@ -4648,7 +4645,7 @@
       <c r="E32" s="5">
         <v>120.5</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4662,7 +4659,7 @@
       <c r="J32" s="5">
         <v>103.85</v>
       </c>
-      <c r="K32" s="7">
+      <c r="K32" s="6">
         <f t="shared" si="1"/>
         <v>-0.91699999999998738</v>
       </c>
@@ -4672,7 +4669,7 @@
       <c r="M32" s="5">
         <v>102.483</v>
       </c>
-      <c r="N32" s="7">
+      <c r="N32" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4682,7 +4679,7 @@
       <c r="P32" s="5">
         <v>6894.89</v>
       </c>
-      <c r="Q32" s="9">
+      <c r="Q32" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4692,7 +4689,7 @@
       <c r="S32" s="5">
         <v>6954.46</v>
       </c>
-      <c r="T32" s="9">
+      <c r="T32" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4700,14 +4697,14 @@
       <c r="V32" s="5">
         <v>0</v>
       </c>
-      <c r="W32" s="10"/>
+      <c r="W32" s="9"/>
       <c r="X32" s="1">
         <v>13584.57</v>
       </c>
       <c r="Y32" s="5">
         <v>18651.54</v>
       </c>
-      <c r="Z32" s="9">
+      <c r="Z32" s="8">
         <f t="shared" si="5"/>
         <v>-5066.9700000000012</v>
       </c>
@@ -4717,7 +4714,7 @@
       <c r="AB32" s="5">
         <v>44693.81</v>
       </c>
-      <c r="AC32" s="9">
+      <c r="AC32" s="8">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -4727,22 +4724,22 @@
       <c r="AE32" s="5">
         <v>93355.41</v>
       </c>
-      <c r="AF32" s="9">
+      <c r="AF32" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG32" s="14">
+      <c r="AG32" s="13">
         <v>0.91000303824766082</v>
       </c>
-      <c r="AH32" s="20">
+      <c r="AH32">
         <v>0.91107800000000005</v>
       </c>
-      <c r="AI32" s="15">
+      <c r="AI32" s="14">
         <f t="shared" si="8"/>
         <v>-1.0749617523392319E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>47</v>
       </c>
@@ -4758,7 +4755,7 @@
       <c r="E33" s="5">
         <v>120.267</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="6">
         <f t="shared" si="0"/>
         <v>-3.3999999999991815E-2</v>
       </c>
@@ -4772,7 +4769,7 @@
       <c r="J33" s="5">
         <v>102.883</v>
       </c>
-      <c r="K33" s="7">
+      <c r="K33" s="6">
         <f t="shared" si="1"/>
         <v>-0.66599999999999682</v>
       </c>
@@ -4782,7 +4779,7 @@
       <c r="M33" s="5">
         <v>101.5</v>
       </c>
-      <c r="N33" s="7">
+      <c r="N33" s="6">
         <f t="shared" si="2"/>
         <v>1.6999999999995907E-2</v>
       </c>
@@ -4792,7 +4789,7 @@
       <c r="P33" s="5">
         <v>7237.02</v>
       </c>
-      <c r="Q33" s="9">
+      <c r="Q33" s="8">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
@@ -4802,7 +4799,7 @@
       <c r="S33" s="5">
         <v>7296.25</v>
       </c>
-      <c r="T33" s="9">
+      <c r="T33" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4810,14 +4807,14 @@
       <c r="V33" s="5">
         <v>0</v>
       </c>
-      <c r="W33" s="10"/>
+      <c r="W33" s="9"/>
       <c r="X33" s="1">
         <v>13926.23</v>
       </c>
       <c r="Y33" s="5">
         <v>19650.3</v>
       </c>
-      <c r="Z33" s="9">
+      <c r="Z33" s="8">
         <f t="shared" si="5"/>
         <v>-5724.07</v>
       </c>
@@ -4827,7 +4824,7 @@
       <c r="AB33" s="5">
         <v>45035.69</v>
       </c>
-      <c r="AC33" s="9">
+      <c r="AC33" s="8">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -4837,22 +4834,22 @@
       <c r="AE33" s="5">
         <v>93696.33</v>
       </c>
-      <c r="AF33" s="9">
+      <c r="AF33" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG33" s="14">
+      <c r="AG33" s="13">
         <v>0.91609225355188495</v>
       </c>
-      <c r="AH33" s="20">
+      <c r="AH33">
         <v>0.916883</v>
       </c>
-      <c r="AI33" s="15">
+      <c r="AI33" s="14">
         <f t="shared" si="8"/>
         <v>-7.907464481150539E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>48</v>
       </c>
@@ -4868,7 +4865,7 @@
       <c r="E34" s="5">
         <v>125.017</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <f t="shared" si="0"/>
         <v>-1.6999999999995907E-2</v>
       </c>
@@ -4882,7 +4879,7 @@
       <c r="J34" s="5">
         <v>113.883</v>
       </c>
-      <c r="K34" s="7">
+      <c r="K34" s="6">
         <f t="shared" si="1"/>
         <v>0.15000000000000568</v>
       </c>
@@ -4892,7 +4889,7 @@
       <c r="M34" s="5">
         <v>110.3</v>
       </c>
-      <c r="N34" s="7">
+      <c r="N34" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4902,7 +4899,7 @@
       <c r="P34" s="5">
         <v>8360.42</v>
       </c>
-      <c r="Q34" s="9">
+      <c r="Q34" s="8">
         <f t="shared" si="3"/>
         <v>-0.98999999999978172</v>
       </c>
@@ -4912,7 +4909,7 @@
       <c r="S34" s="5">
         <v>8419.6299999999992</v>
       </c>
-      <c r="T34" s="9">
+      <c r="T34" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -4920,14 +4917,14 @@
       <c r="V34" s="5">
         <v>0</v>
       </c>
-      <c r="W34" s="10"/>
+      <c r="W34" s="9"/>
       <c r="X34" s="1">
         <v>15047.09</v>
       </c>
       <c r="Y34" s="5">
         <v>15365.1</v>
       </c>
-      <c r="Z34" s="9">
+      <c r="Z34" s="8">
         <f t="shared" si="5"/>
         <v>-318.01000000000022</v>
       </c>
@@ -4937,7 +4934,7 @@
       <c r="AB34" s="5">
         <v>46157.95</v>
       </c>
-      <c r="AC34" s="9">
+      <c r="AC34" s="8">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
@@ -4947,22 +4944,22 @@
       <c r="AE34" s="5">
         <v>94819.75</v>
       </c>
-      <c r="AF34" s="9">
+      <c r="AF34" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG34" s="14">
+      <c r="AG34" s="13">
         <v>0.93137405678912</v>
       </c>
-      <c r="AH34" s="20">
+      <c r="AH34">
         <v>0.932176</v>
       </c>
-      <c r="AI34" s="15">
+      <c r="AI34" s="14">
         <f t="shared" si="8"/>
         <v>-8.0194321088000731E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>50</v>
       </c>
@@ -4978,7 +4975,7 @@
       <c r="E35" s="5">
         <v>124.117</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4992,7 +4989,7 @@
       <c r="J35" s="5">
         <v>120.06699999999999</v>
       </c>
-      <c r="K35" s="7">
+      <c r="K35" s="6">
         <f t="shared" si="1"/>
         <v>-7.3839999999999861</v>
       </c>
@@ -5002,7 +4999,7 @@
       <c r="M35" s="5">
         <v>123.917</v>
       </c>
-      <c r="N35" s="7">
+      <c r="N35" s="6">
         <f t="shared" si="2"/>
         <v>-14.733999999999995</v>
       </c>
@@ -5012,7 +5009,7 @@
       <c r="P35" s="5">
         <v>8171.06</v>
       </c>
-      <c r="Q35" s="9">
+      <c r="Q35" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5022,7 +5019,7 @@
       <c r="S35" s="5">
         <v>8231.0400000000009</v>
       </c>
-      <c r="T35" s="9">
+      <c r="T35" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -5030,14 +5027,14 @@
       <c r="V35" s="5">
         <v>0</v>
       </c>
-      <c r="W35" s="10"/>
+      <c r="W35" s="9"/>
       <c r="X35" s="1">
         <v>14854.03</v>
       </c>
       <c r="Y35" s="5">
         <v>11307.67</v>
       </c>
-      <c r="Z35" s="9">
+      <c r="Z35" s="8">
         <f t="shared" si="5"/>
         <v>3546.3600000000006</v>
       </c>
@@ -5047,7 +5044,7 @@
       <c r="AB35" s="5">
         <v>14232.62</v>
       </c>
-      <c r="AC35" s="9">
+      <c r="AC35" s="8">
         <f t="shared" si="6"/>
         <v>31737.589999999997</v>
       </c>
@@ -5057,22 +5054,22 @@
       <c r="AE35" s="5">
         <v>94632.22</v>
       </c>
-      <c r="AF35" s="9">
+      <c r="AF35" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG35" s="14">
+      <c r="AG35" s="13">
         <v>0.93408475016627335</v>
       </c>
-      <c r="AH35" s="20">
+      <c r="AH35">
         <v>0.93575699999999995</v>
       </c>
-      <c r="AI35" s="15">
+      <c r="AI35" s="14">
         <f t="shared" si="8"/>
         <v>-1.6722498337266023E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>51</v>
       </c>
@@ -5088,7 +5085,7 @@
       <c r="E36" s="5">
         <v>124.967</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="6">
         <f t="shared" si="0"/>
         <v>-1.6999999999995907E-2</v>
       </c>
@@ -5102,7 +5099,7 @@
       <c r="J36" s="5">
         <v>120.667</v>
       </c>
-      <c r="K36" s="7">
+      <c r="K36" s="6">
         <f t="shared" si="1"/>
         <v>-6.8170000000000073</v>
       </c>
@@ -5112,7 +5109,7 @@
       <c r="M36" s="5">
         <v>125.283</v>
       </c>
-      <c r="N36" s="7">
+      <c r="N36" s="6">
         <f t="shared" si="2"/>
         <v>-15.283000000000001</v>
       </c>
@@ -5122,7 +5119,7 @@
       <c r="P36" s="5">
         <v>8439.42</v>
       </c>
-      <c r="Q36" s="9">
+      <c r="Q36" s="8">
         <f t="shared" si="3"/>
         <v>-1.5499999999992724</v>
       </c>
@@ -5132,7 +5129,7 @@
       <c r="S36" s="5">
         <v>8497.9</v>
       </c>
-      <c r="T36" s="9">
+      <c r="T36" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -5140,14 +5137,14 @@
       <c r="V36" s="5">
         <v>0</v>
       </c>
-      <c r="W36" s="10"/>
+      <c r="W36" s="9"/>
       <c r="X36" s="1">
         <v>15122.77</v>
       </c>
       <c r="Y36" s="5">
         <v>11573.9</v>
       </c>
-      <c r="Z36" s="9">
+      <c r="Z36" s="8">
         <f t="shared" si="5"/>
         <v>3548.8700000000008</v>
       </c>
@@ -5157,7 +5154,7 @@
       <c r="AB36" s="5">
         <v>14498.96</v>
       </c>
-      <c r="AC36" s="9">
+      <c r="AC36" s="8">
         <f t="shared" si="6"/>
         <v>31738.230000000003</v>
       </c>
@@ -5167,22 +5164,22 @@
       <c r="AE36" s="5">
         <v>94899.36</v>
       </c>
-      <c r="AF36" s="9">
+      <c r="AF36" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG36" s="14">
+      <c r="AG36" s="13">
         <v>0.9313425672130492</v>
       </c>
-      <c r="AH36" s="20">
+      <c r="AH36">
         <v>0.93194100000000002</v>
       </c>
-      <c r="AI36" s="15">
+      <c r="AI36" s="14">
         <f t="shared" si="8"/>
         <v>-5.9843278695081992E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>52</v>
       </c>
@@ -5198,7 +5195,7 @@
       <c r="E37" s="5">
         <v>124.5</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5212,7 +5209,7 @@
       <c r="J37" s="5">
         <v>119.483</v>
       </c>
-      <c r="K37" s="7">
+      <c r="K37" s="6">
         <f t="shared" si="1"/>
         <v>-6.666000000000011</v>
       </c>
@@ -5222,7 +5219,7 @@
       <c r="M37" s="5">
         <v>124.583</v>
       </c>
-      <c r="N37" s="7">
+      <c r="N37" s="6">
         <f t="shared" si="2"/>
         <v>-15.182999999999993</v>
       </c>
@@ -5232,7 +5229,7 @@
       <c r="P37" s="5">
         <v>8416.5499999999993</v>
       </c>
-      <c r="Q37" s="9">
+      <c r="Q37" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5242,7 +5239,7 @@
       <c r="S37" s="5">
         <v>8476.1</v>
       </c>
-      <c r="T37" s="9">
+      <c r="T37" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -5250,14 +5247,14 @@
       <c r="V37" s="5">
         <v>0</v>
       </c>
-      <c r="W37" s="10"/>
+      <c r="W37" s="9"/>
       <c r="X37" s="1">
         <v>15103.71</v>
       </c>
       <c r="Y37" s="5">
         <v>11556.2</v>
       </c>
-      <c r="Z37" s="9">
+      <c r="Z37" s="8">
         <f t="shared" si="5"/>
         <v>3547.5099999999984</v>
       </c>
@@ -5267,7 +5264,7 @@
       <c r="AB37" s="5">
         <v>14477.93</v>
       </c>
-      <c r="AC37" s="9">
+      <c r="AC37" s="8">
         <f t="shared" si="6"/>
         <v>31737.129999999997</v>
       </c>
@@ -5277,22 +5274,22 @@
       <c r="AE37" s="5">
         <v>94877.36</v>
       </c>
-      <c r="AF37" s="9">
+      <c r="AF37" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG37" s="14">
+      <c r="AG37" s="13">
         <v>0.92871686126712338</v>
       </c>
-      <c r="AH37" s="20">
+      <c r="AH37">
         <v>0.92961099999999997</v>
       </c>
-      <c r="AI37" s="15">
+      <c r="AI37" s="14">
         <f t="shared" si="8"/>
         <v>-8.9413873287658152E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>53</v>
       </c>
@@ -5306,7 +5303,7 @@
         <v>124.8</v>
       </c>
       <c r="E38" s="5"/>
-      <c r="F38" s="7">
+      <c r="F38" s="6">
         <f t="shared" si="0"/>
         <v>124.8</v>
       </c>
@@ -5316,7 +5313,7 @@
         <v>114.133</v>
       </c>
       <c r="J38" s="5"/>
-      <c r="K38" s="7">
+      <c r="K38" s="6">
         <f t="shared" si="1"/>
         <v>114.133</v>
       </c>
@@ -5324,7 +5321,7 @@
         <v>110.283</v>
       </c>
       <c r="M38" s="5"/>
-      <c r="N38" s="7">
+      <c r="N38" s="6">
         <f t="shared" si="2"/>
         <v>110.283</v>
       </c>
@@ -5332,7 +5329,7 @@
         <v>8581.5300000000007</v>
       </c>
       <c r="P38" s="5"/>
-      <c r="Q38" s="9">
+      <c r="Q38" s="8">
         <f t="shared" si="3"/>
         <v>8581.5300000000007</v>
       </c>
@@ -5340,18 +5337,18 @@
         <v>8642.0499999999993</v>
       </c>
       <c r="S38" s="5"/>
-      <c r="T38" s="9">
+      <c r="T38" s="8">
         <f t="shared" si="4"/>
         <v>8642.0499999999993</v>
       </c>
       <c r="U38" s="1"/>
       <c r="V38" s="5"/>
-      <c r="W38" s="10"/>
+      <c r="W38" s="9"/>
       <c r="X38" s="1">
         <v>15268.74</v>
       </c>
       <c r="Y38" s="5"/>
-      <c r="Z38" s="9">
+      <c r="Z38" s="8">
         <f t="shared" si="5"/>
         <v>15268.74</v>
       </c>
@@ -5359,7 +5356,7 @@
         <v>46381.13</v>
       </c>
       <c r="AB38" s="5"/>
-      <c r="AC38" s="9">
+      <c r="AC38" s="8">
         <f t="shared" si="6"/>
         <v>46381.13</v>
       </c>
@@ -5367,22 +5364,22 @@
         <v>95043.94</v>
       </c>
       <c r="AE38" s="5"/>
-      <c r="AF38" s="9">
+      <c r="AF38" s="8">
         <f t="shared" si="7"/>
         <v>95043.94</v>
       </c>
-      <c r="AG38" s="14">
+      <c r="AG38" s="13">
         <v>0.92668440912607419</v>
       </c>
-      <c r="AH38" s="20">
+      <c r="AH38">
         <v>0.93071999999999999</v>
       </c>
-      <c r="AI38" s="15">
+      <c r="AI38" s="14">
         <f t="shared" si="8"/>
         <v>-4.0355908739257984E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>55</v>
       </c>
@@ -5398,7 +5395,7 @@
       <c r="E39" s="5">
         <v>125.3</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5412,7 +5409,7 @@
       <c r="J39" s="5">
         <v>120.283</v>
       </c>
-      <c r="K39" s="7">
+      <c r="K39" s="6">
         <f t="shared" si="1"/>
         <v>-5.8329999999999984</v>
       </c>
@@ -5422,7 +5419,7 @@
       <c r="M39" s="5">
         <v>125.417</v>
       </c>
-      <c r="N39" s="7">
+      <c r="N39" s="6">
         <f t="shared" si="2"/>
         <v>-14.834000000000003</v>
       </c>
@@ -5432,7 +5429,7 @@
       <c r="P39" s="5">
         <v>7198.68</v>
       </c>
-      <c r="Q39" s="9">
+      <c r="Q39" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5442,7 +5439,7 @@
       <c r="S39" s="5">
         <v>7258.19</v>
       </c>
-      <c r="T39" s="9">
+      <c r="T39" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -5450,14 +5447,14 @@
       <c r="V39" s="5">
         <v>0</v>
       </c>
-      <c r="W39" s="10"/>
+      <c r="W39" s="9"/>
       <c r="X39" s="1">
         <v>13886.24</v>
       </c>
       <c r="Y39" s="5">
         <v>10336.27</v>
       </c>
-      <c r="Z39" s="9">
+      <c r="Z39" s="8">
         <f t="shared" si="5"/>
         <v>3549.9699999999993</v>
       </c>
@@ -5467,7 +5464,7 @@
       <c r="AB39" s="5">
         <v>13260.2</v>
       </c>
-      <c r="AC39" s="9">
+      <c r="AC39" s="8">
         <f t="shared" si="6"/>
         <v>31737.05</v>
       </c>
@@ -5477,22 +5474,22 @@
       <c r="AE39" s="5">
         <v>93659.01</v>
       </c>
-      <c r="AF39" s="9">
+      <c r="AF39" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG39" s="14">
+      <c r="AG39" s="13">
         <v>0.93102933417843436</v>
       </c>
-      <c r="AH39" s="20">
+      <c r="AH39">
         <v>0.93223800000000001</v>
       </c>
-      <c r="AI39" s="15">
+      <c r="AI39" s="14">
         <f t="shared" si="8"/>
         <v>-1.2086658215656465E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>56</v>
       </c>
@@ -5508,7 +5505,7 @@
       <c r="E40" s="5">
         <v>124.083</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="6">
         <f t="shared" si="0"/>
         <v>3.4000000000006025E-2</v>
       </c>
@@ -5522,7 +5519,7 @@
       <c r="J40" s="5">
         <v>121.283</v>
       </c>
-      <c r="K40" s="7">
+      <c r="K40" s="6">
         <f t="shared" si="1"/>
         <v>-8.8499999999999943</v>
       </c>
@@ -5532,7 +5529,7 @@
       <c r="M40" s="5">
         <v>123.983</v>
       </c>
-      <c r="N40" s="7">
+      <c r="N40" s="6">
         <f t="shared" si="2"/>
         <v>-14.816000000000003</v>
       </c>
@@ -5542,7 +5539,7 @@
       <c r="P40" s="5">
         <v>8427.66</v>
       </c>
-      <c r="Q40" s="9">
+      <c r="Q40" s="8">
         <f t="shared" si="3"/>
         <v>-1.0300000000006548</v>
       </c>
@@ -5552,7 +5549,7 @@
       <c r="S40" s="5">
         <v>8487.11</v>
       </c>
-      <c r="T40" s="9">
+      <c r="T40" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -5560,14 +5557,14 @@
       <c r="V40" s="5">
         <v>0</v>
       </c>
-      <c r="W40" s="10"/>
+      <c r="W40" s="9"/>
       <c r="X40" s="1">
         <v>15114.83</v>
       </c>
       <c r="Y40" s="5">
         <v>11566.78</v>
       </c>
-      <c r="Z40" s="9">
+      <c r="Z40" s="8">
         <f t="shared" si="5"/>
         <v>3548.0499999999993</v>
       </c>
@@ -5577,7 +5574,7 @@
       <c r="AB40" s="5">
         <v>14488.73</v>
       </c>
-      <c r="AC40" s="9">
+      <c r="AC40" s="8">
         <f t="shared" si="6"/>
         <v>31737.969999999998</v>
       </c>
@@ -5587,22 +5584,22 @@
       <c r="AE40" s="5">
         <v>94889.5</v>
       </c>
-      <c r="AF40" s="9">
+      <c r="AF40" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG40" s="14">
+      <c r="AG40" s="13">
         <v>0.92971749366237477</v>
       </c>
-      <c r="AH40" s="20">
+      <c r="AH40">
         <v>0.93131399999999998</v>
       </c>
-      <c r="AI40" s="15">
+      <c r="AI40" s="14">
         <f t="shared" si="8"/>
         <v>-1.5965063376252031E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
@@ -5618,7 +5615,7 @@
       <c r="E41" s="5">
         <v>159.69999999999999</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5632,7 +5629,7 @@
       <c r="J41" s="5">
         <v>146.19999999999999</v>
       </c>
-      <c r="K41" s="7">
+      <c r="K41" s="6">
         <f t="shared" si="1"/>
         <v>6.7000000000007276E-2</v>
       </c>
@@ -5642,7 +5639,7 @@
       <c r="M41" s="5">
         <v>141.88300000000001</v>
       </c>
-      <c r="N41" s="7">
+      <c r="N41" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5652,7 +5649,7 @@
       <c r="P41" s="5">
         <v>23193.74</v>
       </c>
-      <c r="Q41" s="9">
+      <c r="Q41" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5662,7 +5659,7 @@
       <c r="S41" s="5">
         <v>23253.25</v>
       </c>
-      <c r="T41" s="9">
+      <c r="T41" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -5670,14 +5667,14 @@
       <c r="V41" s="5">
         <v>0</v>
       </c>
-      <c r="W41" s="10"/>
+      <c r="W41" s="9"/>
       <c r="X41" s="1">
         <v>29882.43</v>
       </c>
       <c r="Y41" s="5">
         <v>30194.39</v>
       </c>
-      <c r="Z41" s="9">
+      <c r="Z41" s="8">
         <f t="shared" si="5"/>
         <v>-311.95999999999913</v>
       </c>
@@ -5687,7 +5684,7 @@
       <c r="AB41" s="5">
         <v>60992.01</v>
       </c>
-      <c r="AC41" s="9">
+      <c r="AC41" s="8">
         <f t="shared" si="6"/>
         <v>1.0099999999947613</v>
       </c>
@@ -5697,22 +5694,22 @@
       <c r="AE41" s="5">
         <v>109654.47</v>
       </c>
-      <c r="AF41" s="9">
+      <c r="AF41" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG41" s="14">
+      <c r="AG41" s="13">
         <v>0.88089077504082924</v>
       </c>
-      <c r="AH41" s="20">
+      <c r="AH41">
         <v>0.88151199999999996</v>
       </c>
-      <c r="AI41" s="15">
+      <c r="AI41" s="14">
         <f t="shared" si="8"/>
         <v>-6.2122495917071863E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>58</v>
       </c>
@@ -5728,7 +5725,7 @@
       <c r="E42" s="5">
         <v>125.4</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5742,7 +5739,7 @@
       <c r="J42" s="5">
         <v>114.483</v>
       </c>
-      <c r="K42" s="7">
+      <c r="K42" s="6">
         <f t="shared" si="1"/>
         <v>1.6999999999995907E-2</v>
       </c>
@@ -5752,7 +5749,7 @@
       <c r="M42" s="5">
         <v>111.017</v>
       </c>
-      <c r="N42" s="7">
+      <c r="N42" s="6">
         <f t="shared" si="2"/>
         <v>4.9999999999997158E-2</v>
       </c>
@@ -5762,7 +5759,7 @@
       <c r="P42" s="5">
         <v>8579.2099999999991</v>
       </c>
-      <c r="Q42" s="9">
+      <c r="Q42" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5772,7 +5769,7 @@
       <c r="S42" s="5">
         <v>8638.86</v>
       </c>
-      <c r="T42" s="9">
+      <c r="T42" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -5780,14 +5777,14 @@
       <c r="V42" s="5">
         <v>0</v>
       </c>
-      <c r="W42" s="10"/>
+      <c r="W42" s="9"/>
       <c r="X42" s="1">
         <v>15264.06</v>
       </c>
       <c r="Y42" s="5">
         <v>15573.43</v>
       </c>
-      <c r="Z42" s="9">
+      <c r="Z42" s="8">
         <f t="shared" si="5"/>
         <v>-309.3700000000008</v>
       </c>
@@ -5797,7 +5794,7 @@
       <c r="AB42" s="5">
         <v>46377.88</v>
       </c>
-      <c r="AC42" s="9">
+      <c r="AC42" s="8">
         <f t="shared" si="6"/>
         <v>0.99000000000523869</v>
       </c>
@@ -5807,22 +5804,22 @@
       <c r="AE42" s="5">
         <v>95040.7</v>
       </c>
-      <c r="AF42" s="9">
+      <c r="AF42" s="8">
         <f t="shared" si="7"/>
         <v>-2.9899999999906868</v>
       </c>
-      <c r="AG42" s="14">
+      <c r="AG42" s="13">
         <v>0.9331024980123428</v>
       </c>
-      <c r="AH42" s="20">
+      <c r="AH42">
         <v>0.93426500000000001</v>
       </c>
-      <c r="AI42" s="15">
+      <c r="AI42" s="14">
         <f t="shared" si="8"/>
         <v>-1.1625019876572162E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>60</v>
       </c>
@@ -5838,7 +5835,7 @@
       <c r="E43" s="5">
         <v>125.25</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5852,7 +5849,7 @@
       <c r="J43" s="5">
         <v>113.833</v>
       </c>
-      <c r="K43" s="7">
+      <c r="K43" s="6">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
@@ -5862,7 +5859,7 @@
       <c r="M43" s="5">
         <v>109.967</v>
       </c>
-      <c r="N43" s="7">
+      <c r="N43" s="6">
         <f t="shared" si="2"/>
         <v>-1.6999999999995907E-2</v>
       </c>
@@ -5872,7 +5869,7 @@
       <c r="P43" s="5">
         <v>8082.61</v>
       </c>
-      <c r="Q43" s="9">
+      <c r="Q43" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5882,7 +5879,7 @@
       <c r="S43" s="5">
         <v>8142.15</v>
       </c>
-      <c r="T43" s="9">
+      <c r="T43" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -5890,14 +5887,14 @@
       <c r="V43" s="5">
         <v>0</v>
       </c>
-      <c r="W43" s="10"/>
+      <c r="W43" s="9"/>
       <c r="X43" s="1">
         <v>14766.28</v>
       </c>
       <c r="Y43" s="5">
         <v>15093.26</v>
       </c>
-      <c r="Z43" s="9">
+      <c r="Z43" s="8">
         <f t="shared" si="5"/>
         <v>-326.97999999999956</v>
       </c>
@@ -5907,7 +5904,7 @@
       <c r="AB43" s="5">
         <v>45880.59</v>
       </c>
-      <c r="AC43" s="9">
+      <c r="AC43" s="8">
         <f t="shared" si="6"/>
         <v>1.0100000000020373</v>
       </c>
@@ -5917,22 +5914,22 @@
       <c r="AE43" s="5">
         <v>94542.42</v>
       </c>
-      <c r="AF43" s="9">
+      <c r="AF43" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG43" s="14">
+      <c r="AG43" s="13">
         <v>0.92968255944153733</v>
       </c>
-      <c r="AH43" s="20">
+      <c r="AH43">
         <v>0.93054800000000004</v>
       </c>
-      <c r="AI43" s="15">
+      <c r="AI43" s="14">
         <f t="shared" si="8"/>
         <v>-8.6544055846271561E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>61</v>
       </c>
@@ -5948,7 +5945,7 @@
       <c r="E44" s="5">
         <v>125.217</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F44" s="6">
         <f t="shared" si="0"/>
         <v>-6.6999999999993065E-2</v>
       </c>
@@ -5962,7 +5959,7 @@
       <c r="J44" s="5">
         <v>120.55</v>
       </c>
-      <c r="K44" s="7">
+      <c r="K44" s="6">
         <f t="shared" si="1"/>
         <v>-6.8499999999999943</v>
       </c>
@@ -5972,7 +5969,7 @@
       <c r="M44" s="5">
         <v>125.533</v>
       </c>
-      <c r="N44" s="7">
+      <c r="N44" s="6">
         <f t="shared" si="2"/>
         <v>-15.783000000000001</v>
       </c>
@@ -5982,7 +5979,7 @@
       <c r="P44" s="5">
         <v>8657.41</v>
       </c>
-      <c r="Q44" s="9">
+      <c r="Q44" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5992,7 +5989,7 @@
       <c r="S44" s="5">
         <v>8717.08</v>
       </c>
-      <c r="T44" s="9">
+      <c r="T44" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6000,14 +5997,14 @@
       <c r="V44" s="5">
         <v>0</v>
       </c>
-      <c r="W44" s="10"/>
+      <c r="W44" s="9"/>
       <c r="X44" s="1">
         <v>15343.28</v>
       </c>
       <c r="Y44" s="5">
         <v>11796.7</v>
       </c>
-      <c r="Z44" s="9">
+      <c r="Z44" s="8">
         <f t="shared" si="5"/>
         <v>3546.58</v>
       </c>
@@ -6017,7 +6014,7 @@
       <c r="AB44" s="5">
         <v>14717.97</v>
       </c>
-      <c r="AC44" s="9">
+      <c r="AC44" s="8">
         <f t="shared" si="6"/>
         <v>31737.559999999998</v>
       </c>
@@ -6027,22 +6024,22 @@
       <c r="AE44" s="5">
         <v>95118.77</v>
       </c>
-      <c r="AF44" s="9">
+      <c r="AF44" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG44" s="14">
+      <c r="AG44" s="13">
         <v>0.92867786805463182</v>
       </c>
-      <c r="AH44" s="20">
+      <c r="AH44">
         <v>0.92902600000000002</v>
       </c>
-      <c r="AI44" s="15">
+      <c r="AI44" s="14">
         <f t="shared" si="8"/>
         <v>-3.4813194536820191E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>62</v>
       </c>
@@ -6058,7 +6055,7 @@
       <c r="E45" s="5">
         <v>125.18300000000001</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F45" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6072,7 +6069,7 @@
       <c r="J45" s="5">
         <v>113.217</v>
       </c>
-      <c r="K45" s="7">
+      <c r="K45" s="6">
         <f t="shared" si="1"/>
         <v>0.34999999999999432</v>
       </c>
@@ -6082,7 +6079,7 @@
       <c r="M45" s="5">
         <v>109.68300000000001</v>
       </c>
-      <c r="N45" s="7">
+      <c r="N45" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6092,7 +6089,7 @@
       <c r="P45" s="5">
         <v>8541.34</v>
       </c>
-      <c r="Q45" s="9">
+      <c r="Q45" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -6102,7 +6099,7 @@
       <c r="S45" s="5">
         <v>8601.07</v>
       </c>
-      <c r="T45" s="9">
+      <c r="T45" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6110,14 +6107,14 @@
       <c r="V45" s="5">
         <v>0</v>
       </c>
-      <c r="W45" s="10"/>
+      <c r="W45" s="9"/>
       <c r="X45" s="1">
         <v>15226.12</v>
       </c>
       <c r="Y45" s="5">
         <v>15559.11</v>
       </c>
-      <c r="Z45" s="9">
+      <c r="Z45" s="8">
         <f t="shared" si="5"/>
         <v>-332.98999999999978</v>
       </c>
@@ -6127,7 +6124,7 @@
       <c r="AB45" s="5">
         <v>46340.84</v>
       </c>
-      <c r="AC45" s="9">
+      <c r="AC45" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -6137,22 +6134,22 @@
       <c r="AE45" s="5">
         <v>95004.06</v>
       </c>
-      <c r="AF45" s="9">
+      <c r="AF45" s="8">
         <f t="shared" si="7"/>
         <v>-3</v>
       </c>
-      <c r="AG45" s="14">
+      <c r="AG45" s="13">
         <v>0.92883400573334829</v>
       </c>
-      <c r="AH45" s="20">
+      <c r="AH45">
         <v>0.93041700000000005</v>
       </c>
-      <c r="AI45" s="15">
+      <c r="AI45" s="14">
         <f t="shared" si="8"/>
         <v>-1.5829942666517605E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>63</v>
       </c>
@@ -6162,7 +6159,7 @@
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="5"/>
-      <c r="F46" s="7">
+      <c r="F46" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6170,59 +6167,59 @@
       <c r="H46" s="5"/>
       <c r="I46" s="3"/>
       <c r="J46" s="5"/>
-      <c r="K46" s="7">
+      <c r="K46" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="5"/>
-      <c r="N46" s="7">
+      <c r="N46" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="5"/>
-      <c r="Q46" s="9">
+      <c r="Q46" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R46" s="1"/>
       <c r="S46" s="5"/>
-      <c r="T46" s="9">
+      <c r="T46" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U46" s="1"/>
       <c r="V46" s="5"/>
-      <c r="W46" s="10"/>
+      <c r="W46" s="9"/>
       <c r="X46" s="1"/>
       <c r="Y46" s="5"/>
-      <c r="Z46" s="9">
+      <c r="Z46" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA46" s="1"/>
       <c r="AB46" s="5"/>
-      <c r="AC46" s="9">
+      <c r="AC46" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD46" s="1"/>
       <c r="AE46" s="5"/>
-      <c r="AF46" s="9">
+      <c r="AF46" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG46" s="1"/>
-      <c r="AH46" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI46" s="13">
+      <c r="AH46">
+        <v>0</v>
+      </c>
+      <c r="AI46" s="12">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>64</v>
       </c>
@@ -6238,7 +6235,7 @@
       <c r="E47" s="5">
         <v>119.95</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6252,7 +6249,7 @@
       <c r="J47" s="5">
         <v>119.18300000000001</v>
       </c>
-      <c r="K47" s="7">
+      <c r="K47" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6262,7 +6259,7 @@
       <c r="M47" s="5">
         <v>121.467</v>
       </c>
-      <c r="N47" s="7">
+      <c r="N47" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6272,7 +6269,7 @@
       <c r="P47" s="5">
         <v>6020.29</v>
       </c>
-      <c r="Q47" s="9">
+      <c r="Q47" s="8">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -6282,7 +6279,7 @@
       <c r="S47" s="5">
         <v>6079.98</v>
       </c>
-      <c r="T47" s="9">
+      <c r="T47" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6290,14 +6287,14 @@
       <c r="V47" s="5">
         <v>0</v>
       </c>
-      <c r="W47" s="10"/>
+      <c r="W47" s="9"/>
       <c r="X47" s="1">
         <v>17453.740000000002</v>
       </c>
       <c r="Y47" s="5">
         <v>17453.740000000002</v>
       </c>
-      <c r="Z47" s="9">
+      <c r="Z47" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -6307,7 +6304,7 @@
       <c r="AB47" s="5">
         <v>43820.19</v>
       </c>
-      <c r="AC47" s="9">
+      <c r="AC47" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -6317,80 +6314,80 @@
       <c r="AE47" s="5">
         <v>92481.75</v>
       </c>
-      <c r="AF47" s="9">
+      <c r="AF47" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG47" s="1">
         <v>0.90073495789560953</v>
       </c>
-      <c r="AH47" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI47" s="13">
+      <c r="AH47">
+        <v>0</v>
+      </c>
+      <c r="AI47" s="12">
         <f t="shared" si="8"/>
         <v>0.90073495789560953</v>
       </c>
     </row>
-    <row r="48" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
-      <c r="AH48" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI48" s="9">
+    <row r="48" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AH48">
+        <v>0</v>
+      </c>
+      <c r="AI48" s="8">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="34:35" hidden="1" x14ac:dyDescent="0.3">
-      <c r="AH49" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI49" s="9">
+    <row r="49" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AH49">
+        <v>0</v>
+      </c>
+      <c r="AI49" s="8">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="34:35" hidden="1" x14ac:dyDescent="0.3">
-      <c r="AH50" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI50" s="9">
+    <row r="50" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AH50">
+        <v>0</v>
+      </c>
+      <c r="AI50" s="8">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="34:35" hidden="1" x14ac:dyDescent="0.3">
-      <c r="AH51" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI51" s="9">
+    <row r="51" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AH51">
+        <v>0</v>
+      </c>
+      <c r="AI51" s="8">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="34:35" hidden="1" x14ac:dyDescent="0.3">
-      <c r="AH52" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI52" s="9">
+    <row r="52" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AH52">
+        <v>0</v>
+      </c>
+      <c r="AI52" s="8">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="34:35" hidden="1" x14ac:dyDescent="0.3">
-      <c r="AH53" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI53" s="9">
+    <row r="53" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AH53">
+        <v>0</v>
+      </c>
+      <c r="AI53" s="8">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="34:35" hidden="1" x14ac:dyDescent="0.3">
-      <c r="AH54" s="20">
+    <row r="54" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AH54">
         <v>0.81740599999999997</v>
       </c>
-      <c r="AI54" s="9">
+      <c r="AI54" s="8">
         <f t="shared" si="8"/>
         <v>-0.81740599999999997</v>
       </c>

</xml_diff>

<commit_message>
Several updates to fix FHR calculation
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/UEF Check Sheet.xlsx
+++ b/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/UEF Check Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19D62BC-75B1-4E46-BDD4-6D1139C5294A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0DA583-FE5D-46BB-9A84-F18D702A7C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4525C065-1982-4190-BA1C-76B51CDE7E26}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="96">
   <si>
     <t>Type</t>
   </si>
@@ -364,6 +364,21 @@
   </si>
   <si>
     <t>21WS1092</t>
+  </si>
+  <si>
+    <t>24WS1597</t>
+  </si>
+  <si>
+    <t>50 Heat Pump</t>
+  </si>
+  <si>
+    <t>Lab_ID_65 HP120 DoE_Model</t>
+  </si>
+  <si>
+    <t>65 Heat Pump</t>
+  </si>
+  <si>
+    <t>24WS1595</t>
   </si>
 </sst>
 </file>
@@ -939,7 +954,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -950,6 +964,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1306,15 +1323,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E368A452-0E99-44F6-9903-45AB1358FD53}">
-  <dimension ref="A2:AI54"/>
+  <dimension ref="A2:AI57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AJ9" sqref="AJ9"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AM11" sqref="AM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" hidden="1" customWidth="1"/>
@@ -1349,12 +1366,8 @@
     <col min="33" max="33" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="29" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27.85546875" customWidth="1"/>
-    <col min="40" max="40" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -1468,45 +1481,45 @@
       <c r="A3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>30</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="15">
+      <c r="F3" s="15"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="14">
         <v>4904.07</v>
       </c>
-      <c r="P3" s="15"/>
+      <c r="P3" s="14"/>
       <c r="Q3" s="8">
         <f>O3-P3</f>
         <v>4904.07</v>
       </c>
-      <c r="R3" s="15">
+      <c r="R3" s="14">
         <v>4963.07</v>
       </c>
-      <c r="S3" s="15"/>
+      <c r="S3" s="14"/>
       <c r="T3" s="8">
         <f>R3-S3</f>
         <v>4963.07</v>
       </c>
-      <c r="U3" s="15">
+      <c r="U3" s="14">
         <v>6744.1</v>
       </c>
-      <c r="V3" s="15"/>
+      <c r="V3" s="14"/>
       <c r="W3" s="9"/>
-      <c r="X3" s="15">
+      <c r="X3" s="14">
         <v>13847.21</v>
       </c>
       <c r="Y3" s="5"/>
@@ -1514,31 +1527,31 @@
         <f>X3-Y3</f>
         <v>13847.21</v>
       </c>
-      <c r="AA3" s="15">
+      <c r="AA3" s="14">
         <v>42702.74</v>
       </c>
-      <c r="AB3" s="15"/>
+      <c r="AB3" s="14"/>
       <c r="AC3" s="8">
         <f>AA3-AB3</f>
         <v>42702.74</v>
       </c>
-      <c r="AD3" s="15">
+      <c r="AD3" s="14">
         <v>91372.67</v>
       </c>
-      <c r="AE3" s="15"/>
+      <c r="AE3" s="14"/>
       <c r="AF3" s="8">
         <f>AD3-AE3</f>
         <v>91372.67</v>
       </c>
-      <c r="AG3" s="17">
+      <c r="AG3" s="16">
         <v>0.61577700000000002</v>
       </c>
       <c r="AH3">
-        <v>0.61577700000000002</v>
-      </c>
-      <c r="AI3" s="14">
+        <v>0.617282</v>
+      </c>
+      <c r="AI3" s="13">
         <f>AG3-AH3</f>
-        <v>0</v>
+        <v>-1.5049999999999786E-3</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -1644,15 +1657,15 @@
         <f>AD4-AE4</f>
         <v>0</v>
       </c>
-      <c r="AG4" s="13">
+      <c r="AG4" s="12">
         <v>0.63692918484900474</v>
       </c>
       <c r="AH4">
-        <v>0.63919899999999996</v>
-      </c>
-      <c r="AI4" s="14">
+        <v>0.63977099999999998</v>
+      </c>
+      <c r="AI4" s="13">
         <f>AG4-AH4</f>
-        <v>-2.2698151509952247E-3</v>
+        <v>-2.8418151509952416E-3</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -1758,15 +1771,15 @@
         <f t="shared" ref="AF5:AF47" si="7">AD5-AE5</f>
         <v>0</v>
       </c>
-      <c r="AG5" s="13">
+      <c r="AG5" s="12">
         <v>0.64192391753402256</v>
       </c>
       <c r="AH5">
-        <v>0.64308200000000004</v>
-      </c>
-      <c r="AI5" s="14">
-        <f t="shared" ref="AI5:AI54" si="8">AG5-AH5</f>
-        <v>-1.1580824659774835E-3</v>
+        <v>0.64397099999999996</v>
+      </c>
+      <c r="AI5" s="13">
+        <f t="shared" ref="AI5:AI55" si="8">AG5-AH5</f>
+        <v>-2.0470824659774012E-3</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
@@ -1868,15 +1881,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG6" s="13">
+      <c r="AG6" s="12">
         <v>0.91486436538534088</v>
       </c>
       <c r="AH6">
-        <v>0.91566599999999998</v>
-      </c>
-      <c r="AI6" s="14">
+        <v>0.91712899999999997</v>
+      </c>
+      <c r="AI6" s="13">
         <f t="shared" si="8"/>
-        <v>-8.0163461465909691E-4</v>
+        <v>-2.264634614659089E-3</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -1978,15 +1991,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG7" s="13">
+      <c r="AG7" s="12">
         <v>0.9167086694055423</v>
       </c>
       <c r="AH7">
-        <v>0.91733299999999995</v>
-      </c>
-      <c r="AI7" s="14">
+        <v>0.91855399999999998</v>
+      </c>
+      <c r="AI7" s="13">
         <f t="shared" si="8"/>
-        <v>-6.2433059445765604E-4</v>
+        <v>-1.8453305944576837E-3</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
@@ -2088,15 +2101,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG8" s="13">
+      <c r="AG8" s="12">
         <v>0.92429892689988069</v>
       </c>
       <c r="AH8">
-        <v>0.92431399999999997</v>
-      </c>
-      <c r="AI8" s="14">
+        <v>0.92654499999999995</v>
+      </c>
+      <c r="AI8" s="13">
         <f t="shared" si="8"/>
-        <v>-1.5073100119278315E-5</v>
+        <v>-2.2460731001192613E-3</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
@@ -2198,15 +2211,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG9" s="13">
+      <c r="AG9" s="12">
         <v>0.92263872730338636</v>
       </c>
       <c r="AH9">
-        <v>0.92395300000000002</v>
-      </c>
-      <c r="AI9" s="14">
+        <v>0.92637100000000006</v>
+      </c>
+      <c r="AI9" s="13">
         <f t="shared" si="8"/>
-        <v>-1.3142726966136609E-3</v>
+        <v>-3.7322726966136921E-3</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
@@ -2308,15 +2321,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG10" s="13">
+      <c r="AG10" s="12">
         <v>0.91811639759826613</v>
       </c>
       <c r="AH10">
-        <v>0.91961700000000002</v>
-      </c>
-      <c r="AI10" s="14">
+        <v>0.92491199999999996</v>
+      </c>
+      <c r="AI10" s="13">
         <f t="shared" si="8"/>
-        <v>-1.5006024017338859E-3</v>
+        <v>-6.7956024017338246E-3</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
@@ -2418,15 +2431,15 @@
         <f t="shared" si="7"/>
         <v>-3</v>
       </c>
-      <c r="AG11" s="13">
+      <c r="AG11" s="12">
         <v>0.91780516938713574</v>
       </c>
       <c r="AH11">
-        <v>0.91934800000000005</v>
-      </c>
-      <c r="AI11" s="14">
+        <v>0.92433399999999999</v>
+      </c>
+      <c r="AI11" s="13">
         <f t="shared" si="8"/>
-        <v>-1.5428306128643099E-3</v>
+        <v>-6.5288306128642448E-3</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
@@ -2528,15 +2541,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG12" s="13">
+      <c r="AG12" s="12">
         <v>0.91925132915549479</v>
       </c>
       <c r="AH12">
-        <v>0.91936099999999998</v>
-      </c>
-      <c r="AI12" s="14">
+        <v>0.92336099999999999</v>
+      </c>
+      <c r="AI12" s="13">
         <f t="shared" si="8"/>
-        <v>-1.0967084450519415E-4</v>
+        <v>-4.1096708445051977E-3</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
@@ -2638,15 +2651,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG13" s="13">
+      <c r="AG13" s="12">
         <v>0.88967514351634858</v>
       </c>
       <c r="AH13">
-        <v>0.89018200000000003</v>
-      </c>
-      <c r="AI13" s="14">
+        <v>0.89055700000000004</v>
+      </c>
+      <c r="AI13" s="13">
         <f t="shared" si="8"/>
-        <v>-5.0685648365145219E-4</v>
+        <v>-8.8185648365146641E-4</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -2748,15 +2761,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG14" s="13">
+      <c r="AG14" s="12">
         <v>0.92035093322632699</v>
       </c>
       <c r="AH14">
-        <v>0.92149899999999996</v>
-      </c>
-      <c r="AI14" s="14">
+        <v>0.92383499999999996</v>
+      </c>
+      <c r="AI14" s="13">
         <f t="shared" si="8"/>
-        <v>-1.1480667736729622E-3</v>
+        <v>-3.4840667736729669E-3</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -2858,15 +2871,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG15" s="13">
+      <c r="AG15" s="12">
         <v>0.92238581240683915</v>
       </c>
       <c r="AH15">
-        <v>0.92390399999999995</v>
-      </c>
-      <c r="AI15" s="14">
+        <v>0.92707600000000001</v>
+      </c>
+      <c r="AI15" s="13">
         <f t="shared" si="8"/>
-        <v>-1.5181875931608024E-3</v>
+        <v>-4.6901875931608661E-3</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -2968,15 +2981,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG16" s="13">
+      <c r="AG16" s="12">
         <v>0.91517757628246044</v>
       </c>
       <c r="AH16">
-        <v>0.91652</v>
-      </c>
-      <c r="AI16" s="14">
+        <v>0.91900199999999999</v>
+      </c>
+      <c r="AI16" s="13">
         <f t="shared" si="8"/>
-        <v>-1.3424237175395648E-3</v>
+        <v>-3.824423717539549E-3</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
@@ -3078,15 +3091,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG17" s="13">
+      <c r="AG17" s="12">
         <v>0.91693398324447473</v>
       </c>
       <c r="AH17">
-        <v>0.918161</v>
-      </c>
-      <c r="AI17" s="14">
+        <v>0.92081900000000005</v>
+      </c>
+      <c r="AI17" s="13">
         <f t="shared" si="8"/>
-        <v>-1.2270167555252787E-3</v>
+        <v>-3.8850167555253279E-3</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
@@ -3188,15 +3201,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG18" s="13">
+      <c r="AG18" s="12">
         <v>0.91499736714872371</v>
       </c>
       <c r="AH18">
-        <v>0.91571599999999997</v>
-      </c>
-      <c r="AI18" s="14">
+        <v>0.91797700000000004</v>
+      </c>
+      <c r="AI18" s="13">
         <f t="shared" si="8"/>
-        <v>-7.1863285127626852E-4</v>
+        <v>-2.979632851276337E-3</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
@@ -3298,15 +3311,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG19" s="13">
+      <c r="AG19" s="12">
         <v>0.91584282945008366</v>
       </c>
       <c r="AH19">
-        <v>0.91695899999999997</v>
-      </c>
-      <c r="AI19" s="14">
+        <v>0.920207</v>
+      </c>
+      <c r="AI19" s="13">
         <f t="shared" si="8"/>
-        <v>-1.1161705499163066E-3</v>
+        <v>-4.3641705499163352E-3</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
@@ -3408,15 +3421,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG20" s="13">
+      <c r="AG20" s="12">
         <v>0.90950537153338806</v>
       </c>
       <c r="AH20">
-        <v>0.91079399999999999</v>
-      </c>
-      <c r="AI20" s="14">
+        <v>0.91390700000000002</v>
+      </c>
+      <c r="AI20" s="13">
         <f t="shared" si="8"/>
-        <v>-1.2886284666119296E-3</v>
+        <v>-4.4016284666119621E-3</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
@@ -3518,15 +3531,15 @@
         <f t="shared" si="7"/>
         <v>-2.9900000000052387</v>
       </c>
-      <c r="AG21" s="13">
+      <c r="AG21" s="12">
         <v>0.9181107354306689</v>
       </c>
       <c r="AH21">
-        <v>0.91930999999999996</v>
-      </c>
-      <c r="AI21" s="14">
+        <v>0.92098100000000005</v>
+      </c>
+      <c r="AI21" s="13">
         <f t="shared" si="8"/>
-        <v>-1.19926456933106E-3</v>
+        <v>-2.870264569331149E-3</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
@@ -3628,15 +3641,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG22" s="13">
+      <c r="AG22" s="12">
         <v>0.90923498497209809</v>
       </c>
       <c r="AH22">
-        <v>0.91016799999999998</v>
-      </c>
-      <c r="AI22" s="14">
+        <v>0.91601299999999997</v>
+      </c>
+      <c r="AI22" s="13">
         <f t="shared" si="8"/>
-        <v>-9.3301502790188451E-4</v>
+        <v>-6.7780150279018736E-3</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
@@ -3738,15 +3751,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG23" s="13">
+      <c r="AG23" s="12">
         <v>0.91170649315209085</v>
       </c>
       <c r="AH23">
-        <v>0.91240900000000003</v>
-      </c>
-      <c r="AI23" s="14">
+        <v>0.91816799999999998</v>
+      </c>
+      <c r="AI23" s="13">
         <f t="shared" si="8"/>
-        <v>-7.0250684790917894E-4</v>
+        <v>-6.4615068479091375E-3</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
@@ -3848,15 +3861,15 @@
         <f t="shared" si="7"/>
         <v>-3</v>
       </c>
-      <c r="AG24" s="13">
+      <c r="AG24" s="12">
         <v>0.9235547669353702</v>
       </c>
       <c r="AH24">
-        <v>0.92468399999999995</v>
-      </c>
-      <c r="AI24" s="14">
+        <v>0.92818900000000004</v>
+      </c>
+      <c r="AI24" s="13">
         <f t="shared" si="8"/>
-        <v>-1.1292330646297533E-3</v>
+        <v>-4.6342330646298446E-3</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
@@ -3958,15 +3971,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG25" s="13">
+      <c r="AG25" s="12">
         <v>0.92471339100958849</v>
       </c>
       <c r="AH25">
-        <v>0.92580200000000001</v>
-      </c>
-      <c r="AI25" s="14">
+        <v>0.92814700000000006</v>
+      </c>
+      <c r="AI25" s="13">
         <f t="shared" si="8"/>
-        <v>-1.0886089904115215E-3</v>
+        <v>-3.433608990411563E-3</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
@@ -4068,15 +4081,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG26" s="13">
+      <c r="AG26" s="12">
         <v>0.91440189369811065</v>
       </c>
       <c r="AH26">
-        <v>0.91599799999999998</v>
-      </c>
-      <c r="AI26" s="14">
+        <v>0.91749199999999997</v>
+      </c>
+      <c r="AI26" s="13">
         <f t="shared" si="8"/>
-        <v>-1.5961063018893329E-3</v>
+        <v>-3.0901063018893282E-3</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
@@ -4178,15 +4191,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG27" s="13">
+      <c r="AG27" s="12">
         <v>0.91119750217455808</v>
       </c>
       <c r="AH27">
-        <v>0.912215</v>
-      </c>
-      <c r="AI27" s="14">
+        <v>0.914493</v>
+      </c>
+      <c r="AI27" s="13">
         <f t="shared" si="8"/>
-        <v>-1.0174978254419154E-3</v>
+        <v>-3.2954978254419176E-3</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
@@ -4288,15 +4301,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG28" s="13">
+      <c r="AG28" s="12">
         <v>0.91740136721349375</v>
       </c>
       <c r="AH28">
-        <v>0.91833699999999996</v>
-      </c>
-      <c r="AI28" s="14">
+        <v>0.92059599999999997</v>
+      </c>
+      <c r="AI28" s="13">
         <f t="shared" si="8"/>
-        <v>-9.3563278650621307E-4</v>
+        <v>-3.1946327865062241E-3</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
@@ -4398,15 +4411,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG29" s="13">
+      <c r="AG29" s="12">
         <v>0.90184813249726981</v>
       </c>
       <c r="AH29">
-        <v>0.90239000000000003</v>
-      </c>
-      <c r="AI29" s="14">
+        <v>0.90315299999999998</v>
+      </c>
+      <c r="AI29" s="13">
         <f t="shared" si="8"/>
-        <v>-5.4186750273022E-4</v>
+        <v>-1.3048675027301782E-3</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
@@ -4508,15 +4521,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG30" s="13">
+      <c r="AG30" s="12">
         <v>0.91584433411827804</v>
       </c>
       <c r="AH30">
-        <v>0.91680700000000004</v>
-      </c>
-      <c r="AI30" s="14">
+        <v>0.91937199999999997</v>
+      </c>
+      <c r="AI30" s="13">
         <f t="shared" si="8"/>
-        <v>-9.626658817220024E-4</v>
+        <v>-3.5276658817219309E-3</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
@@ -4618,15 +4631,15 @@
         <f t="shared" si="7"/>
         <v>-2.9899999999906868</v>
       </c>
-      <c r="AG31" s="13">
+      <c r="AG31" s="12">
         <v>0.91582419377934587</v>
       </c>
       <c r="AH31">
-        <v>0.91665300000000005</v>
-      </c>
-      <c r="AI31" s="14">
+        <v>0.91816200000000003</v>
+      </c>
+      <c r="AI31" s="13">
         <f t="shared" si="8"/>
-        <v>-8.2880622065417686E-4</v>
+        <v>-2.3378062206541594E-3</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
@@ -4728,15 +4741,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG32" s="13">
+      <c r="AG32" s="12">
         <v>0.91000303824766082</v>
       </c>
       <c r="AH32">
-        <v>0.91107800000000005</v>
-      </c>
-      <c r="AI32" s="14">
+        <v>0.91394399999999998</v>
+      </c>
+      <c r="AI32" s="13">
         <f t="shared" si="8"/>
-        <v>-1.0749617523392319E-3</v>
+        <v>-3.940961752339156E-3</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
@@ -4838,15 +4851,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG33" s="13">
+      <c r="AG33" s="12">
         <v>0.91609225355188495</v>
       </c>
       <c r="AH33">
-        <v>0.916883</v>
-      </c>
-      <c r="AI33" s="14">
+        <v>0.91958300000000004</v>
+      </c>
+      <c r="AI33" s="13">
         <f t="shared" si="8"/>
-        <v>-7.907464481150539E-4</v>
+        <v>-3.4907464481150896E-3</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
@@ -4948,15 +4961,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG34" s="13">
+      <c r="AG34" s="12">
         <v>0.93137405678912</v>
       </c>
       <c r="AH34">
-        <v>0.932176</v>
-      </c>
-      <c r="AI34" s="14">
+        <v>0.93376300000000001</v>
+      </c>
+      <c r="AI34" s="13">
         <f t="shared" si="8"/>
-        <v>-8.0194321088000731E-4</v>
+        <v>-2.3889432108800124E-3</v>
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
@@ -5058,15 +5071,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG35" s="13">
+      <c r="AG35" s="12">
         <v>0.93408475016627335</v>
       </c>
       <c r="AH35">
-        <v>0.93575699999999995</v>
-      </c>
-      <c r="AI35" s="14">
+        <v>0.93809600000000004</v>
+      </c>
+      <c r="AI35" s="13">
         <f t="shared" si="8"/>
-        <v>-1.6722498337266023E-3</v>
+        <v>-4.0112498337266933E-3</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
@@ -5168,15 +5181,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG36" s="13">
+      <c r="AG36" s="12">
         <v>0.9313425672130492</v>
       </c>
       <c r="AH36">
-        <v>0.93194100000000002</v>
-      </c>
-      <c r="AI36" s="14">
+        <v>0.933361</v>
+      </c>
+      <c r="AI36" s="13">
         <f t="shared" si="8"/>
-        <v>-5.9843278695081992E-4</v>
+        <v>-2.0184327869507968E-3</v>
       </c>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
@@ -5278,15 +5291,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG37" s="13">
+      <c r="AG37" s="12">
         <v>0.92871686126712338</v>
       </c>
       <c r="AH37">
-        <v>0.92961099999999997</v>
-      </c>
-      <c r="AI37" s="14">
+        <v>0.93140699999999998</v>
+      </c>
+      <c r="AI37" s="13">
         <f t="shared" si="8"/>
-        <v>-8.9413873287658152E-4</v>
+        <v>-2.6901387328766013E-3</v>
       </c>
     </row>
     <row r="38" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
@@ -5368,15 +5381,15 @@
         <f t="shared" si="7"/>
         <v>95043.94</v>
       </c>
-      <c r="AG38" s="13">
+      <c r="AG38" s="12">
         <v>0.92668440912607419</v>
       </c>
       <c r="AH38">
-        <v>0.93071999999999999</v>
-      </c>
-      <c r="AI38" s="14">
+        <v>0.93493800000000005</v>
+      </c>
+      <c r="AI38" s="13">
         <f t="shared" si="8"/>
-        <v>-4.0355908739257984E-3</v>
+        <v>-8.2535908739258534E-3</v>
       </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.25">
@@ -5478,15 +5491,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG39" s="13">
+      <c r="AG39" s="12">
         <v>0.93102933417843436</v>
       </c>
       <c r="AH39">
-        <v>0.93223800000000001</v>
-      </c>
-      <c r="AI39" s="14">
+        <v>0.93530400000000002</v>
+      </c>
+      <c r="AI39" s="13">
         <f t="shared" si="8"/>
-        <v>-1.2086658215656465E-3</v>
+        <v>-4.2746658215656597E-3</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
@@ -5588,15 +5601,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG40" s="13">
+      <c r="AG40" s="12">
         <v>0.92971749366237477</v>
       </c>
       <c r="AH40">
-        <v>0.93131399999999998</v>
-      </c>
-      <c r="AI40" s="14">
+        <v>0.93538699999999997</v>
+      </c>
+      <c r="AI40" s="13">
         <f t="shared" si="8"/>
-        <v>-1.5965063376252031E-3</v>
+        <v>-5.6695063376251964E-3</v>
       </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.25">
@@ -5698,15 +5711,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG41" s="13">
+      <c r="AG41" s="12">
         <v>0.88089077504082924</v>
       </c>
       <c r="AH41">
-        <v>0.88151199999999996</v>
-      </c>
-      <c r="AI41" s="14">
+        <v>0.88384600000000002</v>
+      </c>
+      <c r="AI41" s="13">
         <f t="shared" si="8"/>
-        <v>-6.2122495917071863E-4</v>
+        <v>-2.9552249591707769E-3</v>
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.25">
@@ -5808,15 +5821,15 @@
         <f t="shared" si="7"/>
         <v>-2.9899999999906868</v>
       </c>
-      <c r="AG42" s="13">
+      <c r="AG42" s="12">
         <v>0.9331024980123428</v>
       </c>
       <c r="AH42">
-        <v>0.93426500000000001</v>
-      </c>
-      <c r="AI42" s="14">
+        <v>0.93689500000000003</v>
+      </c>
+      <c r="AI42" s="13">
         <f t="shared" si="8"/>
-        <v>-1.1625019876572162E-3</v>
+        <v>-3.7925019876572374E-3</v>
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.25">
@@ -5918,15 +5931,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG43" s="13">
+      <c r="AG43" s="12">
         <v>0.92968255944153733</v>
       </c>
       <c r="AH43">
-        <v>0.93054800000000004</v>
-      </c>
-      <c r="AI43" s="14">
+        <v>0.932477</v>
+      </c>
+      <c r="AI43" s="13">
         <f t="shared" si="8"/>
-        <v>-8.6544055846271561E-4</v>
+        <v>-2.7944405584626741E-3</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.25">
@@ -6028,15 +6041,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AG44" s="13">
+      <c r="AG44" s="12">
         <v>0.92867786805463182</v>
       </c>
       <c r="AH44">
-        <v>0.92902600000000002</v>
-      </c>
-      <c r="AI44" s="14">
+        <v>0.93054000000000003</v>
+      </c>
+      <c r="AI44" s="13">
         <f t="shared" si="8"/>
-        <v>-3.4813194536820191E-4</v>
+        <v>-1.8621319453682172E-3</v>
       </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.25">
@@ -6138,15 +6151,15 @@
         <f t="shared" si="7"/>
         <v>-3</v>
       </c>
-      <c r="AG45" s="13">
+      <c r="AG45" s="12">
         <v>0.92883400573334829</v>
       </c>
       <c r="AH45">
-        <v>0.93041700000000005</v>
-      </c>
-      <c r="AI45" s="14">
+        <v>0.93174599999999996</v>
+      </c>
+      <c r="AI45" s="13">
         <f t="shared" si="8"/>
-        <v>-1.5829942666517605E-3</v>
+        <v>-2.911994266651674E-3</v>
       </c>
     </row>
     <row r="46" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
@@ -6214,7 +6227,7 @@
       <c r="AH46">
         <v>0</v>
       </c>
-      <c r="AI46" s="12">
+      <c r="AI46" s="13">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -6324,7 +6337,7 @@
       <c r="AH47">
         <v>0</v>
       </c>
-      <c r="AI47" s="12">
+      <c r="AI47" s="13">
         <f t="shared" si="8"/>
         <v>0.90073495789560953</v>
       </c>
@@ -6333,63 +6346,213 @@
       <c r="AH48">
         <v>0</v>
       </c>
-      <c r="AI48" s="8">
+      <c r="AI48" s="13">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="AH49">
         <v>0</v>
       </c>
-      <c r="AI49" s="8">
+      <c r="AI49" s="13">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="AH50">
         <v>0</v>
       </c>
-      <c r="AI50" s="8">
+      <c r="AI50" s="13">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="AH51">
         <v>0</v>
       </c>
-      <c r="AI51" s="8">
+      <c r="AI51" s="13">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="AH52">
         <v>0</v>
       </c>
-      <c r="AI52" s="8">
+      <c r="AI52" s="13">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="AH53">
         <v>0</v>
       </c>
-      <c r="AI53" s="8">
+      <c r="AI53" s="13">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="34:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="AH54">
-        <v>0.81740599999999997</v>
-      </c>
-      <c r="AI54" s="8">
+        <v>0.83083099999999999</v>
+      </c>
+      <c r="AI54" s="13">
         <f t="shared" si="8"/>
-        <v>-0.81740599999999997</v>
+        <v>-0.83083099999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="3">
+        <v>50</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="3"/>
+      <c r="V55" s="3"/>
+      <c r="W55" s="3"/>
+      <c r="X55" s="3"/>
+      <c r="Y55" s="3"/>
+      <c r="Z55" s="3"/>
+      <c r="AA55" s="3"/>
+      <c r="AB55" s="3"/>
+      <c r="AC55" s="3"/>
+      <c r="AD55" s="3"/>
+      <c r="AE55" s="3"/>
+      <c r="AF55" s="3"/>
+      <c r="AG55" s="3">
+        <v>4.7050599999999996</v>
+      </c>
+      <c r="AH55" s="3">
+        <v>4.7050289999999997</v>
+      </c>
+      <c r="AI55" s="13">
+        <f t="shared" si="8"/>
+        <v>3.0999999999892225E-5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="3">
+        <v>49.8</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="3"/>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="3"/>
+      <c r="AA56" s="3"/>
+      <c r="AB56" s="3"/>
+      <c r="AC56" s="3"/>
+      <c r="AD56" s="3"/>
+      <c r="AE56" s="3"/>
+      <c r="AF56" s="3"/>
+      <c r="AG56" s="3">
+        <v>4.3026799999999996</v>
+      </c>
+      <c r="AH56" s="3">
+        <v>4.3045099999999996</v>
+      </c>
+      <c r="AI56" s="13">
+        <f>AG56-AH56</f>
+        <v>-1.8299999999999983E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="3">
+        <v>65</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="3"/>
+      <c r="U57" s="3"/>
+      <c r="V57" s="3"/>
+      <c r="W57" s="3"/>
+      <c r="X57" s="3"/>
+      <c r="Y57" s="3"/>
+      <c r="Z57" s="3"/>
+      <c r="AA57" s="3"/>
+      <c r="AB57" s="3"/>
+      <c r="AC57" s="3"/>
+      <c r="AD57" s="3"/>
+      <c r="AE57" s="3"/>
+      <c r="AF57" s="3"/>
+      <c r="AG57" s="3">
+        <v>3.04</v>
+      </c>
+      <c r="AH57" s="3">
+        <v>3.0362200000000001</v>
+      </c>
+      <c r="AI57" s="13">
+        <f>AG57-AH57</f>
+        <v>3.7799999999998946E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating FHR code at 15 sec into draw
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/UEF Check Sheet.xlsx
+++ b/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/UEF Check Sheet.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52791B2C-D3A5-4A2D-8413-6B75B28FE9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADD062E-0B40-44BC-8D54-F590DA113673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4525C065-1982-4190-BA1C-76B51CDE7E26}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4525C065-1982-4190-BA1C-76B51CDE7E26}"/>
   </bookViews>
   <sheets>
     <sheet name="UEF Check" sheetId="1" r:id="rId1"/>
     <sheet name="FHR Check" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="216">
   <si>
     <t>Type</t>
   </si>
@@ -427,66 +428,36 @@
     <t>Partial Bonus Draw?</t>
   </si>
   <si>
-    <t>Macro Rating (Gallons)</t>
-  </si>
-  <si>
     <t>Difference</t>
   </si>
   <si>
     <t>20WS1064</t>
   </si>
   <si>
-    <t>TR_AWP20WS10184_Lab_ID_20WS1064_Md_GG50T12BXR01 08_59FHR</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>20WS1095-Run1</t>
   </si>
   <si>
-    <t>TR_AWP21WS10211_Lab_ID_21WS1095_Model_GG50S08_Date_06_10_2021_Time_09_45FHR_File0_Data</t>
-  </si>
-  <si>
     <t>21WS1095-Run 2</t>
   </si>
   <si>
-    <t>TR_AWP21WS10211_Lab_ID_21WS1095_Model_GG50S08_Date_06_10_2021_Time_14_33FHR_File1_Data</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TR_AWP24WS10416_Lab_ID_24WS1597_Model_PH50S10BNY_Date_09_27_2024_Time_21_581st Hour Rating_File1_Data</t>
-  </si>
-  <si>
-    <t>TR_AWP24WS10416_Lab_ID_24WS1595_Model_PH50S10BNY_Date_09_24_2024_Time_14_051st Hour Rating_File0_Data</t>
-  </si>
-  <si>
     <t>GE50S08BAM01</t>
   </si>
   <si>
-    <t>TR_sheldon_energy_50g_top_t_p_Lab_ID_GZ600462X_Model_GE50S08BAM01 _Date_10_08_2024_Time_16_30FHR_</t>
-  </si>
-  <si>
     <t>Data Set 4</t>
   </si>
   <si>
-    <t>TR_AWP24WS10416_Lab_ID_24WS1596_Model_PH50S10BNY_Date_10_22_2024_Time_18_311st Hour Rating_</t>
-  </si>
-  <si>
     <t>Data Set 5</t>
   </si>
   <si>
-    <t>TR_AWP24WS10429_Lab_ID_24WS1687_Model_PJ50S10FPY_Date_11_21_2024_Time_13_031st Hour Rating_File0_Data</t>
-  </si>
-  <si>
     <t>FHD Mistake</t>
   </si>
   <si>
-    <t>TR_AWP25WS10441_Lab_ID_25WS1753_Model_GE50S08BAY_Date_02_19_2025_Time_12_191st Hour Rating_File0_Data</t>
-  </si>
-  <si>
     <t>FHD Mistake 2</t>
   </si>
   <si>
@@ -496,57 +467,30 @@
     <t>FHD Mistake 3</t>
   </si>
   <si>
-    <t>TR_AWP25WS10450_Lab_ID_25WS1804_Model_PK65S10FNY_Date_03_28_2025_Time_08_401st Hour Rating_File0_Data</t>
-  </si>
-  <si>
     <t>25WS1794</t>
   </si>
   <si>
-    <t>TR_AWP25WS10443_Lab_ID_25WS1794_Model_PJ65S10FPY_Date_03_12_2025_Time_14_071st Hour Rating_</t>
-  </si>
-  <si>
     <t>25WS1795</t>
   </si>
   <si>
-    <t>TR_AWP25WS10443_Lab_ID_25WS1795_Model_PF65S10FPY_Date_03_04_2025_Time_14_301st Hour Rating_</t>
-  </si>
-  <si>
     <t>25WS1799</t>
   </si>
   <si>
-    <t>TR_AWP25WS10444_Lab_ID_25WS1799_Model_PH65S10BPY_Date_03_04_2025_Time_14_161st Hour Rating_File2_Data</t>
-  </si>
-  <si>
     <t>25WS1802</t>
   </si>
   <si>
-    <t>TR_AWP25WS10450_Lab_ID_25WS1802_Model_PK65S10FNY_Date_04_03_2025_Time_15_031st Hour Rating_File2_Data</t>
-  </si>
-  <si>
     <t>25WS1810</t>
   </si>
   <si>
-    <t>TR_AWP25WS10447_Lab_ID_25WS1810_Model_PF80S10FPY_Date_04_14_2025_Time_07_061st Hour Rating_</t>
-  </si>
-  <si>
     <t>25WS1814</t>
   </si>
   <si>
-    <t>TR_AWP25WS10448_Lab_ID_25WS1814_Model_PH80S10BPY_Date_04_11_2025_Time_21_551st Hour Rating_File1_Data</t>
-  </si>
-  <si>
     <t>25WS1807</t>
   </si>
   <si>
-    <t>TR_AWP25WS10452_Lab_ID_25WS1807_Model_PK80S10FNY_Date_04_05_2025_Time_21_291st Hour Rating_File2_Data</t>
-  </si>
-  <si>
     <t>25WS1806</t>
   </si>
   <si>
-    <t>TR_AWP25WS10446_Lab_ID_25WS1806_Model_PH80S10FBNY_Date_03_25_2025_Time_17_331st Hour Rating_File1_Data</t>
-  </si>
-  <si>
     <t>22WS1081</t>
   </si>
   <si>
@@ -701,6 +645,78 @@
   </si>
   <si>
     <t>65 Gallon HP</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>Version 42</t>
+  </si>
+  <si>
+    <t>Macro Rating (Gallons)-V42</t>
+  </si>
+  <si>
+    <t>New Macro</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\1. Gas\2022 Camden Gas Water Heater\GG50T - NG\20WS1064\TR_AWP20WS10184_Lab_ID_20WS1064_Md_GG50T12BXR01 08_59FHR.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\1. Gas\2022 Camden Gas Water Heater\GG50S - NG\21WS1095\21WS1095-Run1\TR_AWP21WS10211_Lab_ID_21WS1095_Model_GG50S08_Date_06_10_2021_Time_09_45FHR_File0_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\1. Gas\2022 Camden Gas Water Heater\GG50S - NG\21WS1095\21WS1095-Run2\TR_AWP21WS10211_Lab_ID_21WS1095_Model_GG50S08_Date_06_10_2021_Time_14_33FHR_File1_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\50 gallon 240V non-EMV\24WS1597\TR_AWP24WS10416_Lab_ID_24WS1597_Model_PH50S10BNY_Date_09_27_2024_Time_21_581st Hour Rating_File1_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\65 Gallon\25WS1804\TR_AWP25WS10450_Lab_ID_25WS1804_Model_PK65S10FNY_Date_03_28_2025_Time_08_401st Hour Rating_File0_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\2. Storage Electric\50 Short\25WS1753\TR_AWP25WS10441_Lab_ID_25WS1753_Model_GE50S08BAY_Date_02_19_2025_Time_12_191st Hour Rating_File0_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\50 Gallon 120V EMV Canada\24WS1687\TR_AWP24WS10429_Lab_ID_24WS1687_Model_PJ50S10FPY_Date_11_21_2024_Time_13_031st Hour Rating_File0_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\50 gallon 240V non-EMV\24WS1596\TR_AWP24WS10416_Lab_ID_24WS1596_Model_PH50S10BNY_Date_10_22_2024_Time_18_311st Hour Rating_File3_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\2. Storage Electric\50 Short\GE50S08BAM01\TR_sheldon_energy_50g_top_t_p_Lab_ID_GZ600462X_Model_GE50S08BAM01 _Date_10_08_2024_Time_16_30FHR_File0_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\50 gallon 240V non-EMV\24WS1595\TR_AWP24WS10416_Lab_ID_24WS1595_Model_PH50S10BNY_Date_09_24_2024_Time_14_051st Hour Rating_File0_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\65 Gallon\25WS1794\TR_AWP25WS10443_Lab_ID_25WS1794_Model_PJ65S10FPY_Date_03_12_2025_Time_14_071st Hour Rating_File0_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\65 Gallon\25WS1795\TR_AWP25WS10443_Lab_ID_25WS1795_Model_PF65S10FPY_Date_03_04_2025_Time_14_301st Hour Rating_File2_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\65 Gallon\25WS1799\TR_AWP25WS10444_Lab_ID_25WS1799_Model_PH65S10BPY_Date_03_04_2025_Time_14_161st Hour Rating_File2_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\65 Gallon\25WS1802\TR_AWP25WS10450_Lab_ID_25WS1802_Model_PK65S10FNY_Date_04_03_2025_Time_15_031st Hour Rating_File2_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\80 Gallon\25WS1810\TR_AWP25WS10447_Lab_ID_25WS1810_Model_PF80S10FPY_Date_04_14_2025_Time_07_061st Hour Rating_File0_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\80 Gallon\25WS1814\TR_AWP25WS10448_Lab_ID_25WS1814_Model_PH80S10BPY_Date_04_11_2025_Time_21_551st Hour Rating_File1_Data.csv</t>
+  </si>
+  <si>
+    <t>C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\80 Gallon\25WS1807\TR_AWP25WS10452_Lab_ID_25WS1807_Model_PK80S10FNY_Date_04_05_2025_Time_21_291st Hour Rating_File2_Data.csv</t>
+  </si>
+  <si>
+    <t>vC:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\4. Heat Pump\80 Gallon\25WS1806\TR_AWP25WS10446_Lab_ID_25WS1806_Model_PH80S10FBNY_Date_03_25_2025_Time_17_331st Hour Rating_File1_Data.csv</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>New Macro Correct</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1099,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1239,6 +1255,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1284,7 +1311,7 @@
     <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1330,6 +1357,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1685,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E368A452-0E99-44F6-9903-45AB1358FD53}">
-  <dimension ref="A2:AI116"/>
+  <dimension ref="A2:AJ116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AI13" sqref="AI13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AM10" sqref="AM10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,13 +1761,14 @@
     <col min="31" max="31" width="28.7109375" hidden="1" customWidth="1"/>
     <col min="32" max="32" width="15.140625" hidden="1" customWidth="1"/>
     <col min="33" max="33" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.42578125" customWidth="1"/>
+    <col min="35" max="35" width="12" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="29" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1833,18 +1869,21 @@
         <v>9</v>
       </c>
       <c r="AH2" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="AI2" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="AI2" s="21" t="s">
+      <c r="AJ2" s="21" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C3" s="4">
         <v>30</v>
@@ -1881,20 +1920,23 @@
       <c r="AG3" s="4">
         <v>0.59599999999999997</v>
       </c>
-      <c r="AH3" s="4">
-        <v>0.59571799999999997</v>
-      </c>
-      <c r="AI3" s="14">
-        <f t="shared" ref="AI3:AI35" si="0">AG3-AH3</f>
-        <v>2.8200000000000447E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH3" s="11">
+        <v>0.59609999999999996</v>
+      </c>
+      <c r="AI3">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="AJ3" s="14">
+        <f>AH3-AI3</f>
+        <v>9.9999999999988987E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C4" s="4">
         <v>30</v>
@@ -1931,20 +1973,23 @@
       <c r="AG4" s="4">
         <v>0.59599999999999997</v>
       </c>
-      <c r="AH4" s="4">
-        <v>0.59663999999999995</v>
-      </c>
-      <c r="AI4" s="14">
-        <f t="shared" si="0"/>
-        <v>-6.3999999999997392E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH4" s="11">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="AI4">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="AJ4" s="14">
+        <f t="shared" ref="AJ4:AJ67" si="0">AH4-AI4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C5" s="4">
         <v>30</v>
@@ -1981,20 +2026,23 @@
       <c r="AG5" s="4">
         <v>0.59499999999999997</v>
       </c>
-      <c r="AH5" s="4">
-        <v>0.59517100000000001</v>
-      </c>
-      <c r="AI5" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.7100000000003224E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH5" s="11">
+        <v>0.59540000000000004</v>
+      </c>
+      <c r="AI5">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="AJ5" s="14">
+        <f t="shared" si="0"/>
+        <v>4.0000000000006697E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C6" s="4">
         <v>30</v>
@@ -2031,20 +2079,23 @@
       <c r="AG6" s="4">
         <v>0.59799999999999998</v>
       </c>
-      <c r="AH6" s="4">
-        <v>0.59843199999999996</v>
-      </c>
-      <c r="AI6" s="14">
-        <f t="shared" si="0"/>
-        <v>-4.3199999999998795E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH6" s="11">
+        <v>0.5988</v>
+      </c>
+      <c r="AI6">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="AJ6" s="14">
+        <f t="shared" si="0"/>
+        <v>8.0000000000002292E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C7" s="4">
         <v>40</v>
@@ -2081,20 +2132,23 @@
       <c r="AG7" s="4">
         <v>0.63600000000000001</v>
       </c>
-      <c r="AH7" s="4">
-        <v>0.63904300000000003</v>
-      </c>
-      <c r="AI7" s="14">
-        <f t="shared" si="0"/>
-        <v>-3.0430000000000179E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH7" s="11">
+        <v>0.63780000000000003</v>
+      </c>
+      <c r="AI7">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="AJ7" s="14">
+        <f t="shared" si="0"/>
+        <v>-1.1999999999999789E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C8" s="4">
         <v>40</v>
@@ -2131,20 +2185,23 @@
       <c r="AG8" s="4">
         <v>0.63400000000000001</v>
       </c>
-      <c r="AH8" s="4">
-        <v>0.63503100000000001</v>
-      </c>
-      <c r="AI8" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.0310000000000041E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH8" s="11">
+        <v>0.63519999999999999</v>
+      </c>
+      <c r="AI8">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="AJ8" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9999999999997797E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C9" s="4">
         <v>40</v>
@@ -2181,20 +2238,23 @@
       <c r="AG9" s="4">
         <v>0.64900000000000002</v>
       </c>
-      <c r="AH9" s="4">
-        <v>0.64888400000000002</v>
-      </c>
-      <c r="AI9" s="14">
-        <f t="shared" si="0"/>
-        <v>1.1600000000000499E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH9" s="11">
+        <v>0.64910000000000001</v>
+      </c>
+      <c r="AI9">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="AJ9" s="14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999988987E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C10" s="4">
         <v>39.9</v>
@@ -2231,20 +2291,23 @@
       <c r="AG10" s="4">
         <v>0.64400000000000002</v>
       </c>
-      <c r="AH10" s="4">
-        <v>0.64411799999999997</v>
-      </c>
-      <c r="AI10" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.1799999999995148E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH10" s="11">
+        <v>0.64470000000000005</v>
+      </c>
+      <c r="AI10">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="AJ10" s="14">
+        <f t="shared" si="0"/>
+        <v>7.0000000000003393E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C11" s="4">
         <v>50.2</v>
@@ -2281,20 +2344,23 @@
       <c r="AG11" s="4">
         <v>0.63500000000000001</v>
       </c>
-      <c r="AH11" s="4">
-        <v>0.63413799999999998</v>
-      </c>
-      <c r="AI11" s="14">
-        <f t="shared" si="0"/>
-        <v>8.6200000000002941E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH11" s="11">
+        <v>0.63460000000000005</v>
+      </c>
+      <c r="AI11">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="AJ11" s="14">
+        <f t="shared" si="0"/>
+        <v>6.0000000000004494E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C12" s="4">
         <v>50</v>
@@ -2331,20 +2397,23 @@
       <c r="AG12" s="4">
         <v>0.63400000000000001</v>
       </c>
-      <c r="AH12" s="4">
-        <v>0.633521</v>
-      </c>
-      <c r="AI12" s="14">
-        <f t="shared" si="0"/>
-        <v>4.790000000000072E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH12" s="11">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="AI12">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="AJ12" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C13" s="4">
         <v>47.75</v>
@@ -2381,20 +2450,23 @@
       <c r="AG13" s="4">
         <v>0.65100000000000002</v>
       </c>
-      <c r="AH13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="14">
-        <f t="shared" si="0"/>
-        <v>0.65100000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH13" s="11">
+        <v>0.6472</v>
+      </c>
+      <c r="AI13">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="AJ13" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9999999999997797E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C14" s="4">
         <v>50</v>
@@ -2431,20 +2503,23 @@
       <c r="AG14" s="4">
         <v>0.64200000000000002</v>
       </c>
-      <c r="AH14" s="4">
-        <v>0.641455</v>
-      </c>
-      <c r="AI14" s="14">
-        <f t="shared" si="0"/>
-        <v>5.4500000000001769E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH14" s="11">
+        <v>0.64190000000000003</v>
+      </c>
+      <c r="AI14">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="AJ14" s="14">
+        <f t="shared" si="0"/>
+        <v>9.000000000000119E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C15" s="4">
         <v>50</v>
@@ -2481,20 +2556,23 @@
       <c r="AG15" s="4">
         <v>0.64700000000000002</v>
       </c>
-      <c r="AH15" s="4">
-        <v>0.64722800000000003</v>
-      </c>
-      <c r="AI15" s="14">
-        <f t="shared" si="0"/>
-        <v>-2.2800000000000598E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH15" s="11">
+        <v>0.64759999999999995</v>
+      </c>
+      <c r="AI15">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="AJ15" s="14">
+        <f t="shared" si="0"/>
+        <v>5.9999999999993392E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C16" s="4">
         <v>30</v>
@@ -2531,20 +2609,23 @@
       <c r="AG16" s="4">
         <v>0.71299999999999997</v>
       </c>
-      <c r="AH16" s="4">
-        <v>0.71314699999999998</v>
-      </c>
-      <c r="AI16" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.4700000000000824E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH16" s="11">
+        <v>0.7137</v>
+      </c>
+      <c r="AI16">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="AJ16" s="14">
+        <f t="shared" si="0"/>
+        <v>7.0000000000003393E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C17" s="4">
         <v>30</v>
@@ -2581,20 +2662,23 @@
       <c r="AG17" s="4">
         <v>0.72799999999999998</v>
       </c>
-      <c r="AH17" s="4">
-        <v>0.727939</v>
-      </c>
-      <c r="AI17" s="14">
-        <f t="shared" si="0"/>
-        <v>6.0999999999977739E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH17" s="11">
+        <v>0.72829999999999995</v>
+      </c>
+      <c r="AI17">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="AJ17" s="14">
+        <f t="shared" si="0"/>
+        <v>2.9999999999996696E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C18" s="4">
         <v>39.9</v>
@@ -2631,20 +2715,23 @@
       <c r="AG18" s="4">
         <v>0.64100000000000001</v>
       </c>
-      <c r="AH18" s="4">
-        <v>0.64254199999999995</v>
-      </c>
-      <c r="AI18" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.5419999999999323E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH18" s="11">
+        <v>0.64249999999999996</v>
+      </c>
+      <c r="AI18">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="AJ18" s="14">
+        <f t="shared" si="0"/>
+        <v>-5.0000000000005596E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C19" s="4">
         <v>39.9</v>
@@ -2681,20 +2768,23 @@
       <c r="AG19" s="4">
         <v>0.64500000000000002</v>
       </c>
-      <c r="AH19" s="4">
-        <v>0.64676400000000001</v>
-      </c>
-      <c r="AI19" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.7639999999999878E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH19" s="11">
+        <v>0.64629999999999999</v>
+      </c>
+      <c r="AI19">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="AJ19" s="14">
+        <f t="shared" si="0"/>
+        <v>-7.0000000000003393E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C20" s="4">
         <v>39.9</v>
@@ -2731,20 +2821,23 @@
       <c r="AG20" s="4">
         <v>0.69399999999999995</v>
       </c>
-      <c r="AH20" s="4">
-        <v>0.695025</v>
-      </c>
-      <c r="AI20" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.0250000000000536E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH20" s="11">
+        <v>0.69479999999999997</v>
+      </c>
+      <c r="AI20">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="AJ20" s="14">
+        <f t="shared" si="0"/>
+        <v>-1.9999999999997797E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C21" s="4">
         <v>49.9</v>
@@ -2781,20 +2874,23 @@
       <c r="AG21" s="4">
         <v>0.68</v>
       </c>
-      <c r="AH21" s="4">
-        <v>0.68067599999999995</v>
-      </c>
-      <c r="AI21" s="14">
-        <f t="shared" si="0"/>
-        <v>-6.759999999998989E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH21" s="11">
+        <v>0.68110000000000004</v>
+      </c>
+      <c r="AI21">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="AJ21" s="14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999988987E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C22" s="4">
         <v>50</v>
@@ -2831,20 +2927,23 @@
       <c r="AG22" s="4">
         <v>0.61799999999999999</v>
       </c>
-      <c r="AH22" s="4">
-        <v>0.61975899999999995</v>
-      </c>
-      <c r="AI22" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.758999999999955E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH22" s="11">
+        <v>0.61970000000000003</v>
+      </c>
+      <c r="AI22">
+        <v>0.62</v>
+      </c>
+      <c r="AJ22" s="14">
+        <f t="shared" si="0"/>
+        <v>-2.9999999999996696E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C23" s="4">
         <v>50</v>
@@ -2881,20 +2980,23 @@
       <c r="AG23" s="4">
         <v>0.627</v>
       </c>
-      <c r="AH23" s="4">
-        <v>0.62831599999999999</v>
-      </c>
-      <c r="AI23" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.3159999999999838E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH23" s="11">
+        <v>0.62870000000000004</v>
+      </c>
+      <c r="AI23">
+        <v>0.628</v>
+      </c>
+      <c r="AJ23" s="14">
+        <f t="shared" si="0"/>
+        <v>7.0000000000003393E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C24" s="4">
         <v>49.9</v>
@@ -2931,20 +3033,23 @@
       <c r="AG24" s="4">
         <v>0.70099999999999996</v>
       </c>
-      <c r="AH24" s="4">
-        <v>0.70088899999999998</v>
-      </c>
-      <c r="AI24" s="14">
-        <f t="shared" si="0"/>
-        <v>1.1099999999997223E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH24" s="11">
+        <v>0.70109999999999995</v>
+      </c>
+      <c r="AI24">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="AJ24" s="14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999988987E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C25" s="4">
         <v>40</v>
@@ -2981,20 +3086,23 @@
       <c r="AG25" s="4">
         <v>0.69099999999999995</v>
       </c>
-      <c r="AH25" s="4">
-        <v>0.69155500000000003</v>
-      </c>
-      <c r="AI25" s="14">
-        <f t="shared" si="0"/>
-        <v>-5.550000000000832E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH25" s="11">
+        <v>0.6915</v>
+      </c>
+      <c r="AI25">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="AJ25" s="14">
+        <f t="shared" si="0"/>
+        <v>-4.9999999999994493E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C26" s="4">
         <v>39.9</v>
@@ -3031,20 +3139,23 @@
       <c r="AG26" s="4">
         <v>0.64</v>
       </c>
-      <c r="AH26" s="4">
-        <v>0.64025399999999999</v>
-      </c>
-      <c r="AI26" s="14">
-        <f t="shared" si="0"/>
-        <v>-2.5399999999997647E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH26" s="11">
+        <v>0.64019999999999999</v>
+      </c>
+      <c r="AI26">
+        <v>0.64</v>
+      </c>
+      <c r="AJ26" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9999999999997797E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C27" s="4">
         <v>39.9</v>
@@ -3081,20 +3192,23 @@
       <c r="AG27" s="4">
         <v>0.64200000000000002</v>
       </c>
-      <c r="AH27" s="4">
-        <v>0.64249400000000001</v>
-      </c>
-      <c r="AI27" s="14">
-        <f t="shared" si="0"/>
-        <v>-4.9399999999999444E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH27" s="11">
+        <v>0.6421</v>
+      </c>
+      <c r="AI27">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="AJ27" s="14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999988987E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C28" s="4">
         <v>39.9</v>
@@ -3131,20 +3245,23 @@
       <c r="AG28" s="4">
         <v>0.625</v>
       </c>
-      <c r="AH28" s="4">
-        <v>0.62518600000000002</v>
-      </c>
-      <c r="AI28" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.8600000000001948E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH28" s="11">
+        <v>0.625</v>
+      </c>
+      <c r="AI28">
+        <v>0.625</v>
+      </c>
+      <c r="AJ28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C29" s="4">
         <v>39.9</v>
@@ -3181,20 +3298,23 @@
       <c r="AG29" s="4">
         <v>0.63400000000000001</v>
       </c>
-      <c r="AH29" s="4">
-        <v>0.68722700000000003</v>
-      </c>
-      <c r="AI29" s="14">
-        <f t="shared" si="0"/>
-        <v>-5.3227000000000024E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH29" s="11">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="AI29">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="AJ29" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C30" s="4">
         <v>39.9</v>
@@ -3231,20 +3351,23 @@
       <c r="AG30" s="4">
         <v>0.63</v>
       </c>
-      <c r="AH30" s="4">
-        <v>0.63024000000000002</v>
-      </c>
-      <c r="AI30" s="14">
-        <f t="shared" si="0"/>
-        <v>-2.4000000000001798E-4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH30" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="AI30">
+        <v>0.63</v>
+      </c>
+      <c r="AJ30" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C31" s="4">
         <v>39.9</v>
@@ -3281,20 +3404,23 @@
       <c r="AG31" s="4">
         <v>0.628</v>
       </c>
-      <c r="AH31" s="4">
-        <v>0.62778400000000001</v>
-      </c>
-      <c r="AI31" s="14">
-        <f t="shared" si="0"/>
-        <v>2.1599999999999397E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH31" s="11">
+        <v>0.62770000000000004</v>
+      </c>
+      <c r="AI31">
+        <v>0.628</v>
+      </c>
+      <c r="AJ31" s="14">
+        <f t="shared" si="0"/>
+        <v>-2.9999999999996696E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C32" s="4">
         <v>49.9</v>
@@ -3331,20 +3457,23 @@
       <c r="AG32" s="4">
         <v>0.625</v>
       </c>
-      <c r="AH32" s="4">
-        <v>0.62478400000000001</v>
-      </c>
-      <c r="AI32" s="14">
-        <f t="shared" si="0"/>
-        <v>2.1599999999999397E-4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH32" s="11">
+        <v>0.62480000000000002</v>
+      </c>
+      <c r="AI32">
+        <v>0.625</v>
+      </c>
+      <c r="AJ32" s="14">
+        <f t="shared" si="0"/>
+        <v>-1.9999999999997797E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C33" s="4">
         <v>49.9</v>
@@ -3381,20 +3510,23 @@
       <c r="AG33" s="4">
         <v>0.65100000000000002</v>
       </c>
-      <c r="AH33" s="4">
-        <v>0.65118699999999996</v>
-      </c>
-      <c r="AI33" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.8699999999993722E-4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH33" s="11">
+        <v>0.65110000000000001</v>
+      </c>
+      <c r="AI33">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AJ33" s="14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999988987E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C34" s="4">
         <v>49.8</v>
@@ -3431,20 +3563,23 @@
       <c r="AG34" s="4">
         <v>0.622</v>
       </c>
-      <c r="AH34" s="4">
-        <v>0.62179700000000004</v>
-      </c>
-      <c r="AI34" s="14">
-        <f t="shared" si="0"/>
-        <v>2.0299999999995322E-4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH34" s="11">
+        <v>0.62180000000000002</v>
+      </c>
+      <c r="AI34">
+        <v>0.622</v>
+      </c>
+      <c r="AJ34" s="14">
+        <f t="shared" si="0"/>
+        <v>-1.9999999999997797E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C35" s="4">
         <v>49.9</v>
@@ -3481,20 +3616,23 @@
       <c r="AG35" s="4">
         <v>0.626</v>
       </c>
-      <c r="AH35" s="4">
-        <v>0.62557700000000005</v>
-      </c>
-      <c r="AI35" s="14">
-        <f t="shared" si="0"/>
-        <v>4.2299999999995119E-4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH35" s="11">
+        <v>0.62580000000000002</v>
+      </c>
+      <c r="AI35">
+        <v>0.626</v>
+      </c>
+      <c r="AJ35" s="14">
+        <f t="shared" si="0"/>
+        <v>-1.9999999999997797E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C36" s="4">
         <v>38.47</v>
@@ -3586,20 +3724,23 @@
       <c r="AG36" s="14">
         <v>0.63692918484900474</v>
       </c>
-      <c r="AH36" s="4">
-        <v>0.64006099999999999</v>
-      </c>
-      <c r="AI36" s="14">
-        <f>AG36-AH36</f>
-        <v>-3.1318151509952541E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH36" s="23">
+        <v>0.63980000000000004</v>
+      </c>
+      <c r="AI36">
+        <v>0.64</v>
+      </c>
+      <c r="AJ36" s="14">
+        <f t="shared" si="0"/>
+        <v>-1.9999999999997797E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C37" s="4">
         <v>38.47</v>
@@ -3691,17 +3832,20 @@
       <c r="AG37" s="14">
         <v>0.64192391753402256</v>
       </c>
-      <c r="AH37" s="4">
-        <v>0.64558000000000004</v>
-      </c>
-      <c r="AI37" s="14">
-        <f t="shared" ref="AI37:AI116" si="10">AG37-AH37</f>
-        <v>-3.6560824659774838E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH37" s="23">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="AI37">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="AJ37" s="14">
+        <f t="shared" si="0"/>
+        <v>-2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>17</v>
@@ -3741,17 +3885,20 @@
       <c r="AG38" s="19">
         <v>0.92300000000000004</v>
       </c>
-      <c r="AH38" s="16">
-        <v>0.92746700000000004</v>
-      </c>
-      <c r="AI38" s="19">
-        <f t="shared" si="10"/>
-        <v>-4.4669999999999987E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH38" s="24">
+        <v>0.92720000000000002</v>
+      </c>
+      <c r="AI38">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="AJ38" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9999999999997797E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>17</v>
@@ -3791,15 +3938,18 @@
       <c r="AG39" s="19">
         <v>0.92600000000000005</v>
       </c>
-      <c r="AH39" s="16">
-        <v>0.92891500000000005</v>
-      </c>
-      <c r="AI39" s="19">
-        <f t="shared" si="10"/>
-        <v>-2.9150000000000009E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH39" s="24">
+        <v>0.92869999999999997</v>
+      </c>
+      <c r="AI39">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="AJ39" s="14">
+        <f t="shared" si="0"/>
+        <v>-3.0000000000007798E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>13</v>
       </c>
@@ -3892,15 +4042,18 @@
       <c r="AG40" s="19">
         <v>0.91486436538534088</v>
       </c>
-      <c r="AH40" s="16">
-        <v>0.91719300000000004</v>
-      </c>
-      <c r="AI40" s="19">
-        <f t="shared" si="10"/>
-        <v>-2.328634614659153E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH40" s="24">
+        <v>0.91710000000000003</v>
+      </c>
+      <c r="AI40">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="AJ40" s="14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999988987E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>14</v>
       </c>
@@ -3993,15 +4146,18 @@
       <c r="AG41" s="19">
         <v>0.9167086694055423</v>
       </c>
-      <c r="AH41" s="16">
-        <v>0.91864100000000004</v>
-      </c>
-      <c r="AI41" s="19">
-        <f t="shared" si="10"/>
-        <v>-1.9323305944577429E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH41" s="24">
+        <v>0.91859999999999997</v>
+      </c>
+      <c r="AI41">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="AJ41" s="14">
+        <f t="shared" si="0"/>
+        <v>-4.0000000000006697E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>15</v>
       </c>
@@ -4094,15 +4250,18 @@
       <c r="AG42" s="19">
         <v>0.92429892689988069</v>
       </c>
-      <c r="AH42" s="16">
-        <v>0.92649000000000004</v>
-      </c>
-      <c r="AI42" s="19">
-        <f t="shared" si="10"/>
-        <v>-2.1910731001193451E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH42" s="24">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="AI42">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="AJ42" s="14">
+        <f t="shared" si="0"/>
+        <v>4.9999999999994493E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>16</v>
       </c>
@@ -4195,15 +4354,18 @@
       <c r="AG43" s="19">
         <v>0.92263872730338636</v>
       </c>
-      <c r="AH43" s="16">
-        <v>0.926454</v>
-      </c>
-      <c r="AI43" s="19">
-        <f t="shared" si="10"/>
-        <v>-3.8152726966136363E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH43" s="24">
+        <v>0.9264</v>
+      </c>
+      <c r="AI43">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="AJ43" s="14">
+        <f t="shared" si="0"/>
+        <v>3.9999999999995595E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>18</v>
       </c>
@@ -4296,15 +4458,18 @@
       <c r="AG44" s="19">
         <v>0.91811639759826613</v>
       </c>
-      <c r="AH44" s="16">
-        <v>0.92491800000000002</v>
-      </c>
-      <c r="AI44" s="19">
-        <f t="shared" si="10"/>
-        <v>-6.8016024017338861E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH44" s="24">
+        <v>0.92490000000000006</v>
+      </c>
+      <c r="AI44">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="AJ44" s="14">
+        <f t="shared" si="0"/>
+        <v>-9.9999999999988987E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
         <v>19</v>
       </c>
@@ -4397,15 +4562,18 @@
       <c r="AG45" s="19">
         <v>0.91780516938713574</v>
       </c>
-      <c r="AH45" s="16">
-        <v>0.92433699999999996</v>
-      </c>
-      <c r="AI45" s="19">
-        <f t="shared" si="10"/>
-        <v>-6.5318306128642201E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH45" s="24">
+        <v>0.92430000000000001</v>
+      </c>
+      <c r="AI45">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="AJ45" s="14">
+        <f t="shared" si="0"/>
+        <v>2.9999999999996696E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>20</v>
       </c>
@@ -4498,15 +4666,18 @@
       <c r="AG46" s="19">
         <v>0.91925132915549479</v>
       </c>
-      <c r="AH46" s="16">
-        <v>0.92342100000000005</v>
-      </c>
-      <c r="AI46" s="19">
-        <f t="shared" si="10"/>
-        <v>-4.1696708445052577E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH46" s="24">
+        <v>0.9234</v>
+      </c>
+      <c r="AI46">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="AJ46" s="14">
+        <f t="shared" si="0"/>
+        <v>3.9999999999995595E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>21</v>
       </c>
@@ -4599,17 +4770,20 @@
       <c r="AG47" s="19">
         <v>0.88967514351634858</v>
       </c>
-      <c r="AH47" s="16">
-        <v>0.890544</v>
-      </c>
-      <c r="AI47" s="19">
-        <f t="shared" si="10"/>
-        <v>-8.6885648365142565E-4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH47" s="24">
+        <v>0.89059999999999995</v>
+      </c>
+      <c r="AI47">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="AJ47" s="14">
+        <f t="shared" si="0"/>
+        <v>-4.0000000000006697E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="B48" s="15" t="s">
         <v>24</v>
@@ -4649,17 +4823,20 @@
       <c r="AG48" s="19">
         <v>0.92</v>
       </c>
-      <c r="AH48" s="16">
-        <v>0</v>
-      </c>
-      <c r="AI48" s="19">
-        <f t="shared" si="10"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH48" s="24">
+        <v>0.92190000000000005</v>
+      </c>
+      <c r="AI48">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="AJ48" s="14">
+        <f t="shared" si="0"/>
+        <v>-9.9999999999988987E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="B49" s="15" t="s">
         <v>24</v>
@@ -4699,15 +4876,18 @@
       <c r="AG49" s="19">
         <v>0.92500000000000004</v>
       </c>
-      <c r="AH49" s="16">
-        <v>0.92713800000000002</v>
-      </c>
-      <c r="AI49" s="19">
-        <f t="shared" si="10"/>
-        <v>-2.1379999999999733E-3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH49" s="24">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="AI49">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="AJ49" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
         <v>23</v>
       </c>
@@ -4800,15 +4980,18 @@
       <c r="AG50" s="19">
         <v>0.92035093322632699</v>
       </c>
-      <c r="AH50" s="16">
-        <v>0.92389600000000005</v>
-      </c>
-      <c r="AI50" s="19">
-        <f t="shared" si="10"/>
-        <v>-3.5450667736730557E-3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH50" s="24">
+        <v>0.92379999999999995</v>
+      </c>
+      <c r="AI50">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="AJ50" s="14">
+        <f t="shared" si="0"/>
+        <v>-2.00000000000089E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
         <v>25</v>
       </c>
@@ -4901,15 +5084,18 @@
       <c r="AG51" s="19">
         <v>0.92279999999999995</v>
       </c>
-      <c r="AH51" s="16">
-        <v>0.927145</v>
-      </c>
-      <c r="AI51" s="19">
-        <f t="shared" si="10"/>
-        <v>-4.3450000000000433E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH51" s="24">
+        <v>0.92710000000000004</v>
+      </c>
+      <c r="AI51">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="AJ51" s="14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999988987E-5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
         <v>26</v>
       </c>
@@ -5002,15 +5188,18 @@
       <c r="AG52" s="19">
         <v>0.91517757628246044</v>
       </c>
-      <c r="AH52" s="16">
-        <v>0.91883599999999999</v>
-      </c>
-      <c r="AI52" s="19">
-        <f t="shared" si="10"/>
-        <v>-3.6584237175395495E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH52" s="24">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="AI52">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="AJ52" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
         <v>27</v>
       </c>
@@ -5103,17 +5292,20 @@
       <c r="AG53" s="19">
         <v>0.91693398324447473</v>
       </c>
-      <c r="AH53" s="16">
-        <v>0.92089799999999999</v>
-      </c>
-      <c r="AI53" s="19">
-        <f t="shared" si="10"/>
-        <v>-3.9640167555252681E-3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH53" s="24">
+        <v>0.92079999999999995</v>
+      </c>
+      <c r="AI53">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="AJ53" s="14">
+        <f t="shared" si="0"/>
+        <v>-2.00000000000089E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="B54" s="15" t="s">
         <v>29</v>
@@ -5153,15 +5345,16 @@
       <c r="AG54" s="19">
         <v>0.92500000000000004</v>
       </c>
-      <c r="AH54" s="16"/>
-      <c r="AI54" s="19">
-        <f t="shared" si="10"/>
-        <v>0.92500000000000004</v>
-      </c>
-    </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH54" s="19"/>
+      <c r="AI54" s="16"/>
+      <c r="AJ54" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="B55" s="15" t="s">
         <v>29</v>
@@ -5201,13 +5394,14 @@
       <c r="AG55" s="19">
         <v>0.93100000000000005</v>
       </c>
-      <c r="AH55" s="16"/>
-      <c r="AI55" s="19">
-        <f t="shared" si="10"/>
-        <v>0.93100000000000005</v>
-      </c>
-    </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH55" s="19"/>
+      <c r="AI55" s="16"/>
+      <c r="AJ55" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>28</v>
       </c>
@@ -5300,13 +5494,14 @@
       <c r="AG56" s="19">
         <v>0.91499736714872371</v>
       </c>
-      <c r="AH56" s="16"/>
-      <c r="AI56" s="19">
-        <f t="shared" si="10"/>
-        <v>0.91499736714872371</v>
-      </c>
-    </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH56" s="19"/>
+      <c r="AI56" s="16"/>
+      <c r="AJ56" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>30</v>
       </c>
@@ -5399,13 +5594,14 @@
       <c r="AG57" s="19">
         <v>0.91584282945008366</v>
       </c>
-      <c r="AH57" s="16"/>
-      <c r="AI57" s="19">
-        <f t="shared" si="10"/>
-        <v>0.91584282945008366</v>
-      </c>
-    </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH57" s="19"/>
+      <c r="AI57" s="16"/>
+      <c r="AJ57" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
         <v>31</v>
       </c>
@@ -5498,13 +5694,14 @@
       <c r="AG58" s="19">
         <v>0.90950537153338806</v>
       </c>
-      <c r="AH58" s="16"/>
-      <c r="AI58" s="19">
-        <f t="shared" si="10"/>
-        <v>0.90950537153338806</v>
-      </c>
-    </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH58" s="19"/>
+      <c r="AI58" s="16"/>
+      <c r="AJ58" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
         <v>32</v>
       </c>
@@ -5597,13 +5794,14 @@
       <c r="AG59" s="19">
         <v>0.9181107354306689</v>
       </c>
-      <c r="AH59" s="16"/>
-      <c r="AI59" s="19">
-        <f t="shared" si="10"/>
-        <v>0.9181107354306689</v>
-      </c>
-    </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH59" s="19"/>
+      <c r="AI59" s="16"/>
+      <c r="AJ59" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
         <v>33</v>
       </c>
@@ -5696,13 +5894,14 @@
       <c r="AG60" s="19">
         <v>0.90923498497209809</v>
       </c>
-      <c r="AH60" s="16"/>
-      <c r="AI60" s="19">
-        <f t="shared" si="10"/>
-        <v>0.90923498497209809</v>
-      </c>
-    </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH60" s="19"/>
+      <c r="AI60" s="16"/>
+      <c r="AJ60" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
         <v>35</v>
       </c>
@@ -5795,13 +5994,14 @@
       <c r="AG61" s="19">
         <v>0.91170649315209085</v>
       </c>
-      <c r="AH61" s="16"/>
-      <c r="AI61" s="19">
-        <f t="shared" si="10"/>
-        <v>0.91170649315209085</v>
-      </c>
-    </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH61" s="19"/>
+      <c r="AI61" s="16"/>
+      <c r="AJ61" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>36</v>
       </c>
@@ -5894,13 +6094,14 @@
       <c r="AG62" s="19">
         <v>0.9235547669353702</v>
       </c>
-      <c r="AH62" s="16"/>
-      <c r="AI62" s="19">
-        <f t="shared" si="10"/>
-        <v>0.9235547669353702</v>
-      </c>
-    </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH62" s="19"/>
+      <c r="AI62" s="16"/>
+      <c r="AJ62" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
         <v>37</v>
       </c>
@@ -5993,15 +6194,16 @@
       <c r="AG63" s="19">
         <v>0.92471339100958849</v>
       </c>
-      <c r="AH63" s="16"/>
-      <c r="AI63" s="19">
-        <f t="shared" si="10"/>
-        <v>0.92471339100958849</v>
-      </c>
-    </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH63" s="19"/>
+      <c r="AI63" s="16"/>
+      <c r="AJ63" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="B64" s="15" t="s">
         <v>39</v>
@@ -6041,15 +6243,16 @@
       <c r="AG64" s="19">
         <v>0.92700000000000005</v>
       </c>
-      <c r="AH64" s="16"/>
-      <c r="AI64" s="19">
-        <f t="shared" si="10"/>
-        <v>0.92700000000000005</v>
-      </c>
-    </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH64" s="19"/>
+      <c r="AI64" s="16"/>
+      <c r="AJ64" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="B65" s="15" t="s">
         <v>39</v>
@@ -6089,13 +6292,14 @@
       <c r="AG65" s="19">
         <v>0.91600000000000004</v>
       </c>
-      <c r="AH65" s="16"/>
-      <c r="AI65" s="19">
-        <f t="shared" si="10"/>
-        <v>0.91600000000000004</v>
-      </c>
-    </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH65" s="19"/>
+      <c r="AI65" s="16"/>
+      <c r="AJ65" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
         <v>38</v>
       </c>
@@ -6188,13 +6392,14 @@
       <c r="AG66" s="19">
         <v>0.91440189369811065</v>
       </c>
-      <c r="AH66" s="16"/>
-      <c r="AI66" s="19">
-        <f t="shared" si="10"/>
-        <v>0.91440189369811065</v>
-      </c>
-    </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH66" s="19"/>
+      <c r="AI66" s="16"/>
+      <c r="AJ66" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
         <v>40</v>
       </c>
@@ -6287,13 +6492,14 @@
       <c r="AG67" s="19">
         <v>0.91119750217455808</v>
       </c>
-      <c r="AH67" s="16"/>
-      <c r="AI67" s="19">
-        <f t="shared" si="10"/>
-        <v>0.91119750217455808</v>
-      </c>
-    </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH67" s="19"/>
+      <c r="AI67" s="16"/>
+      <c r="AJ67" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
         <v>41</v>
       </c>
@@ -6386,13 +6592,14 @@
       <c r="AG68" s="19">
         <v>0.91740136721349375</v>
       </c>
-      <c r="AH68" s="16"/>
-      <c r="AI68" s="19">
-        <f t="shared" si="10"/>
-        <v>0.91740136721349375</v>
-      </c>
-    </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH68" s="19"/>
+      <c r="AI68" s="16"/>
+      <c r="AJ68" s="14">
+        <f t="shared" ref="AJ68:AJ116" si="10">AH68-AI68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
         <v>42</v>
       </c>
@@ -6485,13 +6692,14 @@
       <c r="AG69" s="19">
         <v>0.90184813249726981</v>
       </c>
-      <c r="AH69" s="16"/>
-      <c r="AI69" s="19">
+      <c r="AH69" s="19"/>
+      <c r="AI69" s="16"/>
+      <c r="AJ69" s="14">
         <f t="shared" si="10"/>
-        <v>0.90184813249726981</v>
-      </c>
-    </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
         <v>43</v>
       </c>
@@ -6584,13 +6792,14 @@
       <c r="AG70" s="19">
         <v>0.91584433411827804</v>
       </c>
-      <c r="AH70" s="16"/>
-      <c r="AI70" s="19">
+      <c r="AH70" s="19"/>
+      <c r="AI70" s="16"/>
+      <c r="AJ70" s="14">
         <f t="shared" si="10"/>
-        <v>0.91584433411827804</v>
-      </c>
-    </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
         <v>44</v>
       </c>
@@ -6683,13 +6892,14 @@
       <c r="AG71" s="19">
         <v>0.91582419377934587</v>
       </c>
-      <c r="AH71" s="16"/>
-      <c r="AI71" s="19">
+      <c r="AH71" s="19"/>
+      <c r="AI71" s="16"/>
+      <c r="AJ71" s="14">
         <f t="shared" si="10"/>
-        <v>0.91582419377934587</v>
-      </c>
-    </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
         <v>45</v>
       </c>
@@ -6782,13 +6992,14 @@
       <c r="AG72" s="19">
         <v>0.91000303824766082</v>
       </c>
-      <c r="AH72" s="16"/>
-      <c r="AI72" s="19">
+      <c r="AH72" s="19"/>
+      <c r="AI72" s="16"/>
+      <c r="AJ72" s="14">
         <f t="shared" si="10"/>
-        <v>0.91000303824766082</v>
-      </c>
-    </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
         <v>46</v>
       </c>
@@ -6881,15 +7092,16 @@
       <c r="AG73" s="19">
         <v>0.91609225355188495</v>
       </c>
-      <c r="AH73" s="16"/>
-      <c r="AI73" s="19">
+      <c r="AH73" s="19"/>
+      <c r="AI73" s="16"/>
+      <c r="AJ73" s="14">
         <f t="shared" si="10"/>
-        <v>0.91609225355188495</v>
-      </c>
-    </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="B74" s="15" t="s">
         <v>48</v>
@@ -6929,15 +7141,16 @@
       <c r="AG74" s="19">
         <v>0.93400000000000005</v>
       </c>
-      <c r="AH74" s="16"/>
-      <c r="AI74" s="19">
+      <c r="AH74" s="19"/>
+      <c r="AI74" s="16"/>
+      <c r="AJ74" s="14">
         <f t="shared" si="10"/>
-        <v>0.93400000000000005</v>
-      </c>
-    </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="B75" s="15" t="s">
         <v>48</v>
@@ -6977,13 +7190,14 @@
       <c r="AG75" s="19">
         <v>0.93500000000000005</v>
       </c>
-      <c r="AH75" s="16"/>
-      <c r="AI75" s="19">
+      <c r="AH75" s="19"/>
+      <c r="AI75" s="16"/>
+      <c r="AJ75" s="14">
         <f t="shared" si="10"/>
-        <v>0.93500000000000005</v>
-      </c>
-    </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
         <v>47</v>
       </c>
@@ -7076,13 +7290,14 @@
       <c r="AG76" s="19">
         <v>0.93137405678912</v>
       </c>
-      <c r="AH76" s="16"/>
-      <c r="AI76" s="19">
+      <c r="AH76" s="19"/>
+      <c r="AI76" s="16"/>
+      <c r="AJ76" s="14">
         <f t="shared" si="10"/>
-        <v>0.93137405678912</v>
-      </c>
-    </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
         <v>49</v>
       </c>
@@ -7175,13 +7390,14 @@
       <c r="AG77" s="19">
         <v>0.93408475016627335</v>
       </c>
-      <c r="AH77" s="16"/>
-      <c r="AI77" s="19">
+      <c r="AH77" s="19"/>
+      <c r="AI77" s="16"/>
+      <c r="AJ77" s="14">
         <f t="shared" si="10"/>
-        <v>0.93408475016627335</v>
-      </c>
-    </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
         <v>50</v>
       </c>
@@ -7274,13 +7490,14 @@
       <c r="AG78" s="19">
         <v>0.9313425672130492</v>
       </c>
-      <c r="AH78" s="16"/>
-      <c r="AI78" s="19">
+      <c r="AH78" s="19"/>
+      <c r="AI78" s="16"/>
+      <c r="AJ78" s="14">
         <f t="shared" si="10"/>
-        <v>0.9313425672130492</v>
-      </c>
-    </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
         <v>51</v>
       </c>
@@ -7373,13 +7590,14 @@
       <c r="AG79" s="19">
         <v>0.92871686126712338</v>
       </c>
-      <c r="AH79" s="16"/>
-      <c r="AI79" s="19">
+      <c r="AH79" s="19"/>
+      <c r="AI79" s="16"/>
+      <c r="AJ79" s="14">
         <f t="shared" si="10"/>
-        <v>0.92871686126712338</v>
-      </c>
-    </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
         <v>52</v>
       </c>
@@ -7421,13 +7639,14 @@
       <c r="AG80" s="19">
         <v>0.92700000000000005</v>
       </c>
-      <c r="AH80" s="16"/>
-      <c r="AI80" s="19">
+      <c r="AH80" s="19"/>
+      <c r="AI80" s="16"/>
+      <c r="AJ80" s="14">
         <f t="shared" si="10"/>
-        <v>0.92700000000000005</v>
-      </c>
-    </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
         <v>54</v>
       </c>
@@ -7520,13 +7739,14 @@
       <c r="AG81" s="19">
         <v>0.93102933417843436</v>
       </c>
-      <c r="AH81" s="16"/>
-      <c r="AI81" s="19">
+      <c r="AH81" s="19"/>
+      <c r="AI81" s="16"/>
+      <c r="AJ81" s="14">
         <f t="shared" si="10"/>
-        <v>0.93102933417843436</v>
-      </c>
-    </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
         <v>55</v>
       </c>
@@ -7619,13 +7839,14 @@
       <c r="AG82" s="19">
         <v>0.92971749366237477</v>
       </c>
-      <c r="AH82" s="16"/>
-      <c r="AI82" s="19">
+      <c r="AH82" s="19"/>
+      <c r="AI82" s="16"/>
+      <c r="AJ82" s="14">
         <f t="shared" si="10"/>
-        <v>0.92971749366237477</v>
-      </c>
-    </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
         <v>56</v>
       </c>
@@ -7718,15 +7939,16 @@
       <c r="AG83" s="19">
         <v>0.88089077504082924</v>
       </c>
-      <c r="AH83" s="16"/>
-      <c r="AI83" s="19">
+      <c r="AH83" s="19"/>
+      <c r="AI83" s="16"/>
+      <c r="AJ83" s="14">
         <f t="shared" si="10"/>
-        <v>0.88089077504082924</v>
-      </c>
-    </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="B84" s="15" t="s">
         <v>58</v>
@@ -7766,15 +7988,16 @@
       <c r="AG84" s="19">
         <v>0.92500000000000004</v>
       </c>
-      <c r="AH84" s="16"/>
-      <c r="AI84" s="19">
+      <c r="AH84" s="19"/>
+      <c r="AI84" s="16"/>
+      <c r="AJ84" s="14">
         <f t="shared" si="10"/>
-        <v>0.92500000000000004</v>
-      </c>
-    </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="B85" s="15" t="s">
         <v>58</v>
@@ -7814,13 +8037,14 @@
       <c r="AG85" s="19">
         <v>0.93899999999999995</v>
       </c>
-      <c r="AH85" s="16"/>
-      <c r="AI85" s="19">
+      <c r="AH85" s="19"/>
+      <c r="AI85" s="16"/>
+      <c r="AJ85" s="14">
         <f t="shared" si="10"/>
-        <v>0.93899999999999995</v>
-      </c>
-    </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
         <v>57</v>
       </c>
@@ -7913,13 +8137,14 @@
       <c r="AG86" s="19">
         <v>0.9331024980123428</v>
       </c>
-      <c r="AH86" s="16"/>
-      <c r="AI86" s="19">
+      <c r="AH86" s="19"/>
+      <c r="AI86" s="16"/>
+      <c r="AJ86" s="14">
         <f t="shared" si="10"/>
-        <v>0.9331024980123428</v>
-      </c>
-    </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
         <v>59</v>
       </c>
@@ -8012,13 +8237,14 @@
       <c r="AG87" s="19">
         <v>0.92968255944153733</v>
       </c>
-      <c r="AH87" s="16"/>
-      <c r="AI87" s="19">
+      <c r="AH87" s="19"/>
+      <c r="AI87" s="16"/>
+      <c r="AJ87" s="14">
         <f t="shared" si="10"/>
-        <v>0.92968255944153733</v>
-      </c>
-    </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
         <v>60</v>
       </c>
@@ -8111,13 +8337,14 @@
       <c r="AG88" s="19">
         <v>0.92867786805463182</v>
       </c>
-      <c r="AH88" s="16"/>
-      <c r="AI88" s="19">
+      <c r="AH88" s="19"/>
+      <c r="AI88" s="16"/>
+      <c r="AJ88" s="14">
         <f t="shared" si="10"/>
-        <v>0.92867786805463182</v>
-      </c>
-    </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
         <v>61</v>
       </c>
@@ -8210,18 +8437,19 @@
       <c r="AG89" s="19">
         <v>0.92883400573334829</v>
       </c>
-      <c r="AH89" s="16"/>
-      <c r="AI89" s="19">
+      <c r="AH89" s="19"/>
+      <c r="AI89" s="16"/>
+      <c r="AJ89" s="14">
         <f t="shared" si="10"/>
-        <v>0.92883400573334829</v>
-      </c>
-    </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="C90" s="4">
         <v>0</v>
@@ -8258,18 +8486,19 @@
       <c r="AG90" s="14">
         <v>0.82101800000000003</v>
       </c>
-      <c r="AH90" s="4"/>
-      <c r="AI90" s="14">
+      <c r="AH90" s="14"/>
+      <c r="AI90" s="4"/>
+      <c r="AJ90" s="14">
         <f t="shared" si="10"/>
-        <v>0.82101800000000003</v>
-      </c>
-    </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="C91" s="4">
         <v>0</v>
@@ -8306,13 +8535,14 @@
       <c r="AG91" s="14">
         <v>0.81592699999999996</v>
       </c>
-      <c r="AH91" s="4"/>
-      <c r="AI91" s="14">
+      <c r="AH91" s="14"/>
+      <c r="AI91" s="4"/>
+      <c r="AJ91" s="14">
         <f t="shared" si="10"/>
-        <v>0.81592699999999996</v>
-      </c>
-    </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
         <v>88</v>
       </c>
@@ -8355,12 +8585,13 @@
         <v>3.2120000000000002</v>
       </c>
       <c r="AH92" s="16"/>
-      <c r="AI92" s="16">
+      <c r="AI92" s="16"/>
+      <c r="AJ92" s="14">
         <f t="shared" si="10"/>
-        <v>3.2120000000000002</v>
-      </c>
-    </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
         <v>89</v>
       </c>
@@ -8403,12 +8634,13 @@
         <v>3.27</v>
       </c>
       <c r="AH93" s="16"/>
-      <c r="AI93" s="16">
+      <c r="AI93" s="16"/>
+      <c r="AJ93" s="14">
         <f t="shared" si="10"/>
-        <v>3.27</v>
-      </c>
-    </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
         <v>90</v>
       </c>
@@ -8451,12 +8683,13 @@
         <v>3.2050000000000001</v>
       </c>
       <c r="AH94" s="16"/>
-      <c r="AI94" s="16">
+      <c r="AI94" s="16"/>
+      <c r="AJ94" s="14">
         <f t="shared" si="10"/>
-        <v>3.2050000000000001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
         <v>91</v>
       </c>
@@ -8499,12 +8732,13 @@
         <v>3.2250000000000001</v>
       </c>
       <c r="AH95" s="16"/>
-      <c r="AI95" s="16">
+      <c r="AI95" s="16"/>
+      <c r="AJ95" s="14">
         <f t="shared" si="10"/>
-        <v>3.2250000000000001</v>
-      </c>
-    </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
         <v>92</v>
       </c>
@@ -8547,12 +8781,13 @@
         <v>4.2759999999999998</v>
       </c>
       <c r="AH96" s="16"/>
-      <c r="AI96" s="16">
+      <c r="AI96" s="16"/>
+      <c r="AJ96" s="14">
         <f t="shared" si="10"/>
-        <v>4.2759999999999998</v>
-      </c>
-    </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
         <v>93</v>
       </c>
@@ -8595,12 +8830,13 @@
         <v>4.4980000000000002</v>
       </c>
       <c r="AH97" s="16"/>
-      <c r="AI97" s="16">
+      <c r="AI97" s="16"/>
+      <c r="AJ97" s="14">
         <f t="shared" si="10"/>
-        <v>4.4980000000000002</v>
-      </c>
-    </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
         <v>94</v>
       </c>
@@ -8643,12 +8879,13 @@
         <v>4.3769999999999998</v>
       </c>
       <c r="AH98" s="16"/>
-      <c r="AI98" s="16">
+      <c r="AI98" s="16"/>
+      <c r="AJ98" s="14">
         <f t="shared" si="10"/>
-        <v>4.3769999999999998</v>
-      </c>
-    </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
         <v>95</v>
       </c>
@@ -8691,12 +8928,13 @@
         <v>4.4580000000000002</v>
       </c>
       <c r="AH99" s="16"/>
-      <c r="AI99" s="16">
+      <c r="AI99" s="16"/>
+      <c r="AJ99" s="14">
         <f t="shared" si="10"/>
-        <v>4.4580000000000002</v>
-      </c>
-    </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
         <v>96</v>
       </c>
@@ -8739,12 +8977,13 @@
         <v>3.3519999999999999</v>
       </c>
       <c r="AH100" s="16"/>
-      <c r="AI100" s="16">
+      <c r="AI100" s="16"/>
+      <c r="AJ100" s="14">
         <f t="shared" si="10"/>
-        <v>3.3519999999999999</v>
-      </c>
-    </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
         <v>97</v>
       </c>
@@ -8787,12 +9026,13 @@
         <v>3.383</v>
       </c>
       <c r="AH101" s="16"/>
-      <c r="AI101" s="16">
+      <c r="AI101" s="16"/>
+      <c r="AJ101" s="14">
         <f t="shared" si="10"/>
-        <v>3.383</v>
-      </c>
-    </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
         <v>98</v>
       </c>
@@ -8835,12 +9075,13 @@
         <v>3.274</v>
       </c>
       <c r="AH102" s="16"/>
-      <c r="AI102" s="16">
+      <c r="AI102" s="16"/>
+      <c r="AJ102" s="14">
         <f t="shared" si="10"/>
-        <v>3.274</v>
-      </c>
-    </row>
-    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
         <v>99</v>
       </c>
@@ -8883,12 +9124,13 @@
         <v>3.278</v>
       </c>
       <c r="AH103" s="16"/>
-      <c r="AI103" s="16">
+      <c r="AI103" s="16"/>
+      <c r="AJ103" s="14">
         <f t="shared" si="10"/>
-        <v>3.278</v>
-      </c>
-    </row>
-    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
         <v>100</v>
       </c>
@@ -8931,12 +9173,13 @@
         <v>3.2490000000000001</v>
       </c>
       <c r="AH104" s="16"/>
-      <c r="AI104" s="16">
+      <c r="AI104" s="16"/>
+      <c r="AJ104" s="14">
         <f t="shared" si="10"/>
-        <v>3.2490000000000001</v>
-      </c>
-    </row>
-    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
         <v>101</v>
       </c>
@@ -8979,12 +9222,13 @@
         <v>4.4269999999999996</v>
       </c>
       <c r="AH105" s="16"/>
-      <c r="AI105" s="16">
+      <c r="AI105" s="16"/>
+      <c r="AJ105" s="14">
         <f t="shared" si="10"/>
-        <v>4.4269999999999996</v>
-      </c>
-    </row>
-    <row r="106" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
         <v>102</v>
       </c>
@@ -9027,12 +9271,13 @@
         <v>4.5419999999999998</v>
       </c>
       <c r="AH106" s="16"/>
-      <c r="AI106" s="16">
+      <c r="AI106" s="16"/>
+      <c r="AJ106" s="14">
         <f t="shared" si="10"/>
-        <v>4.5419999999999998</v>
-      </c>
-    </row>
-    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
         <v>103</v>
       </c>
@@ -9075,12 +9320,13 @@
         <v>4.4059999999999997</v>
       </c>
       <c r="AH107" s="16"/>
-      <c r="AI107" s="16">
+      <c r="AI107" s="16"/>
+      <c r="AJ107" s="14">
         <f t="shared" si="10"/>
-        <v>4.4059999999999997</v>
-      </c>
-    </row>
-    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
         <v>104</v>
       </c>
@@ -9123,12 +9369,13 @@
         <v>4.4729999999999999</v>
       </c>
       <c r="AH108" s="16"/>
-      <c r="AI108" s="16">
+      <c r="AI108" s="16"/>
+      <c r="AJ108" s="14">
         <f t="shared" si="10"/>
-        <v>4.4729999999999999</v>
-      </c>
-    </row>
-    <row r="109" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
         <v>87</v>
       </c>
@@ -9171,12 +9418,13 @@
         <v>4.7240000000000002</v>
       </c>
       <c r="AH109" s="16"/>
-      <c r="AI109" s="16">
+      <c r="AI109" s="16"/>
+      <c r="AJ109" s="14">
         <f t="shared" si="10"/>
-        <v>4.7240000000000002</v>
-      </c>
-    </row>
-    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
         <v>105</v>
       </c>
@@ -9219,12 +9467,13 @@
         <v>4.5880000000000001</v>
       </c>
       <c r="AH110" s="16"/>
-      <c r="AI110" s="16">
+      <c r="AI110" s="16"/>
+      <c r="AJ110" s="14">
         <f t="shared" si="10"/>
-        <v>4.5880000000000001</v>
-      </c>
-    </row>
-    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A111" s="15" t="s">
         <v>86</v>
       </c>
@@ -9267,12 +9516,13 @@
         <v>4.6989999999999998</v>
       </c>
       <c r="AH111" s="16"/>
-      <c r="AI111" s="16">
+      <c r="AI111" s="16"/>
+      <c r="AJ111" s="14">
         <f t="shared" si="10"/>
-        <v>4.6989999999999998</v>
-      </c>
-    </row>
-    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
         <v>106</v>
       </c>
@@ -9315,12 +9565,13 @@
         <v>4.673</v>
       </c>
       <c r="AH112" s="16"/>
-      <c r="AI112" s="16">
+      <c r="AI112" s="16"/>
+      <c r="AJ112" s="14">
         <f t="shared" si="10"/>
-        <v>4.673</v>
-      </c>
-    </row>
-    <row r="113" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
         <v>87</v>
       </c>
@@ -9363,12 +9614,13 @@
         <v>4.431</v>
       </c>
       <c r="AH113" s="16"/>
-      <c r="AI113" s="16">
+      <c r="AI113" s="16"/>
+      <c r="AJ113" s="14">
         <f t="shared" si="10"/>
-        <v>4.431</v>
-      </c>
-    </row>
-    <row r="114" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
         <v>86</v>
       </c>
@@ -9411,12 +9663,13 @@
         <v>4.3029999999999999</v>
       </c>
       <c r="AH114" s="16"/>
-      <c r="AI114" s="16">
+      <c r="AI114" s="16"/>
+      <c r="AJ114" s="14">
         <f t="shared" si="10"/>
-        <v>4.3029999999999999</v>
-      </c>
-    </row>
-    <row r="115" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
         <v>106</v>
       </c>
@@ -9459,17 +9712,18 @@
         <v>4.4050000000000002</v>
       </c>
       <c r="AH115" s="16"/>
-      <c r="AI115" s="16">
+      <c r="AI115" s="16"/>
+      <c r="AJ115" s="14">
         <f t="shared" si="10"/>
-        <v>4.4050000000000002</v>
-      </c>
-    </row>
-    <row r="116" spans="1:35" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="C116" s="16">
         <v>65</v>
@@ -9507,9 +9761,10 @@
         <v>3.04</v>
       </c>
       <c r="AH116" s="16"/>
-      <c r="AI116" s="16">
+      <c r="AI116" s="16"/>
+      <c r="AJ116" s="14">
         <f t="shared" si="10"/>
-        <v>3.04</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9522,10 +9777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49E1281-A08B-45E5-9207-66F51863EDCD}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9534,11 +9789,13 @@
     <col min="2" max="2" width="109.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>115</v>
       </c>
@@ -9552,407 +9809,474 @@
         <v>118</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="26" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="B2" s="3" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="C2" s="8">
         <v>85.646000000000001</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E2" s="9">
         <v>85.646000000000001</v>
       </c>
-      <c r="F2" s="3">
-        <f>E2-C2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="9">
+        <v>85.257000000000005</v>
+      </c>
+      <c r="G2" s="3">
+        <f>E2-F2</f>
+        <v>0.38899999999999579</v>
+      </c>
+      <c r="H2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>125</v>
+        <v>197</v>
       </c>
       <c r="C3" s="8">
         <v>86.947500000000005</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E3" s="9">
         <v>86.947500000000005</v>
       </c>
-      <c r="F3" s="3">
-        <f t="shared" ref="F3:F20" si="0">E3-C3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="9">
+        <v>86.850999999999999</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G20" si="0">E3-F3</f>
+        <v>9.6500000000006025E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>127</v>
+        <v>198</v>
       </c>
       <c r="C4" s="8">
         <v>81.051599999999993</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E4" s="9">
         <v>81.078400000000002</v>
       </c>
-      <c r="F4" s="3">
-        <f t="shared" si="0"/>
-        <v>2.6800000000008595E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="9">
+        <v>81.069000000000003</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>9.3999999999994088E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>129</v>
+        <v>199</v>
       </c>
       <c r="C5" s="8">
         <v>74.319999999999993</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E5" s="9">
         <v>74.319999999999993</v>
       </c>
-      <c r="F5" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="9">
+        <v>74.319999999999993</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>130</v>
+        <v>205</v>
       </c>
       <c r="C6" s="8">
         <v>75.23</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E6" s="9">
         <v>75.227000000000004</v>
       </c>
-      <c r="F6" s="3">
-        <f t="shared" si="0"/>
-        <v>-3.0000000000001137E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="9">
+        <v>75.227000000000004</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>132</v>
+        <v>204</v>
       </c>
       <c r="C7" s="8">
         <v>72.918000000000006</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E7" s="9">
         <v>72.918000000000006</v>
       </c>
-      <c r="F7" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="9">
+        <v>72.918000000000006</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>134</v>
+        <v>203</v>
       </c>
       <c r="C8" s="8">
         <v>75.293999999999997</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E8" s="9">
         <v>75.293999999999997</v>
       </c>
-      <c r="F8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="9">
+        <v>75.293999999999997</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>136</v>
+        <v>202</v>
       </c>
       <c r="C9" s="8">
         <v>59.203000000000003</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E9" s="9">
         <v>59.203000000000003</v>
       </c>
-      <c r="F9" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="9">
+        <v>59.203000000000003</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>138</v>
+        <v>201</v>
       </c>
       <c r="C10" s="8">
         <v>74.22</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E10" s="3">
         <v>74.215000000000003</v>
       </c>
-      <c r="F10" s="8">
-        <f>E10-C10</f>
-        <v>-4.9999999999954525E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="3">
+        <v>74.069000000000003</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1460000000000008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C11" s="8">
         <v>85.36</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E11" s="3">
         <v>85.355000000000004</v>
       </c>
-      <c r="F11" s="3">
-        <f t="shared" si="0"/>
-        <v>-4.9999999999954525E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
+        <v>85.355000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>142</v>
+        <v>200</v>
       </c>
       <c r="C12" s="8">
         <v>67.576999999999998</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E12" s="3">
         <v>67.577299999999994</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="0"/>
-        <v>2.9999999999574811E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67.578999999999994</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="0"/>
+        <v>-1.6999999999995907E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>144</v>
+        <v>206</v>
       </c>
       <c r="C13" s="8">
         <v>77.831000000000003</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E13" s="3">
         <v>77.831000000000003</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>77.831000000000003</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>146</v>
+        <v>207</v>
       </c>
       <c r="C14" s="8">
         <v>77.823999999999998</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E14" s="3">
         <v>77.823999999999998</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>77.7</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.12399999999999523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>148</v>
+        <v>208</v>
       </c>
       <c r="C15" s="8">
         <v>87.028000000000006</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E15" s="3">
         <v>87.028000000000006</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>87.028000000000006</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>150</v>
+        <v>209</v>
       </c>
       <c r="C16" s="8">
         <v>64.852999999999994</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E16" s="3">
         <v>64.852900000000005</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="0"/>
-        <v>-9.9999999989108801E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64.853999999999999</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="0"/>
+        <v>-1.0999999999938836E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>152</v>
+        <v>210</v>
       </c>
       <c r="C17" s="8">
         <v>94.200999999999993</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E17" s="3">
         <v>94.200999999999993</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>93.664000000000001</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.53699999999999193</v>
+      </c>
+      <c r="H17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="C18" s="8">
         <v>101.06</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E18" s="3">
         <v>101.06</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>101.06</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>156</v>
+        <v>212</v>
       </c>
       <c r="C19" s="8">
         <v>77.057000000000002</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E19" s="3">
         <v>77.057000000000002</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>77.057000000000002</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>158</v>
+        <v>213</v>
       </c>
       <c r="C20" s="8">
         <v>100.973</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E20" s="3">
         <v>100.973</v>
       </c>
       <c r="F20" s="3">
+        <v>100.973</v>
+      </c>
+      <c r="G20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -9960,4 +10284,643 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DEECCF-E929-4319-8A51-3BB9D0CDC2B3}">
+  <dimension ref="A1:C52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="25">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="B2" s="25">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="C2" s="25">
+        <f>A2-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="B3" s="25">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="C3" s="25">
+        <f t="shared" ref="C3:C52" si="0">A3-B3</f>
+        <v>-1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="25">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="B4" s="25">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="C4" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="B5" s="25">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="C5" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="25">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="B6" s="25">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="C6" s="25">
+        <f t="shared" si="0"/>
+        <v>-3.0000000000000027E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="25">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="B7" s="25">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="C7" s="25">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="B8" s="25">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="C8" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="B9" s="25">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="C9" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="25">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="B10" s="25">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="C10" s="25">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="B11" s="25">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="C11" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="25">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="B12" s="25">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="C12" s="25">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="25">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="B13" s="25">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="C13" s="25">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="B14" s="25">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="C14" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="B15" s="25">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="C15" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="25">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="B16" s="25">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="C16" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="25">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="B17" s="25">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="C17" s="25">
+        <f t="shared" si="0"/>
+        <v>-2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="25">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="B18" s="25">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="C18" s="25">
+        <f t="shared" si="0"/>
+        <v>-2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="B19" s="25">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="C19" s="25">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="25">
+        <v>0.68</v>
+      </c>
+      <c r="B20" s="25">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="C20" s="25">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="25">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="B21" s="25">
+        <v>0.62</v>
+      </c>
+      <c r="C21" s="25">
+        <f t="shared" si="0"/>
+        <v>-2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
+        <v>0.627</v>
+      </c>
+      <c r="B22" s="25">
+        <v>0.628</v>
+      </c>
+      <c r="C22" s="25">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="25">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="B23" s="25">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="C23" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="25">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="B24" s="25">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="C24" s="25">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="25">
+        <v>0.64</v>
+      </c>
+      <c r="B25" s="25">
+        <v>0.64</v>
+      </c>
+      <c r="C25" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="25">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="B26" s="25">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="C26" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="25">
+        <v>0.625</v>
+      </c>
+      <c r="B27" s="25">
+        <v>0.625</v>
+      </c>
+      <c r="C27" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="B28" s="25">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="C28" s="25">
+        <f t="shared" si="0"/>
+        <v>-5.3000000000000047E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="25">
+        <v>0.63</v>
+      </c>
+      <c r="B29" s="25">
+        <v>0.63</v>
+      </c>
+      <c r="C29" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="25">
+        <v>0.628</v>
+      </c>
+      <c r="B30" s="25">
+        <v>0.628</v>
+      </c>
+      <c r="C30" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="25">
+        <v>0.625</v>
+      </c>
+      <c r="B31" s="25">
+        <v>0.625</v>
+      </c>
+      <c r="C31" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="25">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="B32" s="25">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="C32" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="25">
+        <v>0.622</v>
+      </c>
+      <c r="B33" s="25">
+        <v>0.622</v>
+      </c>
+      <c r="C33" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="25">
+        <v>0.626</v>
+      </c>
+      <c r="B34" s="25">
+        <v>0.626</v>
+      </c>
+      <c r="C34" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="25">
+        <v>0.63692918484900474</v>
+      </c>
+      <c r="B35" s="25">
+        <v>0.64</v>
+      </c>
+      <c r="C35" s="25">
+        <f t="shared" si="0"/>
+        <v>-3.0708151509952764E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="25">
+        <v>0.64192391753402256</v>
+      </c>
+      <c r="B36" s="25">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="C36" s="25">
+        <f t="shared" si="0"/>
+        <v>-4.0760824659774597E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="25">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="B37" s="25">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="C37" s="25">
+        <f t="shared" si="0"/>
+        <v>-4.0000000000000036E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="25">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="B38" s="25">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="C38" s="25">
+        <f t="shared" si="0"/>
+        <v>-3.0000000000000027E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="25">
+        <v>0.91486436538534088</v>
+      </c>
+      <c r="B39" s="25">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="C39" s="25">
+        <f t="shared" si="0"/>
+        <v>-2.1356346146591543E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="25">
+        <v>0.9167086694055423</v>
+      </c>
+      <c r="B40" s="25">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="C40" s="25">
+        <f t="shared" si="0"/>
+        <v>-2.2913305944577411E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="25">
+        <v>0.92429892689988069</v>
+      </c>
+      <c r="B41" s="25">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="C41" s="25">
+        <f t="shared" si="0"/>
+        <v>-1.7010731001193546E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="25">
+        <v>0.92263872730338636</v>
+      </c>
+      <c r="B42" s="25">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="C42" s="25">
+        <f t="shared" si="0"/>
+        <v>-3.3612726966136819E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="25">
+        <v>0.91811639759826613</v>
+      </c>
+      <c r="B43" s="25">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="C43" s="25">
+        <f t="shared" si="0"/>
+        <v>-6.8836024017339126E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="25">
+        <v>0.91780516938713574</v>
+      </c>
+      <c r="B44" s="25">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="C44" s="25">
+        <f t="shared" si="0"/>
+        <v>-6.1948306128642994E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="25">
+        <v>0.91925132915549479</v>
+      </c>
+      <c r="B45" s="25">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="C45" s="25">
+        <f t="shared" si="0"/>
+        <v>-3.748670844505253E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="25">
+        <v>0.88967514351634858</v>
+      </c>
+      <c r="B46" s="25">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="C46" s="25">
+        <f t="shared" si="0"/>
+        <v>-1.3248564836514376E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="25">
+        <v>0.92</v>
+      </c>
+      <c r="B47" s="25">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="C47" s="25">
+        <f t="shared" si="0"/>
+        <v>-2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="25">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="B48" s="25">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="C48" s="25">
+        <f t="shared" si="0"/>
+        <v>-2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="25">
+        <v>0.92035093322632699</v>
+      </c>
+      <c r="B49" s="25">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="C49" s="25">
+        <f t="shared" si="0"/>
+        <v>-3.6490667736730487E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="25">
+        <v>0.92279999999999995</v>
+      </c>
+      <c r="B50" s="25">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="C50" s="25">
+        <f t="shared" si="0"/>
+        <v>-4.2000000000000925E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="25">
+        <v>0.91517757628246044</v>
+      </c>
+      <c r="B51" s="25">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="C51" s="25">
+        <f t="shared" si="0"/>
+        <v>-3.8224237175396025E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="25">
+        <v>0.91693398324447473</v>
+      </c>
+      <c r="B52" s="25">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="C52" s="25">
+        <f t="shared" si="0"/>
+        <v>-4.0660167555253146E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>